<commit_message>
Get daily reddit data: Tue Jan 14 08:10:43 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_01_19.xlsx
+++ b/data/collected_data/2025_01_19.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C301"/>
+  <dimension ref="A1:C485"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5551,6 +5551,3134 @@
         </is>
       </c>
     </row>
+    <row r="302">
+      <c r="A302" t="inlineStr">
+        <is>
+          <t>1i10z09</t>
+        </is>
+      </c>
+      <c r="B302" t="inlineStr">
+        <is>
+          <t>I'm slowly but surely getting funky with my nails</t>
+        </is>
+      </c>
+      <c r="C302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i10z09</t>
+        </is>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" t="inlineStr">
+        <is>
+          <t>1i10zhc</t>
+        </is>
+      </c>
+      <c r="B303" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Advice </t>
+        </is>
+      </c>
+      <c r="C303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1lyh2koxywce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" t="inlineStr">
+        <is>
+          <t>1i10vx3</t>
+        </is>
+      </c>
+      <c r="B304" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail lifting, not even two weeks yet. </t>
+        </is>
+      </c>
+      <c r="C304" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i10vx3/nail_lifting_not_even_two_weeks_yet/</t>
+        </is>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" t="inlineStr">
+        <is>
+          <t>1i10p64</t>
+        </is>
+      </c>
+      <c r="B305" t="inlineStr">
+        <is>
+          <t>Concert nails ready</t>
+        </is>
+      </c>
+      <c r="C305" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o9fnd986vwce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="306">
+      <c r="A306" t="inlineStr">
+        <is>
+          <t>1i10hzl</t>
+        </is>
+      </c>
+      <c r="B306" t="inlineStr">
+        <is>
+          <t>I find it hard to go out of the natural 🥹</t>
+        </is>
+      </c>
+      <c r="C306" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7daenpsiswce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" t="inlineStr">
+        <is>
+          <t>1i10dze</t>
+        </is>
+      </c>
+      <c r="B307" t="inlineStr">
+        <is>
+          <t>Nail Shape?</t>
+        </is>
+      </c>
+      <c r="C307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i10dze</t>
+        </is>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" t="inlineStr">
+        <is>
+          <t>1i0z0e0</t>
+        </is>
+      </c>
+      <c r="B308" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Are my nails terrible? </t>
+        </is>
+      </c>
+      <c r="C308" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rmj7yz4iawce1</t>
+        </is>
+      </c>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>1i0yzcr</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>So glossy, so clean 🫧</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c064n437awce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>1i0ynrj</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Does anyone know how to get these off the rest of the way</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3pt82oik6wce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>1i0yp5v</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Early Valentines Day set</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wvntkclz6wce1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>1i0yp3r</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>matching nails with bestie</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cgyfa3xy6wce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>1i0yoai</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t>bumblebees &amp; flowers🐝🌷</t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/wkplt3aq6wce1</t>
+        </is>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>1i0ymeu</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>My second set of gel x!</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zviv6lg66wce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>1i0ycu5</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Press Ons I made for lil sis</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4j8bkaqg3wce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>1i0y75x</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Tried press-on nails for the first time but they look so fake😭</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/drrnh92t1wce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>1i0xzs0</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time wearing color, I always wear black and white and I wanted to encourage myself to wear red, do you think it goes with my skin tone? </t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rdx4em9qzvce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>1i0xerl</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>In love, there’s a tiny bear on the middle finger nails!</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0xerl</t>
+        </is>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>1i0x8et</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Are acrylics supposed to have this glue underneath? </t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0x8et</t>
+        </is>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>1i0x764</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Pinknails!</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vk3wdjx1svce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>1i0wj6p</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>How do you remove nail glue from the back of press on nails?</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i0wj6p/how_do_you_remove_nail_glue_from_the_back_of/</t>
+        </is>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>1i0wwgd</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Doing gel x and I need help</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i0wwgd/doing_gel_x_and_i_need_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>1i0wvf9</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>One of my go to colours for winter</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0wvf9</t>
+        </is>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>1i0whu6</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Shiny chonky nails!</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/uhoo7nrilvce1</t>
+        </is>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>1i0vb6n</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t xml:space="preserve">gel polish help </t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cjg4al2tavce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" t="inlineStr">
+        <is>
+          <t>1i0vk0b</t>
+        </is>
+      </c>
+      <c r="B326" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel allergy: will a regular polish base coat protect from an existing gel allergy </t>
+        </is>
+      </c>
+      <c r="C326" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i0vk0b/gel_allergy_will_a_regular_polish_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="327">
+      <c r="A327" t="inlineStr">
+        <is>
+          <t>1i0vpq4</t>
+        </is>
+      </c>
+      <c r="B327" t="inlineStr">
+        <is>
+          <t>Why are the tips of my nails so brittle/flakey?</t>
+        </is>
+      </c>
+      <c r="C327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i0vpq4/why_are_the_tips_of_my_nails_so_brittleflakey/</t>
+        </is>
+      </c>
+    </row>
+    <row r="328">
+      <c r="A328" t="inlineStr">
+        <is>
+          <t>1i0vs6g</t>
+        </is>
+      </c>
+      <c r="B328" t="inlineStr">
+        <is>
+          <t xml:space="preserve">You like? </t>
+        </is>
+      </c>
+      <c r="C328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0vs6g</t>
+        </is>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" t="inlineStr">
+        <is>
+          <t>1i0vnp8</t>
+        </is>
+      </c>
+      <c r="B329" t="inlineStr">
+        <is>
+          <t>Considering trying to paint my own press-ons</t>
+        </is>
+      </c>
+      <c r="C329" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i0vnp8/considering_trying_to_paint_my_own_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" t="inlineStr">
+        <is>
+          <t>1i0vfmn</t>
+        </is>
+      </c>
+      <c r="B330" t="inlineStr">
+        <is>
+          <t>advice on fixing bitten nails</t>
+        </is>
+      </c>
+      <c r="C330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/g7xv8xnxbvce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" t="inlineStr">
+        <is>
+          <t>1i0vf8r</t>
+        </is>
+      </c>
+      <c r="B331" t="inlineStr">
+        <is>
+          <t>Pink and purple theme</t>
+        </is>
+      </c>
+      <c r="C331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0vf8r</t>
+        </is>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" t="inlineStr">
+        <is>
+          <t>1i0vbsy</t>
+        </is>
+      </c>
+      <c r="B332" t="inlineStr">
+        <is>
+          <t>Birthday nailssss🥰🥳✨</t>
+        </is>
+      </c>
+      <c r="C332" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/p3r3tkiyavce1</t>
+        </is>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" t="inlineStr">
+        <is>
+          <t>1i0v50u</t>
+        </is>
+      </c>
+      <c r="B333" t="inlineStr">
+        <is>
+          <t>Evacuated because of the fires, been extremely depressed and traumatized so thought I’d treat myself to a nice manicure…. 🥲😡</t>
+        </is>
+      </c>
+      <c r="C333" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0v50u</t>
+        </is>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" t="inlineStr">
+        <is>
+          <t>1i0uvqc</t>
+        </is>
+      </c>
+      <c r="B334" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do I do this? </t>
+        </is>
+      </c>
+      <c r="C334" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i0uvqc/how_do_i_do_this/</t>
+        </is>
+      </c>
+    </row>
+    <row r="335">
+      <c r="A335" t="inlineStr">
+        <is>
+          <t>1i0us6m</t>
+        </is>
+      </c>
+      <c r="B335" t="inlineStr">
+        <is>
+          <t>Tech poured monomer back in bottle</t>
+        </is>
+      </c>
+      <c r="C335" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i0us6m/tech_poured_monomer_back_in_bottle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="inlineStr">
+        <is>
+          <t>1i0ulkb</t>
+        </is>
+      </c>
+      <c r="B336" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wanna start getting my nails done more- what shape do you guys think is best? </t>
+        </is>
+      </c>
+      <c r="C336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rt4uwp6l4vce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="337">
+      <c r="A337" t="inlineStr">
+        <is>
+          <t>1i0uhnn</t>
+        </is>
+      </c>
+      <c r="B337" t="inlineStr">
+        <is>
+          <t>Here are some Christmas nails that I did, what manicure do you like more?✨</t>
+        </is>
+      </c>
+      <c r="C337" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0uhnn</t>
+        </is>
+      </c>
+    </row>
+    <row r="338">
+      <c r="A338" t="inlineStr">
+        <is>
+          <t>1i0uc8r</t>
+        </is>
+      </c>
+      <c r="B338" t="inlineStr">
+        <is>
+          <t>What could cause this?</t>
+        </is>
+      </c>
+      <c r="C338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0uc8r</t>
+        </is>
+      </c>
+    </row>
+    <row r="339">
+      <c r="A339" t="inlineStr">
+        <is>
+          <t>1i0u86j</t>
+        </is>
+      </c>
+      <c r="B339" t="inlineStr">
+        <is>
+          <t>Picked a preselected dip + chrome duo and I’m loving it 🩵</t>
+        </is>
+      </c>
+      <c r="C339" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0u86j</t>
+        </is>
+      </c>
+    </row>
+    <row r="340">
+      <c r="A340" t="inlineStr">
+        <is>
+          <t>1i0tltu</t>
+        </is>
+      </c>
+      <c r="B340" t="inlineStr">
+        <is>
+          <t>I paint my own nails, but how can I recreate this inspo? My attempt vs @nailsbyzola IG</t>
+        </is>
+      </c>
+      <c r="C340" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0tltu</t>
+        </is>
+      </c>
+    </row>
+    <row r="341">
+      <c r="A341" t="inlineStr">
+        <is>
+          <t>1i0tn61</t>
+        </is>
+      </c>
+      <c r="B341" t="inlineStr">
+        <is>
+          <t>My nails appears to be shrinking?</t>
+        </is>
+      </c>
+      <c r="C341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0tn61</t>
+        </is>
+      </c>
+    </row>
+    <row r="342">
+      <c r="A342" t="inlineStr">
+        <is>
+          <t>1i0si9w</t>
+        </is>
+      </c>
+      <c r="B342" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How common are splinter hemorrhages </t>
+        </is>
+      </c>
+      <c r="C342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0si9w</t>
+        </is>
+      </c>
+    </row>
+    <row r="343">
+      <c r="A343" t="inlineStr">
+        <is>
+          <t>1i0t7sc</t>
+        </is>
+      </c>
+      <c r="B343" t="inlineStr">
+        <is>
+          <t>New January nails</t>
+        </is>
+      </c>
+      <c r="C343" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0t7sc</t>
+        </is>
+      </c>
+    </row>
+    <row r="344">
+      <c r="A344" t="inlineStr">
+        <is>
+          <t>1i0t6la</t>
+        </is>
+      </c>
+      <c r="B344" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail question </t>
+        </is>
+      </c>
+      <c r="C344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vnqmk40lsuce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="345">
+      <c r="A345" t="inlineStr">
+        <is>
+          <t>1i0sq5i</t>
+        </is>
+      </c>
+      <c r="B345" t="inlineStr">
+        <is>
+          <t>Apres nail glue leaving residue on nails</t>
+        </is>
+      </c>
+      <c r="C345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i0sq5i/apres_nail_glue_leaving_residue_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="inlineStr">
+        <is>
+          <t>1i0s6mr</t>
+        </is>
+      </c>
+      <c r="B346" t="inlineStr">
+        <is>
+          <t>Non-dom hand always loses gel-x even with proper prep</t>
+        </is>
+      </c>
+      <c r="C346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0s6mr</t>
+        </is>
+      </c>
+    </row>
+    <row r="347">
+      <c r="A347" t="inlineStr">
+        <is>
+          <t>1i0s60z</t>
+        </is>
+      </c>
+      <c r="B347" t="inlineStr">
+        <is>
+          <t>I did my birthday nails a week early 🤭 first time using rhinestones and I feel so elegant 🤎</t>
+        </is>
+      </c>
+      <c r="C347" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0s60z</t>
+        </is>
+      </c>
+    </row>
+    <row r="348">
+      <c r="A348" t="inlineStr">
+        <is>
+          <t>1i0s0ox</t>
+        </is>
+      </c>
+      <c r="B348" t="inlineStr">
+        <is>
+          <t>rlly bad olive set i made on my natural nails :’) walmart didnt have the right green</t>
+        </is>
+      </c>
+      <c r="C348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1bcm6tb2juce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="349">
+      <c r="A349" t="inlineStr">
+        <is>
+          <t>1i0rxgn</t>
+        </is>
+      </c>
+      <c r="B349" t="inlineStr">
+        <is>
+          <t>Flower Child by ILNP is so pretty 💜✨</t>
+        </is>
+      </c>
+      <c r="C349" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0rxgn</t>
+        </is>
+      </c>
+    </row>
+    <row r="350">
+      <c r="A350" t="inlineStr">
+        <is>
+          <t>1i0rt6f</t>
+        </is>
+      </c>
+      <c r="B350" t="inlineStr">
+        <is>
+          <t>Pretty in pastel pink</t>
+        </is>
+      </c>
+      <c r="C350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0rt6f</t>
+        </is>
+      </c>
+    </row>
+    <row r="351">
+      <c r="A351" t="inlineStr">
+        <is>
+          <t>1i0rlva</t>
+        </is>
+      </c>
+      <c r="B351" t="inlineStr">
+        <is>
+          <t>What's the trick to making cuticles look good?</t>
+        </is>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/16fg0dkrfuce1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="inlineStr">
+        <is>
+          <t>1i0qy6z</t>
+        </is>
+      </c>
+      <c r="B352" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Elegant Winter Wedding Nails: A Gift for the Bride - constructive criticism and tips welcome! </t>
+        </is>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0qy6z</t>
+        </is>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="inlineStr">
+        <is>
+          <t>1i0qw2v</t>
+        </is>
+      </c>
+      <c r="B353" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beautiful nails and beautiful flowers </t>
+        </is>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yyl7g6z5auce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="inlineStr">
+        <is>
+          <t>1i0ql27</t>
+        </is>
+      </c>
+      <c r="B354" t="inlineStr">
+        <is>
+          <t>Ridges!</t>
+        </is>
+      </c>
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i0ql27/ridges/</t>
+        </is>
+      </c>
+    </row>
+    <row r="355">
+      <c r="A355" t="inlineStr">
+        <is>
+          <t>1i0qebm</t>
+        </is>
+      </c>
+      <c r="B355" t="inlineStr">
+        <is>
+          <t>What products do you guys use? Recommendations?</t>
+        </is>
+      </c>
+      <c r="C355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i0qebm/what_products_do_you_guys_use_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="356">
+      <c r="A356" t="inlineStr">
+        <is>
+          <t>1i0pp4s</t>
+        </is>
+      </c>
+      <c r="B356" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Why does my top coat do this? </t>
+        </is>
+      </c>
+      <c r="C356" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0pp4s</t>
+        </is>
+      </c>
+    </row>
+    <row r="357">
+      <c r="A357" t="inlineStr">
+        <is>
+          <t>1i0q958</t>
+        </is>
+      </c>
+      <c r="B357" t="inlineStr">
+        <is>
+          <t>I love this style</t>
+        </is>
+      </c>
+      <c r="C357" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bts4zvva5uce1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="358">
+      <c r="A358" t="inlineStr">
+        <is>
+          <t>1i0px6d</t>
+        </is>
+      </c>
+      <c r="B358" t="inlineStr">
+        <is>
+          <t>Is there a solution for square nails “softening” around the edges between appointments?</t>
+        </is>
+      </c>
+      <c r="C358" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i0px6d/is_there_a_solution_for_square_nails_softening/</t>
+        </is>
+      </c>
+    </row>
+    <row r="359">
+      <c r="A359" t="inlineStr">
+        <is>
+          <t>1i0pss0</t>
+        </is>
+      </c>
+      <c r="B359" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Feeling like a Princess 👸🏾 </t>
+        </is>
+      </c>
+      <c r="C359" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/87evd84v1uce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="360">
+      <c r="A360" t="inlineStr">
+        <is>
+          <t>1i0pn0d</t>
+        </is>
+      </c>
+      <c r="B360" t="inlineStr">
+        <is>
+          <t>Best online nail supply? 🇨🇦</t>
+        </is>
+      </c>
+      <c r="C360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i0pn0d/best_online_nail_supply/</t>
+        </is>
+      </c>
+    </row>
+    <row r="361">
+      <c r="A361" t="inlineStr">
+        <is>
+          <t>1i0pkxi</t>
+        </is>
+      </c>
+      <c r="B361" t="inlineStr">
+        <is>
+          <t>help me open this nail polish remover??</t>
+        </is>
+      </c>
+      <c r="C361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0pkxi</t>
+        </is>
+      </c>
+    </row>
+    <row r="362">
+      <c r="A362" t="inlineStr">
+        <is>
+          <t>1i0phfx</t>
+        </is>
+      </c>
+      <c r="B362" t="inlineStr">
+        <is>
+          <t>Dry cuticles</t>
+        </is>
+      </c>
+      <c r="C362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i0phfx/dry_cuticles/</t>
+        </is>
+      </c>
+    </row>
+    <row r="363">
+      <c r="A363" t="inlineStr">
+        <is>
+          <t>1i0pe8r</t>
+        </is>
+      </c>
+      <c r="B363" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First go at cat eye designs. </t>
+        </is>
+      </c>
+      <c r="C363" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/79lemznsytce1</t>
+        </is>
+      </c>
+    </row>
+    <row r="364">
+      <c r="A364" t="inlineStr">
+        <is>
+          <t>1i0pd66</t>
+        </is>
+      </c>
+      <c r="B364" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Necklace clasps are the worst! </t>
+        </is>
+      </c>
+      <c r="C364" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i0pd66/necklace_clasps_are_the_worst/</t>
+        </is>
+      </c>
+    </row>
+    <row r="365">
+      <c r="A365" t="inlineStr">
+        <is>
+          <t>1i0pbrg</t>
+        </is>
+      </c>
+      <c r="B365" t="inlineStr">
+        <is>
+          <t>New Year, New Nails</t>
+        </is>
+      </c>
+      <c r="C365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3dr7vzv9ytce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="366">
+      <c r="A366" t="inlineStr">
+        <is>
+          <t>1i0osst</t>
+        </is>
+      </c>
+      <c r="B366" t="inlineStr">
+        <is>
+          <t>I need help</t>
+        </is>
+      </c>
+      <c r="C366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i0osst/i_need_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="367">
+      <c r="A367" t="inlineStr">
+        <is>
+          <t>1i0p0bg</t>
+        </is>
+      </c>
+      <c r="B367" t="inlineStr">
+        <is>
+          <t>Are they cooked? 😭</t>
+        </is>
+      </c>
+      <c r="C367" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i0p0bg/are_they_cooked/</t>
+        </is>
+      </c>
+    </row>
+    <row r="368">
+      <c r="A368" t="inlineStr">
+        <is>
+          <t>1i0ows1</t>
+        </is>
+      </c>
+      <c r="B368" t="inlineStr">
+        <is>
+          <t>The white color is the best</t>
+        </is>
+      </c>
+      <c r="C368" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/iapxobj4vtce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="369">
+      <c r="A369" t="inlineStr">
+        <is>
+          <t>1i0otfc</t>
+        </is>
+      </c>
+      <c r="B369" t="inlineStr">
+        <is>
+          <t>Natural nails, I love it when I already have them like this se</t>
+        </is>
+      </c>
+      <c r="C369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0otfc</t>
+        </is>
+      </c>
+    </row>
+    <row r="370">
+      <c r="A370" t="inlineStr">
+        <is>
+          <t>1i0o8x8</t>
+        </is>
+      </c>
+      <c r="B370" t="inlineStr">
+        <is>
+          <t>Just a Trans Woman Showing off her after holiday nails Sorry about the tablecloth I have not changed it yet !</t>
+        </is>
+      </c>
+      <c r="C370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0o8x8</t>
+        </is>
+      </c>
+    </row>
+    <row r="371">
+      <c r="A371" t="inlineStr">
+        <is>
+          <t>1i0nqeh</t>
+        </is>
+      </c>
+      <c r="B371" t="inlineStr">
+        <is>
+          <t>Recommendation for preventing breakage, dont need more length?</t>
+        </is>
+      </c>
+      <c r="C371" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i0nqeh/recommendation_for_preventing_breakage_dont_need/</t>
+        </is>
+      </c>
+    </row>
+    <row r="372">
+      <c r="A372" t="inlineStr">
+        <is>
+          <t>1i0nvgr</t>
+        </is>
+      </c>
+      <c r="B372" t="inlineStr">
+        <is>
+          <t>Pretty 🍷</t>
+        </is>
+      </c>
+      <c r="C372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0nvgr</t>
+        </is>
+      </c>
+    </row>
+    <row r="373">
+      <c r="A373" t="inlineStr">
+        <is>
+          <t>1i0nv74</t>
+        </is>
+      </c>
+      <c r="B373" t="inlineStr">
+        <is>
+          <t>Thinking about taking the online course, thoughts?</t>
+        </is>
+      </c>
+      <c r="C373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i0nv74/thinking_about_taking_the_online_course_thoughts/</t>
+        </is>
+      </c>
+    </row>
+    <row r="374">
+      <c r="A374" t="inlineStr">
+        <is>
+          <t>1i0np45</t>
+        </is>
+      </c>
+      <c r="B374" t="inlineStr">
+        <is>
+          <t>Looking for full coverage nail tips with special s-curve Edge</t>
+        </is>
+      </c>
+      <c r="C374" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0np45</t>
+        </is>
+      </c>
+    </row>
+    <row r="375">
+      <c r="A375" t="inlineStr">
+        <is>
+          <t>1i0n7nj</t>
+        </is>
+      </c>
+      <c r="B375" t="inlineStr">
+        <is>
+          <t>Fashion and nails</t>
+        </is>
+      </c>
+      <c r="C375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0n7nj</t>
+        </is>
+      </c>
+    </row>
+    <row r="376">
+      <c r="A376" t="inlineStr">
+        <is>
+          <t>1i0nkom</t>
+        </is>
+      </c>
+      <c r="B376" t="inlineStr">
+        <is>
+          <t>January set 🥰</t>
+        </is>
+      </c>
+      <c r="C376" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e0w8s07altce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="377">
+      <c r="A377" t="inlineStr">
+        <is>
+          <t>1i0n9lz</t>
+        </is>
+      </c>
+      <c r="B377" t="inlineStr">
+        <is>
+          <t>pink rainbows 🌷🌈</t>
+        </is>
+      </c>
+      <c r="C377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0n9lz</t>
+        </is>
+      </c>
+    </row>
+    <row r="378">
+      <c r="A378" t="inlineStr">
+        <is>
+          <t>1i0mnqr</t>
+        </is>
+      </c>
+      <c r="B378" t="inlineStr">
+        <is>
+          <t>new nails :)</t>
+        </is>
+      </c>
+      <c r="C378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xs333jlletce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="379">
+      <c r="A379" t="inlineStr">
+        <is>
+          <t>1i0mf83</t>
+        </is>
+      </c>
+      <c r="B379" t="inlineStr">
+        <is>
+          <t>Cuticle/nail care tips?</t>
+        </is>
+      </c>
+      <c r="C379" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nlx19qstctce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="380">
+      <c r="A380" t="inlineStr">
+        <is>
+          <t>1i0m5wr</t>
+        </is>
+      </c>
+      <c r="B380" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My past 3 sets, long and sharp! </t>
+        </is>
+      </c>
+      <c r="C380" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0m5wr</t>
+        </is>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="inlineStr">
+        <is>
+          <t>1i0lzxt</t>
+        </is>
+      </c>
+      <c r="B381" t="inlineStr">
+        <is>
+          <t>Dip powder alternatives?</t>
+        </is>
+      </c>
+      <c r="C381" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/l2oaiccq9tce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="inlineStr">
+        <is>
+          <t>1i0lv56</t>
+        </is>
+      </c>
+      <c r="B382" t="inlineStr">
+        <is>
+          <t>Braved the Nail Salon - Love Them!!</t>
+        </is>
+      </c>
+      <c r="C382" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ljmklroq8tce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="inlineStr">
+        <is>
+          <t>1i0kr2w</t>
+        </is>
+      </c>
+      <c r="B383" t="inlineStr">
+        <is>
+          <t>What is this type of breakage called and how to treat it?</t>
+        </is>
+      </c>
+      <c r="C383" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1khsg0po0tce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="inlineStr">
+        <is>
+          <t>1i0l8rj</t>
+        </is>
+      </c>
+      <c r="B384" t="inlineStr">
+        <is>
+          <t>Nobody tell me these nails aren't FIRE!!! I love em'</t>
+        </is>
+      </c>
+      <c r="C384" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ib2qx6ew3tce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="inlineStr">
+        <is>
+          <t>1i0lkjh</t>
+        </is>
+      </c>
+      <c r="B385" t="inlineStr">
+        <is>
+          <t>I kinda get Sailor Moon vibes from my newest set 🌙</t>
+        </is>
+      </c>
+      <c r="C385" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qxnrgnim6tce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="inlineStr">
+        <is>
+          <t>1i0kckt</t>
+        </is>
+      </c>
+      <c r="B386" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love a cat eye moment </t>
+        </is>
+      </c>
+      <c r="C386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bpzs3l0uxsce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="inlineStr">
+        <is>
+          <t>1i0k3ts</t>
+        </is>
+      </c>
+      <c r="B387" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Strengthening gel manicure? </t>
+        </is>
+      </c>
+      <c r="C387" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u1j83rc4wsce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="inlineStr">
+        <is>
+          <t>1i0jumv</t>
+        </is>
+      </c>
+      <c r="B388" t="inlineStr">
+        <is>
+          <t xml:space="preserve">motivational quote but make it nail art </t>
+        </is>
+      </c>
+      <c r="C388" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0jumv</t>
+        </is>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="inlineStr">
+        <is>
+          <t>1i0jtrm</t>
+        </is>
+      </c>
+      <c r="B389" t="inlineStr">
+        <is>
+          <t>Can I use Gel Fake Nails with regular nail glue?</t>
+        </is>
+      </c>
+      <c r="C389" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i0jtrm/can_i_use_gel_fake_nails_with_regular_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="inlineStr">
+        <is>
+          <t>1i0jr3e</t>
+        </is>
+      </c>
+      <c r="B390" t="inlineStr">
+        <is>
+          <t>Do I love this polish or hate it??</t>
+        </is>
+      </c>
+      <c r="C390" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0jr3e</t>
+        </is>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="inlineStr">
+        <is>
+          <t>1i0jq2z</t>
+        </is>
+      </c>
+      <c r="B391" t="inlineStr">
+        <is>
+          <t>Two Years Apart</t>
+        </is>
+      </c>
+      <c r="C391" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0jq2z</t>
+        </is>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="inlineStr">
+        <is>
+          <t>1i0jhnn</t>
+        </is>
+      </c>
+      <c r="B392" t="inlineStr">
+        <is>
+          <t>Have to remove dip nails for wisdom teeth surgery</t>
+        </is>
+      </c>
+      <c r="C392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i0jhnn/have_to_remove_dip_nails_for_wisdom_teeth_surgery/</t>
+        </is>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="inlineStr">
+        <is>
+          <t>1i0jh2h</t>
+        </is>
+      </c>
+      <c r="B393" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Invader zim! </t>
+        </is>
+      </c>
+      <c r="C393" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0jh2h</t>
+        </is>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="inlineStr">
+        <is>
+          <t>1i0jbcx</t>
+        </is>
+      </c>
+      <c r="B394" t="inlineStr">
+        <is>
+          <t>did two small photo shoots for my holiday nails🤭🩵</t>
+        </is>
+      </c>
+      <c r="C394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0jbcx</t>
+        </is>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="inlineStr">
+        <is>
+          <t>1i0etve</t>
+        </is>
+      </c>
+      <c r="B395" t="inlineStr">
+        <is>
+          <t>which nail shape is better o:? the second one is more rounded (did not have a better picture, I am sorry 😭🙏🏻)</t>
+        </is>
+      </c>
+      <c r="C395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0etve</t>
+        </is>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="inlineStr">
+        <is>
+          <t>1i0hste</t>
+        </is>
+      </c>
+      <c r="B396" t="inlineStr">
+        <is>
+          <t>I’ve got a nail appt in 3 days and an event in 5, can the tech work around this break or should I wait for it to fully heal?</t>
+        </is>
+      </c>
+      <c r="C396" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f9wu2c28fsce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="inlineStr">
+        <is>
+          <t>1i0j7un</t>
+        </is>
+      </c>
+      <c r="B397" t="inlineStr">
+        <is>
+          <t>✨</t>
+        </is>
+      </c>
+      <c r="C397" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0j7un</t>
+        </is>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="inlineStr">
+        <is>
+          <t>1i0j7hd</t>
+        </is>
+      </c>
+      <c r="B398" t="inlineStr">
+        <is>
+          <t>I feel like I’ve mastered the super clean manicure! So happy with how they turned out for our engagements</t>
+        </is>
+      </c>
+      <c r="C398" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9vbt351ipsce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="399">
+      <c r="A399" t="inlineStr">
+        <is>
+          <t>1i0j6lb</t>
+        </is>
+      </c>
+      <c r="B399" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Birthday cake set 🎂 </t>
+        </is>
+      </c>
+      <c r="C399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0j6lb</t>
+        </is>
+      </c>
+    </row>
+    <row r="400">
+      <c r="A400" t="inlineStr">
+        <is>
+          <t>1i0j516</t>
+        </is>
+      </c>
+      <c r="B400" t="inlineStr">
+        <is>
+          <t>🖤🖤</t>
+        </is>
+      </c>
+      <c r="C400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0j516</t>
+        </is>
+      </c>
+    </row>
+    <row r="401">
+      <c r="A401" t="inlineStr">
+        <is>
+          <t>1i0j3vm</t>
+        </is>
+      </c>
+      <c r="B401" t="inlineStr">
+        <is>
+          <t>Black and white 🖤</t>
+        </is>
+      </c>
+      <c r="C401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0j3vm</t>
+        </is>
+      </c>
+    </row>
+    <row r="402">
+      <c r="A402" t="inlineStr">
+        <is>
+          <t>1i10ho8</t>
+        </is>
+      </c>
+      <c r="B402" t="inlineStr">
+        <is>
+          <t>How do you clean and sanitize under long nails?</t>
+        </is>
+      </c>
+      <c r="C402" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i10ho8/how_do_you_clean_and_sanitize_under_long_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="403">
+      <c r="A403" t="inlineStr">
+        <is>
+          <t>1i105l8</t>
+        </is>
+      </c>
+      <c r="B403" t="inlineStr">
+        <is>
+          <t>In love with magnetics!</t>
+        </is>
+      </c>
+      <c r="C403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i105l8</t>
+        </is>
+      </c>
+    </row>
+    <row r="404">
+      <c r="A404" t="inlineStr">
+        <is>
+          <t>1i0zv2v</t>
+        </is>
+      </c>
+      <c r="B404" t="inlineStr">
+        <is>
+          <t>Fool's Paradise contains multitudes (and is an unexpectedly good Wicked-themed polish too - see the 4th photo)</t>
+        </is>
+      </c>
+      <c r="C404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0zv2v</t>
+        </is>
+      </c>
+    </row>
+    <row r="405">
+      <c r="A405" t="inlineStr">
+        <is>
+          <t>1i0zrvd</t>
+        </is>
+      </c>
+      <c r="B405" t="inlineStr">
+        <is>
+          <t>When your nail art matches a chicken</t>
+        </is>
+      </c>
+      <c r="C405" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w7iz3w8gjwce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="406">
+      <c r="A406" t="inlineStr">
+        <is>
+          <t>1i0yp82</t>
+        </is>
+      </c>
+      <c r="B406" t="inlineStr">
+        <is>
+          <t>Milky shimmers polish</t>
+        </is>
+      </c>
+      <c r="C406" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i0yp82/milky_shimmers_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="407">
+      <c r="A407" t="inlineStr">
+        <is>
+          <t>1i0yd0n</t>
+        </is>
+      </c>
+      <c r="B407" t="inlineStr">
+        <is>
+          <t>Recent stamping attempts</t>
+        </is>
+      </c>
+      <c r="C407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0yd0n</t>
+        </is>
+      </c>
+    </row>
+    <row r="408">
+      <c r="A408" t="inlineStr">
+        <is>
+          <t>1i0y3da</t>
+        </is>
+      </c>
+      <c r="B408" t="inlineStr">
+        <is>
+          <t>{PR} Sassy Sauce | HHC - ✨ Thighs the Limit ✨</t>
+        </is>
+      </c>
+      <c r="C408" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0y3da</t>
+        </is>
+      </c>
+    </row>
+    <row r="409">
+      <c r="A409" t="inlineStr">
+        <is>
+          <t>1i0xfp8</t>
+        </is>
+      </c>
+      <c r="B409" t="inlineStr">
+        <is>
+          <t>Nail Art Attempt #2</t>
+        </is>
+      </c>
+      <c r="C409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0xfp8</t>
+        </is>
+      </c>
+    </row>
+    <row r="410">
+      <c r="A410" t="inlineStr">
+        <is>
+          <t>1i0wjlt</t>
+        </is>
+      </c>
+      <c r="B410" t="inlineStr">
+        <is>
+          <t>This happens every now and then with some lacquers and I don’t know how to prevent it</t>
+        </is>
+      </c>
+      <c r="C410" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/se3nqxbzlvce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="411">
+      <c r="A411" t="inlineStr">
+        <is>
+          <t>1i0w9mp</t>
+        </is>
+      </c>
+      <c r="B411" t="inlineStr">
+        <is>
+          <t>Fire Ruby</t>
+        </is>
+      </c>
+      <c r="C411" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0w9mp</t>
+        </is>
+      </c>
+    </row>
+    <row r="412">
+      <c r="A412" t="inlineStr">
+        <is>
+          <t>1i0w4g6</t>
+        </is>
+      </c>
+      <c r="B412" t="inlineStr">
+        <is>
+          <t>Capricorn (the goat) ♑️🌙✨💖</t>
+        </is>
+      </c>
+      <c r="C412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0w4g6</t>
+        </is>
+      </c>
+    </row>
+    <row r="413">
+      <c r="A413" t="inlineStr">
+        <is>
+          <t>1i0vuta</t>
+        </is>
+      </c>
+      <c r="B413" t="inlineStr">
+        <is>
+          <t>Adding a topper when you’re too lazy to redo your nails👏</t>
+        </is>
+      </c>
+      <c r="C413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0vuta</t>
+        </is>
+      </c>
+    </row>
+    <row r="414">
+      <c r="A414" t="inlineStr">
+        <is>
+          <t>1i0vjy3</t>
+        </is>
+      </c>
+      <c r="B414" t="inlineStr">
+        <is>
+          <t>Zoya mobile site</t>
+        </is>
+      </c>
+      <c r="C414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i0vjy3/zoya_mobile_site/</t>
+        </is>
+      </c>
+    </row>
+    <row r="415">
+      <c r="A415" t="inlineStr">
+        <is>
+          <t>1i0u40w</t>
+        </is>
+      </c>
+      <c r="B415" t="inlineStr">
+        <is>
+          <t>Casino night ❤️♠️🎱</t>
+        </is>
+      </c>
+      <c r="C415" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eudxudrc0vce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="416">
+      <c r="A416" t="inlineStr">
+        <is>
+          <t>1i0trlu</t>
+        </is>
+      </c>
+      <c r="B416" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Good customer service this week! Plus Psilocin/Norpsilocin. </t>
+        </is>
+      </c>
+      <c r="C416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0trlu</t>
+        </is>
+      </c>
+    </row>
+    <row r="417">
+      <c r="A417" t="inlineStr">
+        <is>
+          <t>1i0tmfl</t>
+        </is>
+      </c>
+      <c r="B417" t="inlineStr">
+        <is>
+          <t>palate cleanser with remixed daybreak</t>
+        </is>
+      </c>
+      <c r="C417" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pfs0ojx8wuce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="418">
+      <c r="A418" t="inlineStr">
+        <is>
+          <t>1i0tbz5</t>
+        </is>
+      </c>
+      <c r="B418" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Am I missing something or is this the craziest price gouging? </t>
+        </is>
+      </c>
+      <c r="C418" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0xcb15vttuce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="419">
+      <c r="A419" t="inlineStr">
+        <is>
+          <t>1i0t3l7</t>
+        </is>
+      </c>
+      <c r="B419" t="inlineStr">
+        <is>
+          <t>Finally finished swatching!</t>
+        </is>
+      </c>
+      <c r="C419" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rky1lh8wruce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="420">
+      <c r="A420" t="inlineStr">
+        <is>
+          <t>1i0smw5</t>
+        </is>
+      </c>
+      <c r="B420" t="inlineStr">
+        <is>
+          <t>Lacquergram: how long does it take to update a polish photo?</t>
+        </is>
+      </c>
+      <c r="C420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i0smw5/lacquergram_how_long_does_it_take_to_update_a/</t>
+        </is>
+      </c>
+    </row>
+    <row r="421">
+      <c r="A421" t="inlineStr">
+        <is>
+          <t>1i0skst</t>
+        </is>
+      </c>
+      <c r="B421" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The first week of my 2025 mani tracker blanket </t>
+        </is>
+      </c>
+      <c r="C421" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r6oar1ymnuce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="422">
+      <c r="A422" t="inlineStr">
+        <is>
+          <t>1i0sh02</t>
+        </is>
+      </c>
+      <c r="B422" t="inlineStr">
+        <is>
+          <t>Is Naps and Nails a Black-owned brand?</t>
+        </is>
+      </c>
+      <c r="C422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i0sh02/is_naps_and_nails_a_blackowned_brand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="423">
+      <c r="A423" t="inlineStr">
+        <is>
+          <t>1i0npbj</t>
+        </is>
+      </c>
+      <c r="B423" t="inlineStr">
+        <is>
+          <t>Questions about gel nail allergies</t>
+        </is>
+      </c>
+      <c r="C423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i0npbj/questions_about_gel_nail_allergies/</t>
+        </is>
+      </c>
+    </row>
+    <row r="424">
+      <c r="A424" t="inlineStr">
+        <is>
+          <t>1i0orl8</t>
+        </is>
+      </c>
+      <c r="B424" t="inlineStr">
+        <is>
+          <t>My favorite deep red/velvet nails</t>
+        </is>
+      </c>
+      <c r="C424" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0orl8</t>
+        </is>
+      </c>
+    </row>
+    <row r="425">
+      <c r="A425" t="inlineStr">
+        <is>
+          <t>1i0rb7m</t>
+        </is>
+      </c>
+      <c r="B425" t="inlineStr">
+        <is>
+          <t>These nails are singlehandedly the reason for my anxiety</t>
+        </is>
+      </c>
+      <c r="C425" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3x8vx49cduce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="426">
+      <c r="A426" t="inlineStr">
+        <is>
+          <t>1i0r1sn</t>
+        </is>
+      </c>
+      <c r="B426" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Need to find a matching creme </t>
+        </is>
+      </c>
+      <c r="C426" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oyziwlqebuce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="427">
+      <c r="A427" t="inlineStr">
+        <is>
+          <t>1i0qv07</t>
+        </is>
+      </c>
+      <c r="B427" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pretty, shifty, chromey </t>
+        </is>
+      </c>
+      <c r="C427" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o6b5m2yw9uce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="428">
+      <c r="A428" t="inlineStr">
+        <is>
+          <t>1i0qorx</t>
+        </is>
+      </c>
+      <c r="B428" t="inlineStr">
+        <is>
+          <t>DaVinci's Nightie</t>
+        </is>
+      </c>
+      <c r="C428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0qorx</t>
+        </is>
+      </c>
+    </row>
+    <row r="429">
+      <c r="A429" t="inlineStr">
+        <is>
+          <t>1i0q7u1</t>
+        </is>
+      </c>
+      <c r="B429" t="inlineStr">
+        <is>
+          <t>Sea Glass💙✨</t>
+        </is>
+      </c>
+      <c r="C429" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/8ecf1d6y4uce1</t>
+        </is>
+      </c>
+    </row>
+    <row r="430">
+      <c r="A430" t="inlineStr">
+        <is>
+          <t>1i0q7xm</t>
+        </is>
+      </c>
+      <c r="B430" t="inlineStr">
+        <is>
+          <t>Nail Polish benefiting Reproductive Healthcare?</t>
+        </is>
+      </c>
+      <c r="C430" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i0q7xm/nail_polish_benefiting_reproductive_healthcare/</t>
+        </is>
+      </c>
+    </row>
+    <row r="431">
+      <c r="A431" t="inlineStr">
+        <is>
+          <t>1i0q75l</t>
+        </is>
+      </c>
+      <c r="B431" t="inlineStr">
+        <is>
+          <t>My nails match my walls! Skate Date</t>
+        </is>
+      </c>
+      <c r="C431" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0q75l</t>
+        </is>
+      </c>
+    </row>
+    <row r="432">
+      <c r="A432" t="inlineStr">
+        <is>
+          <t>1i0pxgd</t>
+        </is>
+      </c>
+      <c r="B432" t="inlineStr">
+        <is>
+          <t>Does this not look like a cute little grassy field??🌱</t>
+        </is>
+      </c>
+      <c r="C432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0pxgd</t>
+        </is>
+      </c>
+    </row>
+    <row r="433">
+      <c r="A433" t="inlineStr">
+        <is>
+          <t>1i0pj2f</t>
+        </is>
+      </c>
+      <c r="B433" t="inlineStr">
+        <is>
+          <t>Mooncat - Am I Everything You Fear?</t>
+        </is>
+      </c>
+      <c r="C433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0pj2f</t>
+        </is>
+      </c>
+    </row>
+    <row r="434">
+      <c r="A434" t="inlineStr">
+        <is>
+          <t>1i0pfob</t>
+        </is>
+      </c>
+      <c r="B434" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lightning in a bottle </t>
+        </is>
+      </c>
+      <c r="C434" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ip4y1tr3ztce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="435">
+      <c r="A435" t="inlineStr">
+        <is>
+          <t>1i0oq1q</t>
+        </is>
+      </c>
+      <c r="B435" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Snowflake French manicure! It was a pain in the butt, but I love it! </t>
+        </is>
+      </c>
+      <c r="C435" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jenqs0ppttce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="436">
+      <c r="A436" t="inlineStr">
+        <is>
+          <t>1i0nwh2</t>
+        </is>
+      </c>
+      <c r="B436" t="inlineStr">
+        <is>
+          <t>How do you trim your nails without cracking/peeling?</t>
+        </is>
+      </c>
+      <c r="C436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i0nwh2/how_do_you_trim_your_nails_without_crackingpeeling/</t>
+        </is>
+      </c>
+    </row>
+    <row r="437">
+      <c r="A437" t="inlineStr">
+        <is>
+          <t>1i0njec</t>
+        </is>
+      </c>
+      <c r="B437" t="inlineStr">
+        <is>
+          <t>Loving the soft glowy vibes!</t>
+        </is>
+      </c>
+      <c r="C437" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/62r6t20uktce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="438">
+      <c r="A438" t="inlineStr">
+        <is>
+          <t>1i0naia</t>
+        </is>
+      </c>
+      <c r="B438" t="inlineStr">
+        <is>
+          <t>BKL - Ghost Walker</t>
+        </is>
+      </c>
+      <c r="C438" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0naia</t>
+        </is>
+      </c>
+    </row>
+    <row r="439">
+      <c r="A439" t="inlineStr">
+        <is>
+          <t>1i0ln43</t>
+        </is>
+      </c>
+      <c r="B439" t="inlineStr">
+        <is>
+          <t>Vintage dusties- peachy melon crelly dupe?</t>
+        </is>
+      </c>
+      <c r="C439" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t402n8t37tce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="440">
+      <c r="A440" t="inlineStr">
+        <is>
+          <t>1i0llp4</t>
+        </is>
+      </c>
+      <c r="B440" t="inlineStr">
+        <is>
+          <t>Dupe for mooncat</t>
+        </is>
+      </c>
+      <c r="C440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i0llp4/dupe_for_mooncat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="441">
+      <c r="A441" t="inlineStr">
+        <is>
+          <t>1i0lk8w</t>
+        </is>
+      </c>
+      <c r="B441" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Good dupe for Olive &amp; June’s CV? </t>
+        </is>
+      </c>
+      <c r="C441" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0lk8w</t>
+        </is>
+      </c>
+    </row>
+    <row r="442">
+      <c r="A442" t="inlineStr">
+        <is>
+          <t>1i0l8e7</t>
+        </is>
+      </c>
+      <c r="B442" t="inlineStr">
+        <is>
+          <t>Label Size for Brother P-Touch for Swatch Labels?</t>
+        </is>
+      </c>
+      <c r="C442" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i0l8e7/label_size_for_brother_ptouch_for_swatch_labels/</t>
+        </is>
+      </c>
+    </row>
+    <row r="443">
+      <c r="A443" t="inlineStr">
+        <is>
+          <t>1i0kk25</t>
+        </is>
+      </c>
+      <c r="B443" t="inlineStr">
+        <is>
+          <t>Favorite Brand for Creams under $10</t>
+        </is>
+      </c>
+      <c r="C443" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i0kk25/favorite_brand_for_creams_under_10/</t>
+        </is>
+      </c>
+    </row>
+    <row r="444">
+      <c r="A444" t="inlineStr">
+        <is>
+          <t>1i0kbc8</t>
+        </is>
+      </c>
+      <c r="B444" t="inlineStr">
+        <is>
+          <t>I present to you: the blurple velvet showdown 💜💙🩵</t>
+        </is>
+      </c>
+      <c r="C444" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/p7pkmd6lxsce1</t>
+        </is>
+      </c>
+    </row>
+    <row r="445">
+      <c r="A445" t="inlineStr">
+        <is>
+          <t>1i0k1c9</t>
+        </is>
+      </c>
+      <c r="B445" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Polishes with a comparable shift to cock a doodle doom? </t>
+        </is>
+      </c>
+      <c r="C445" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i0k1c9/polishes_with_a_comparable_shift_to_cock_a_doodle/</t>
+        </is>
+      </c>
+    </row>
+    <row r="446">
+      <c r="A446" t="inlineStr">
+        <is>
+          <t>1i0jtj8</t>
+        </is>
+      </c>
+      <c r="B446" t="inlineStr">
+        <is>
+          <t>After YEARS of acrylics…</t>
+        </is>
+      </c>
+      <c r="C446" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/txjci4j0usce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="447">
+      <c r="A447" t="inlineStr">
+        <is>
+          <t>1i0jicv</t>
+        </is>
+      </c>
+      <c r="B447" t="inlineStr">
+        <is>
+          <t>Vampy Red Comparisons</t>
+        </is>
+      </c>
+      <c r="C447" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zgm74obnrsce1</t>
+        </is>
+      </c>
+    </row>
+    <row r="448">
+      <c r="A448" t="inlineStr">
+        <is>
+          <t>1i0j4jj</t>
+        </is>
+      </c>
+      <c r="B448" t="inlineStr">
+        <is>
+          <t>Nail Envy Base Coat</t>
+        </is>
+      </c>
+      <c r="C448" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i0j4jj/nail_envy_base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="449">
+      <c r="A449" t="inlineStr">
+        <is>
+          <t>1i0imy3</t>
+        </is>
+      </c>
+      <c r="B449" t="inlineStr">
+        <is>
+          <t>anyone else whips out their camera as soon as they see beautiful plants/flowers to take mani pics?</t>
+        </is>
+      </c>
+      <c r="C449" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0imy3</t>
+        </is>
+      </c>
+    </row>
+    <row r="450">
+      <c r="A450" t="inlineStr">
+        <is>
+          <t>1i0ijyy</t>
+        </is>
+      </c>
+      <c r="B450" t="inlineStr">
+        <is>
+          <t>Pearlescent Nails</t>
+        </is>
+      </c>
+      <c r="C450" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0ijyy</t>
+        </is>
+      </c>
+    </row>
+    <row r="451">
+      <c r="A451" t="inlineStr">
+        <is>
+          <t>1i0ic3b</t>
+        </is>
+      </c>
+      <c r="B451" t="inlineStr">
+        <is>
+          <t>They look like portals into an oceanic abyss</t>
+        </is>
+      </c>
+      <c r="C451" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0ic3b</t>
+        </is>
+      </c>
+    </row>
+    <row r="452">
+      <c r="A452" t="inlineStr">
+        <is>
+          <t>1i0iaq6</t>
+        </is>
+      </c>
+      <c r="B452" t="inlineStr">
+        <is>
+          <t>mooncat order turnaround</t>
+        </is>
+      </c>
+      <c r="C452" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p5icbezyisce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="453">
+      <c r="A453" t="inlineStr">
+        <is>
+          <t>1i0i1se</t>
+        </is>
+      </c>
+      <c r="B453" t="inlineStr">
+        <is>
+          <t>Product recommendations?</t>
+        </is>
+      </c>
+      <c r="C453" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i0i1se/product_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="454">
+      <c r="A454" t="inlineStr">
+        <is>
+          <t>1i0hyhd</t>
+        </is>
+      </c>
+      <c r="B454" t="inlineStr">
+        <is>
+          <t>Rainbow Mountain 🌈🌟</t>
+        </is>
+      </c>
+      <c r="C454" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0hyhd</t>
+        </is>
+      </c>
+    </row>
+    <row r="455">
+      <c r="A455" t="inlineStr">
+        <is>
+          <t>1i0hsm8</t>
+        </is>
+      </c>
+      <c r="B455" t="inlineStr">
+        <is>
+          <t>❄️ Winter velvet ❄️</t>
+        </is>
+      </c>
+      <c r="C455" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0hsm8</t>
+        </is>
+      </c>
+    </row>
+    <row r="456">
+      <c r="A456" t="inlineStr">
+        <is>
+          <t>1i0hoa8</t>
+        </is>
+      </c>
+      <c r="B456" t="inlineStr">
+        <is>
+          <t>An Aurora Borealis on my nails 🤩</t>
+        </is>
+      </c>
+      <c r="C456" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7ygatlr8esce1</t>
+        </is>
+      </c>
+    </row>
+    <row r="457">
+      <c r="A457" t="inlineStr">
+        <is>
+          <t>1i0h6nq</t>
+        </is>
+      </c>
+      <c r="B457" t="inlineStr">
+        <is>
+          <t>HoH is really that b****</t>
+        </is>
+      </c>
+      <c r="C457" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0h6nq</t>
+        </is>
+      </c>
+    </row>
+    <row r="458">
+      <c r="A458" t="inlineStr">
+        <is>
+          <t>1i0gnxo</t>
+        </is>
+      </c>
+      <c r="B458" t="inlineStr">
+        <is>
+          <t>Great Lakes Lacquer shipping</t>
+        </is>
+      </c>
+      <c r="C458" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0gnxo</t>
+        </is>
+      </c>
+    </row>
+    <row r="459">
+      <c r="A459" t="inlineStr">
+        <is>
+          <t>1i0fbfz</t>
+        </is>
+      </c>
+      <c r="B459" t="inlineStr">
+        <is>
+          <t>Night Owl Lacquer - Cloud City ☁️</t>
+        </is>
+      </c>
+      <c r="C459" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0fbfz</t>
+        </is>
+      </c>
+    </row>
+    <row r="460">
+      <c r="A460" t="inlineStr">
+        <is>
+          <t>1i0evns</t>
+        </is>
+      </c>
+      <c r="B460" t="inlineStr">
+        <is>
+          <t>I need help ID-ing this mystery Essie shade (Chocolate cakes?).</t>
+        </is>
+      </c>
+      <c r="C460" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0evns</t>
+        </is>
+      </c>
+    </row>
+    <row r="461">
+      <c r="A461" t="inlineStr">
+        <is>
+          <t>1i0ek34</t>
+        </is>
+      </c>
+      <c r="B461" t="inlineStr">
+        <is>
+          <t>💙Sonic the Hedgehog💙</t>
+        </is>
+      </c>
+      <c r="C461" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0ek34</t>
+        </is>
+      </c>
+    </row>
+    <row r="462">
+      <c r="A462" t="inlineStr">
+        <is>
+          <t>1i0chg4</t>
+        </is>
+      </c>
+      <c r="B462" t="inlineStr">
+        <is>
+          <t>Content creation</t>
+        </is>
+      </c>
+      <c r="C462" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i0chg4/content_creation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="463">
+      <c r="A463" t="inlineStr">
+        <is>
+          <t>1i0c0ng</t>
+        </is>
+      </c>
+      <c r="B463" t="inlineStr">
+        <is>
+          <t xml:space="preserve">W7 Mega Holo </t>
+        </is>
+      </c>
+      <c r="C463" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/mrm6va7dzqce1</t>
+        </is>
+      </c>
+    </row>
+    <row r="464">
+      <c r="A464" t="inlineStr">
+        <is>
+          <t>1i0bjg7</t>
+        </is>
+      </c>
+      <c r="B464" t="inlineStr">
+        <is>
+          <t>No Dumb Questions + Casual Talk</t>
+        </is>
+      </c>
+      <c r="C464" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i0bjg7/no_dumb_questions_casual_talk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="465">
+      <c r="A465" t="inlineStr">
+        <is>
+          <t>1i0bdx3</t>
+        </is>
+      </c>
+      <c r="B465" t="inlineStr">
+        <is>
+          <t>Weird question...</t>
+        </is>
+      </c>
+      <c r="C465" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i0bdx3/weird_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="466">
+      <c r="A466" t="inlineStr">
+        <is>
+          <t>1i0b5rb</t>
+        </is>
+      </c>
+      <c r="B466" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Regretted the color scheme later because it reminds me too much of toothpaste </t>
+        </is>
+      </c>
+      <c r="C466" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hpgl9thboqce1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="467">
+      <c r="A467" t="inlineStr">
+        <is>
+          <t>1i0acit</t>
+        </is>
+      </c>
+      <c r="B467" t="inlineStr">
+        <is>
+          <t>The gradient is slight, but it's still there!!!</t>
+        </is>
+      </c>
+      <c r="C467" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0acit</t>
+        </is>
+      </c>
+    </row>
+    <row r="468">
+      <c r="A468" t="inlineStr">
+        <is>
+          <t>1i0135d</t>
+        </is>
+      </c>
+      <c r="B468" t="inlineStr">
+        <is>
+          <t>I need help with my nails!!</t>
+        </is>
+      </c>
+      <c r="C468" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0135d</t>
+        </is>
+      </c>
+    </row>
+    <row r="469">
+      <c r="A469" t="inlineStr">
+        <is>
+          <t>1i01acv</t>
+        </is>
+      </c>
+      <c r="B469" t="inlineStr">
+        <is>
+          <t>Biab hype??</t>
+        </is>
+      </c>
+      <c r="C469" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i01acv/biab_hype/</t>
+        </is>
+      </c>
+    </row>
+    <row r="470">
+      <c r="A470" t="inlineStr">
+        <is>
+          <t>1i09yre</t>
+        </is>
+      </c>
+      <c r="B470" t="inlineStr">
+        <is>
+          <t>Holo Taco layering combo</t>
+        </is>
+      </c>
+      <c r="C470" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i09yre</t>
+        </is>
+      </c>
+    </row>
+    <row r="471">
+      <c r="A471" t="inlineStr">
+        <is>
+          <t>1i0z8pu</t>
+        </is>
+      </c>
+      <c r="B471" t="inlineStr">
+        <is>
+          <t>Should I make my tips longer or keep as is?</t>
+        </is>
+      </c>
+      <c r="C471" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0z8pu</t>
+        </is>
+      </c>
+    </row>
+    <row r="472">
+      <c r="A472" t="inlineStr">
+        <is>
+          <t>1i0xdpn</t>
+        </is>
+      </c>
+      <c r="B472" t="inlineStr">
+        <is>
+          <t>Nail Art Attempt #2</t>
+        </is>
+      </c>
+      <c r="C472" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0xdpn</t>
+        </is>
+      </c>
+    </row>
+    <row r="473">
+      <c r="A473" t="inlineStr">
+        <is>
+          <t>1i0x87e</t>
+        </is>
+      </c>
+      <c r="B473" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Yellow Animal print </t>
+        </is>
+      </c>
+      <c r="C473" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wymjbz3csvce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="474">
+      <c r="A474" t="inlineStr">
+        <is>
+          <t>1i0vepw</t>
+        </is>
+      </c>
+      <c r="B474" t="inlineStr">
+        <is>
+          <t>Snake Nails</t>
+        </is>
+      </c>
+      <c r="C474" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9canlackbvce1</t>
+        </is>
+      </c>
+    </row>
+    <row r="475">
+      <c r="A475" t="inlineStr">
+        <is>
+          <t>1i0uauq</t>
+        </is>
+      </c>
+      <c r="B475" t="inlineStr">
+        <is>
+          <t>the little prince hand painted🦊🌕</t>
+        </is>
+      </c>
+      <c r="C475" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0uauq</t>
+        </is>
+      </c>
+    </row>
+    <row r="476">
+      <c r="A476" t="inlineStr">
+        <is>
+          <t>1i0u0oa</t>
+        </is>
+      </c>
+      <c r="B476" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Are y’all ready for cute Valentines nails </t>
+        </is>
+      </c>
+      <c r="C476" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/hqqxqbakzuce1</t>
+        </is>
+      </c>
+    </row>
+    <row r="477">
+      <c r="A477" t="inlineStr">
+        <is>
+          <t>1i0qfpy</t>
+        </is>
+      </c>
+      <c r="B477" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Elegant Winter Wedding Nails: A Gift for the Bride - constructive criticism and tips welcome! </t>
+        </is>
+      </c>
+      <c r="C477" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0qfpy</t>
+        </is>
+      </c>
+    </row>
+    <row r="478">
+      <c r="A478" t="inlineStr">
+        <is>
+          <t>1i0pfm4</t>
+        </is>
+      </c>
+      <c r="B478" t="inlineStr">
+        <is>
+          <t>Blue nails🎨🖌️</t>
+        </is>
+      </c>
+      <c r="C478" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8z85kn63ztce1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="479">
+      <c r="A479" t="inlineStr">
+        <is>
+          <t>1i0n435</t>
+        </is>
+      </c>
+      <c r="B479" t="inlineStr">
+        <is>
+          <t>Fashion and nails</t>
+        </is>
+      </c>
+      <c r="C479" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0n435</t>
+        </is>
+      </c>
+    </row>
+    <row r="480">
+      <c r="A480" t="inlineStr">
+        <is>
+          <t>1i0l1am</t>
+        </is>
+      </c>
+      <c r="B480" t="inlineStr">
+        <is>
+          <t>Pink and Black 🌸🖤</t>
+        </is>
+      </c>
+      <c r="C480" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0l1am</t>
+        </is>
+      </c>
+    </row>
+    <row r="481">
+      <c r="A481" t="inlineStr">
+        <is>
+          <t>1i0k8qk</t>
+        </is>
+      </c>
+      <c r="B481" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tried out clear nails 💅 </t>
+        </is>
+      </c>
+      <c r="C481" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0k8qk</t>
+        </is>
+      </c>
+    </row>
+    <row r="482">
+      <c r="A482" t="inlineStr">
+        <is>
+          <t>1i0iann</t>
+        </is>
+      </c>
+      <c r="B482" t="inlineStr">
+        <is>
+          <t>silver lady improving lines</t>
+        </is>
+      </c>
+      <c r="C482" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0iann</t>
+        </is>
+      </c>
+    </row>
+    <row r="483">
+      <c r="A483" t="inlineStr">
+        <is>
+          <t>1i0e9wl</t>
+        </is>
+      </c>
+      <c r="B483" t="inlineStr">
+        <is>
+          <t>Some little hand-painted mushrooms and holographic polish 🥰🍄</t>
+        </is>
+      </c>
+      <c r="C483" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0e9wl</t>
+        </is>
+      </c>
+    </row>
+    <row r="484">
+      <c r="A484" t="inlineStr">
+        <is>
+          <t>1i0cop9</t>
+        </is>
+      </c>
+      <c r="B484" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Molten metal freestyle nail set </t>
+        </is>
+      </c>
+      <c r="C484" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xosm2qi47rce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="485">
+      <c r="A485" t="inlineStr">
+        <is>
+          <t>1i0acvj</t>
+        </is>
+      </c>
+      <c r="B485" t="inlineStr">
+        <is>
+          <t>My first DIY gel nails!</t>
+        </is>
+      </c>
+      <c r="C485" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i0acvj</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Wed Jan 15 08:10:30 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_01_19.xlsx
+++ b/data/collected_data/2025_01_19.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C485"/>
+  <dimension ref="A1:C668"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8679,6 +8679,3117 @@
         </is>
       </c>
     </row>
+    <row r="486">
+      <c r="A486" t="inlineStr">
+        <is>
+          <t>1i1rq1c</t>
+        </is>
+      </c>
+      <c r="B486" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New nails </t>
+        </is>
+      </c>
+      <c r="C486" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xt6aqvqyt3de1</t>
+        </is>
+      </c>
+    </row>
+    <row r="487">
+      <c r="A487" t="inlineStr">
+        <is>
+          <t>1i1rmzy</t>
+        </is>
+      </c>
+      <c r="B487" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Something about a classic nude mani </t>
+        </is>
+      </c>
+      <c r="C487" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a7gymequs3de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="488">
+      <c r="A488" t="inlineStr">
+        <is>
+          <t>1i1r6wy</t>
+        </is>
+      </c>
+      <c r="B488" t="inlineStr">
+        <is>
+          <t>my favorite set from today 💚🤎</t>
+        </is>
+      </c>
+      <c r="C488" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vo7pwfkan3de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="489">
+      <c r="A489" t="inlineStr">
+        <is>
+          <t>1i1q2p6</t>
+        </is>
+      </c>
+      <c r="B489" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Inspired by all the frosty January blues, I had to join! </t>
+        </is>
+      </c>
+      <c r="C489" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wbvdcdxja3de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="490">
+      <c r="A490" t="inlineStr">
+        <is>
+          <t>1i1q2tv</t>
+        </is>
+      </c>
+      <c r="B490" t="inlineStr">
+        <is>
+          <t>Had to share my hand drawn Pepè Le Pew and Penelope Pussycat!</t>
+        </is>
+      </c>
+      <c r="C490" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1q2tv</t>
+        </is>
+      </c>
+    </row>
+    <row r="491">
+      <c r="A491" t="inlineStr">
+        <is>
+          <t>1i1ovl3</t>
+        </is>
+      </c>
+      <c r="B491" t="inlineStr">
+        <is>
+          <t>pom power nails</t>
+        </is>
+      </c>
+      <c r="C491" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1ovl3</t>
+        </is>
+      </c>
+    </row>
+    <row r="492">
+      <c r="A492" t="inlineStr">
+        <is>
+          <t>1i1pnjb</t>
+        </is>
+      </c>
+      <c r="B492" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Simple mani for winter </t>
+        </is>
+      </c>
+      <c r="C492" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1pnjb</t>
+        </is>
+      </c>
+    </row>
+    <row r="493">
+      <c r="A493" t="inlineStr">
+        <is>
+          <t>1i1pi8l</t>
+        </is>
+      </c>
+      <c r="B493" t="inlineStr">
+        <is>
+          <t>idea from a client, I loved the result 😍</t>
+        </is>
+      </c>
+      <c r="C493" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xrza6zsf43de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="494">
+      <c r="A494" t="inlineStr">
+        <is>
+          <t>1i1pahr</t>
+        </is>
+      </c>
+      <c r="B494" t="inlineStr">
+        <is>
+          <t>Why is it impossible to find Cutex nail polish remover in Canada?</t>
+        </is>
+      </c>
+      <c r="C494" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i1pahr/why_is_it_impossible_to_find_cutex_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="495">
+      <c r="A495" t="inlineStr">
+        <is>
+          <t>1i1p6bu</t>
+        </is>
+      </c>
+      <c r="B495" t="inlineStr">
+        <is>
+          <t>Semi cured gel nails… how do they work?!</t>
+        </is>
+      </c>
+      <c r="C495" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i1p6bu/semi_cured_gel_nails_how_do_they_work/</t>
+        </is>
+      </c>
+    </row>
+    <row r="496">
+      <c r="A496" t="inlineStr">
+        <is>
+          <t>1i1ovm5</t>
+        </is>
+      </c>
+      <c r="B496" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Valentine’s nails with cat eye 💖</t>
+        </is>
+      </c>
+      <c r="C496" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1ovm5</t>
+        </is>
+      </c>
+    </row>
+    <row r="497">
+      <c r="A497" t="inlineStr">
+        <is>
+          <t>1i1oshe</t>
+        </is>
+      </c>
+      <c r="B497" t="inlineStr">
+        <is>
+          <t>Update: first time painting my nails</t>
+        </is>
+      </c>
+      <c r="C497" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1oshe</t>
+        </is>
+      </c>
+    </row>
+    <row r="498">
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>1i1nx68</t>
+        </is>
+      </c>
+      <c r="B498" t="inlineStr">
+        <is>
+          <t xml:space="preserve">do i need a different shape? </t>
+        </is>
+      </c>
+      <c r="C498" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1nx68</t>
+        </is>
+      </c>
+    </row>
+    <row r="499">
+      <c r="A499" t="inlineStr">
+        <is>
+          <t>1i1nlbt</t>
+        </is>
+      </c>
+      <c r="B499" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How did you learn to do nails? </t>
+        </is>
+      </c>
+      <c r="C499" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i1nlbt/how_did_you_learn_to_do_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="500">
+      <c r="A500" t="inlineStr">
+        <is>
+          <t>1i1n17x</t>
+        </is>
+      </c>
+      <c r="B500" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to make doing your own nails feel like less of a chore? </t>
+        </is>
+      </c>
+      <c r="C500" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i1n17x/how_to_make_doing_your_own_nails_feel_like_less/</t>
+        </is>
+      </c>
+    </row>
+    <row r="501">
+      <c r="A501" t="inlineStr">
+        <is>
+          <t>1i1msaf</t>
+        </is>
+      </c>
+      <c r="B501" t="inlineStr">
+        <is>
+          <t>Am I crazy for spending $300 to get my nails done by a “celebrity” nail tech?</t>
+        </is>
+      </c>
+      <c r="C501" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i1msaf/am_i_crazy_for_spending_300_to_get_my_nails_done/</t>
+        </is>
+      </c>
+    </row>
+    <row r="502">
+      <c r="A502" t="inlineStr">
+        <is>
+          <t>1i1ms2a</t>
+        </is>
+      </c>
+      <c r="B502" t="inlineStr">
+        <is>
+          <t>Poorly done manicure/chrome?</t>
+        </is>
+      </c>
+      <c r="C502" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1ms2a</t>
+        </is>
+      </c>
+    </row>
+    <row r="503">
+      <c r="A503" t="inlineStr">
+        <is>
+          <t>1i1mo0c</t>
+        </is>
+      </c>
+      <c r="B503" t="inlineStr">
+        <is>
+          <t>The shine on this chrome ✨🤌🏽</t>
+        </is>
+      </c>
+      <c r="C503" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/p7af69o5d2de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="504">
+      <c r="A504" t="inlineStr">
+        <is>
+          <t>1i1mc27</t>
+        </is>
+      </c>
+      <c r="B504" t="inlineStr">
+        <is>
+          <t>One of my best sets yet</t>
+        </is>
+      </c>
+      <c r="C504" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i1mc27/one_of_my_best_sets_yet/</t>
+        </is>
+      </c>
+    </row>
+    <row r="505">
+      <c r="A505" t="inlineStr">
+        <is>
+          <t>1i1m2tv</t>
+        </is>
+      </c>
+      <c r="B505" t="inlineStr">
+        <is>
+          <t>Painting a Simpsons Valentine Set! Starting with Homer 🤩</t>
+        </is>
+      </c>
+      <c r="C505" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/maua8zet72de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="506">
+      <c r="A506" t="inlineStr">
+        <is>
+          <t>1i1lq1d</t>
+        </is>
+      </c>
+      <c r="B506" t="inlineStr">
+        <is>
+          <t>Miffy nails! But what to I call the set?</t>
+        </is>
+      </c>
+      <c r="C506" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1zv41s5p42de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="507">
+      <c r="A507" t="inlineStr">
+        <is>
+          <t>1i1lom9</t>
+        </is>
+      </c>
+      <c r="B507" t="inlineStr">
+        <is>
+          <t>Pretty 🤤</t>
+        </is>
+      </c>
+      <c r="C507" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cr54cezc42de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="508">
+      <c r="A508" t="inlineStr">
+        <is>
+          <t>1i1lnag</t>
+        </is>
+      </c>
+      <c r="B508" t="inlineStr">
+        <is>
+          <t>Chocolate 🍫 nails</t>
+        </is>
+      </c>
+      <c r="C508" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/exar2ul042de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="509">
+      <c r="A509" t="inlineStr">
+        <is>
+          <t>1i1llrf</t>
+        </is>
+      </c>
+      <c r="B509" t="inlineStr">
+        <is>
+          <t>This blue-green glitter is sooooo good</t>
+        </is>
+      </c>
+      <c r="C509" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1llrf</t>
+        </is>
+      </c>
+    </row>
+    <row r="510">
+      <c r="A510" t="inlineStr">
+        <is>
+          <t>1i1lh3r</t>
+        </is>
+      </c>
+      <c r="B510" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Valentines </t>
+        </is>
+      </c>
+      <c r="C510" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u5i8z34j22de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="511">
+      <c r="A511" t="inlineStr">
+        <is>
+          <t>1i1lg85</t>
+        </is>
+      </c>
+      <c r="B511" t="inlineStr">
+        <is>
+          <t>how to fix my c curve</t>
+        </is>
+      </c>
+      <c r="C511" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5jt6mfmb22de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="512">
+      <c r="A512" t="inlineStr">
+        <is>
+          <t>1i1l1id</t>
+        </is>
+      </c>
+      <c r="B512" t="inlineStr">
+        <is>
+          <t>i love this color sm,what y’all think?</t>
+        </is>
+      </c>
+      <c r="C512" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1l1id</t>
+        </is>
+      </c>
+    </row>
+    <row r="513">
+      <c r="A513" t="inlineStr">
+        <is>
+          <t>1i1kiun</t>
+        </is>
+      </c>
+      <c r="B513" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Obsessed with my new manicure </t>
+        </is>
+      </c>
+      <c r="C513" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1kiun</t>
+        </is>
+      </c>
+    </row>
+    <row r="514">
+      <c r="A514" t="inlineStr">
+        <is>
+          <t>1i1ju8b</t>
+        </is>
+      </c>
+      <c r="B514" t="inlineStr">
+        <is>
+          <t>This is the beauty they made for me today</t>
+        </is>
+      </c>
+      <c r="C514" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1ju8b</t>
+        </is>
+      </c>
+    </row>
+    <row r="515">
+      <c r="A515" t="inlineStr">
+        <is>
+          <t>1i1j5wf</t>
+        </is>
+      </c>
+      <c r="B515" t="inlineStr">
+        <is>
+          <t>What happened to Koala Buffer?</t>
+        </is>
+      </c>
+      <c r="C515" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i1j5wf/what_happened_to_koala_buffer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="516">
+      <c r="A516" t="inlineStr">
+        <is>
+          <t>1i1jkav</t>
+        </is>
+      </c>
+      <c r="B516" t="inlineStr">
+        <is>
+          <t>I really loved my nails today. This baby pink is everything</t>
+        </is>
+      </c>
+      <c r="C516" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2ts8zcibm1de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="517">
+      <c r="A517" t="inlineStr">
+        <is>
+          <t>1i1jf6n</t>
+        </is>
+      </c>
+      <c r="B517" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Boyfriend picked the colour and shape 🫶🏻 </t>
+        </is>
+      </c>
+      <c r="C517" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1jf6n</t>
+        </is>
+      </c>
+    </row>
+    <row r="518">
+      <c r="A518" t="inlineStr">
+        <is>
+          <t>1i1isyf</t>
+        </is>
+      </c>
+      <c r="B518" t="inlineStr">
+        <is>
+          <t>Does anybody know what cat eye polish this is? The exact color? LINK? THANKS SO MUCH 🩷</t>
+        </is>
+      </c>
+      <c r="C518" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1isyf</t>
+        </is>
+      </c>
+    </row>
+    <row r="519">
+      <c r="A519" t="inlineStr">
+        <is>
+          <t>1i1icx6</t>
+        </is>
+      </c>
+      <c r="B519" t="inlineStr">
+        <is>
+          <t>NYC Cheap Nails</t>
+        </is>
+      </c>
+      <c r="C519" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i1icx6/nyc_cheap_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="520">
+      <c r="A520" t="inlineStr">
+        <is>
+          <t>1i1hv0z</t>
+        </is>
+      </c>
+      <c r="B520" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nails </t>
+        </is>
+      </c>
+      <c r="C520" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/88s5qals81de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="521">
+      <c r="A521" t="inlineStr">
+        <is>
+          <t>1i1hnda</t>
+        </is>
+      </c>
+      <c r="B521" t="inlineStr">
+        <is>
+          <t>How do we feel about natural nails &amp; home manicures?</t>
+        </is>
+      </c>
+      <c r="C521" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ql2dil1871de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="522">
+      <c r="A522" t="inlineStr">
+        <is>
+          <t>1i1hga2</t>
+        </is>
+      </c>
+      <c r="B522" t="inlineStr">
+        <is>
+          <t>I’ve been so into the transparent look I finally gave it a go with some press ons :)</t>
+        </is>
+      </c>
+      <c r="C522" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fj51ffwp51de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="523">
+      <c r="A523" t="inlineStr">
+        <is>
+          <t>1i1gk9r</t>
+        </is>
+      </c>
+      <c r="B523" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Feeling like Barbie </t>
+        </is>
+      </c>
+      <c r="C523" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r3t304qxy0de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="524">
+      <c r="A524" t="inlineStr">
+        <is>
+          <t>1i1gjaf</t>
+        </is>
+      </c>
+      <c r="B524" t="inlineStr">
+        <is>
+          <t>Fire Emblem Fates Lady Corrin as Stained Glass Painting Nail Art!</t>
+        </is>
+      </c>
+      <c r="C524" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1gjaf</t>
+        </is>
+      </c>
+    </row>
+    <row r="525">
+      <c r="A525" t="inlineStr">
+        <is>
+          <t>1i1g4do</t>
+        </is>
+      </c>
+      <c r="B525" t="inlineStr">
+        <is>
+          <t>First ever press on set completed!</t>
+        </is>
+      </c>
+      <c r="C525" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1g4do</t>
+        </is>
+      </c>
+    </row>
+    <row r="526">
+      <c r="A526" t="inlineStr">
+        <is>
+          <t>1i1g281</t>
+        </is>
+      </c>
+      <c r="B526" t="inlineStr">
+        <is>
+          <t>Valentine’s Day set 💕</t>
+        </is>
+      </c>
+      <c r="C526" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i13xpnhuu0de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="527">
+      <c r="A527" t="inlineStr">
+        <is>
+          <t>1i1frm8</t>
+        </is>
+      </c>
+      <c r="B527" t="inlineStr">
+        <is>
+          <t>First time using holographic powder 😍</t>
+        </is>
+      </c>
+      <c r="C527" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1frm8</t>
+        </is>
+      </c>
+    </row>
+    <row r="528">
+      <c r="A528" t="inlineStr">
+        <is>
+          <t>1i1ez4w</t>
+        </is>
+      </c>
+      <c r="B528" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Couldn’t wait, starting the valentines themed nails early 😄♥️ </t>
+        </is>
+      </c>
+      <c r="C528" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9ccpx029m0de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="529">
+      <c r="A529" t="inlineStr">
+        <is>
+          <t>1i1ex7f</t>
+        </is>
+      </c>
+      <c r="B529" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Presson nails by me 🥰 </t>
+        </is>
+      </c>
+      <c r="C529" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1ex7f</t>
+        </is>
+      </c>
+    </row>
+    <row r="530">
+      <c r="A530" t="inlineStr">
+        <is>
+          <t>1i1evx0</t>
+        </is>
+      </c>
+      <c r="B530" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Natural nails after acrylics </t>
+        </is>
+      </c>
+      <c r="C530" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i1evx0/natural_nails_after_acrylics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="531">
+      <c r="A531" t="inlineStr">
+        <is>
+          <t>1i1evh1</t>
+        </is>
+      </c>
+      <c r="B531" t="inlineStr">
+        <is>
+          <t>💖⭐️</t>
+        </is>
+      </c>
+      <c r="C531" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kc0km1ghl0de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="532">
+      <c r="A532" t="inlineStr">
+        <is>
+          <t>1i1erih</t>
+        </is>
+      </c>
+      <c r="B532" t="inlineStr">
+        <is>
+          <t>Wanted to share my first attempts at fake nails!</t>
+        </is>
+      </c>
+      <c r="C532" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1erih</t>
+        </is>
+      </c>
+    </row>
+    <row r="533">
+      <c r="A533" t="inlineStr">
+        <is>
+          <t>1i1epfh</t>
+        </is>
+      </c>
+      <c r="B533" t="inlineStr">
+        <is>
+          <t xml:space="preserve">IN LOVE </t>
+        </is>
+      </c>
+      <c r="C533" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w1j0ov58k0de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="534">
+      <c r="A534" t="inlineStr">
+        <is>
+          <t>1i1eo01</t>
+        </is>
+      </c>
+      <c r="B534" t="inlineStr">
+        <is>
+          <t>Emo Bows 🖤🖤</t>
+        </is>
+      </c>
+      <c r="C534" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/etloqpcyj0de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="535">
+      <c r="A535" t="inlineStr">
+        <is>
+          <t>1i1en0e</t>
+        </is>
+      </c>
+      <c r="B535" t="inlineStr">
+        <is>
+          <t>Started Doing My Own Nails</t>
+        </is>
+      </c>
+      <c r="C535" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/samfhxuqj0de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="536">
+      <c r="A536" t="inlineStr">
+        <is>
+          <t>1i1ejql</t>
+        </is>
+      </c>
+      <c r="B536" t="inlineStr">
+        <is>
+          <t>To add gems/pearls or leave them alone? 🥲 also advice needed</t>
+        </is>
+      </c>
+      <c r="C536" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1ejql</t>
+        </is>
+      </c>
+    </row>
+    <row r="537">
+      <c r="A537" t="inlineStr">
+        <is>
+          <t>1i1dwwk</t>
+        </is>
+      </c>
+      <c r="B537" t="inlineStr">
+        <is>
+          <t>My dark gothic nails 🖤</t>
+        </is>
+      </c>
+      <c r="C537" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1dwwk</t>
+        </is>
+      </c>
+    </row>
+    <row r="538">
+      <c r="A538" t="inlineStr">
+        <is>
+          <t>1i1eetc</t>
+        </is>
+      </c>
+      <c r="B538" t="inlineStr">
+        <is>
+          <t>What shape suits my short fingers/squarish nails?</t>
+        </is>
+      </c>
+      <c r="C538" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ra4bvhg1i0de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="539">
+      <c r="A539" t="inlineStr">
+        <is>
+          <t>1i1ea7f</t>
+        </is>
+      </c>
+      <c r="B539" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Please help me appreciate that these press ons are going strong even after 10 days. </t>
+        </is>
+      </c>
+      <c r="C539" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ml1tvuu2h0de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="540">
+      <c r="A540" t="inlineStr">
+        <is>
+          <t>1i1e74h</t>
+        </is>
+      </c>
+      <c r="B540" t="inlineStr">
+        <is>
+          <t>january nails done</t>
+        </is>
+      </c>
+      <c r="C540" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qem415ywf0de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="541">
+      <c r="A541" t="inlineStr">
+        <is>
+          <t>1i1e1im</t>
+        </is>
+      </c>
+      <c r="B541" t="inlineStr">
+        <is>
+          <t>Ice Princess mani 🌬️❄️</t>
+        </is>
+      </c>
+      <c r="C541" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ccjmcwbaf0de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="542">
+      <c r="A542" t="inlineStr">
+        <is>
+          <t>1i1dlpq</t>
+        </is>
+      </c>
+      <c r="B542" t="inlineStr">
+        <is>
+          <t>Denim blue with chrome</t>
+        </is>
+      </c>
+      <c r="C542" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qu91pqz1c0de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="543">
+      <c r="A543" t="inlineStr">
+        <is>
+          <t>1i1cuzk</t>
+        </is>
+      </c>
+      <c r="B543" t="inlineStr">
+        <is>
+          <t>Recently engaged and wanted this inspo look (@nailsbyzola) vs my attempt - how do I emulate this look?</t>
+        </is>
+      </c>
+      <c r="C543" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1cuzk</t>
+        </is>
+      </c>
+    </row>
+    <row r="544">
+      <c r="A544" t="inlineStr">
+        <is>
+          <t>1i1d2c4</t>
+        </is>
+      </c>
+      <c r="B544" t="inlineStr">
+        <is>
+          <t>clowns</t>
+        </is>
+      </c>
+      <c r="C544" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3o26xes280de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="545">
+      <c r="A545" t="inlineStr">
+        <is>
+          <t>1i1cv5r</t>
+        </is>
+      </c>
+      <c r="B545" t="inlineStr">
+        <is>
+          <t>need some advice please!!</t>
+        </is>
+      </c>
+      <c r="C545" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1cv5r</t>
+        </is>
+      </c>
+    </row>
+    <row r="546">
+      <c r="A546" t="inlineStr">
+        <is>
+          <t>1i1cghl</t>
+        </is>
+      </c>
+      <c r="B546" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Arcane's Jinx design! | I decided to post here since I saw several men sharing their nails </t>
+        </is>
+      </c>
+      <c r="C546" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1cghl</t>
+        </is>
+      </c>
+    </row>
+    <row r="547">
+      <c r="A547" t="inlineStr">
+        <is>
+          <t>1i1cfr1</t>
+        </is>
+      </c>
+      <c r="B547" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The worst dip nails of my life </t>
+        </is>
+      </c>
+      <c r="C547" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1cfr1</t>
+        </is>
+      </c>
+    </row>
+    <row r="548">
+      <c r="A548" t="inlineStr">
+        <is>
+          <t>1i1c9lm</t>
+        </is>
+      </c>
+      <c r="B548" t="inlineStr">
+        <is>
+          <t>Cuticle cutter</t>
+        </is>
+      </c>
+      <c r="C548" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i1c9lm/cuticle_cutter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="549">
+      <c r="A549" t="inlineStr">
+        <is>
+          <t>1i1bvaw</t>
+        </is>
+      </c>
+      <c r="B549" t="inlineStr">
+        <is>
+          <t xml:space="preserve">early valentine's nails </t>
+        </is>
+      </c>
+      <c r="C549" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/obtzten0zzce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="550">
+      <c r="A550" t="inlineStr">
+        <is>
+          <t>1i1ba1v</t>
+        </is>
+      </c>
+      <c r="B550" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Why did the air pocket appear later on? </t>
+        </is>
+      </c>
+      <c r="C550" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1dw0n3ajuzce1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="551">
+      <c r="A551" t="inlineStr">
+        <is>
+          <t>1i1b39g</t>
+        </is>
+      </c>
+      <c r="B551" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sweater weather! </t>
+        </is>
+      </c>
+      <c r="C551" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/koa7igf4tzce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="552">
+      <c r="A552" t="inlineStr">
+        <is>
+          <t>1i1abot</t>
+        </is>
+      </c>
+      <c r="B552" t="inlineStr">
+        <is>
+          <t>Holographic moment 🩷</t>
+        </is>
+      </c>
+      <c r="C552" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1abot</t>
+        </is>
+      </c>
+    </row>
+    <row r="553">
+      <c r="A553" t="inlineStr">
+        <is>
+          <t>1i1a8i3</t>
+        </is>
+      </c>
+      <c r="B553" t="inlineStr">
+        <is>
+          <t>So many loved my nails…</t>
+        </is>
+      </c>
+      <c r="C553" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1a8i3</t>
+        </is>
+      </c>
+    </row>
+    <row r="554">
+      <c r="A554" t="inlineStr">
+        <is>
+          <t>1i10n73</t>
+        </is>
+      </c>
+      <c r="B554" t="inlineStr">
+        <is>
+          <t>Do i try and patch this lil guy up or am i better off cutting it and letting it grow?</t>
+        </is>
+      </c>
+      <c r="C554" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nzpew0jfuwce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="555">
+      <c r="A555" t="inlineStr">
+        <is>
+          <t>1i13e1l</t>
+        </is>
+      </c>
+      <c r="B555" t="inlineStr">
+        <is>
+          <t>HELP! 1st time getting acrylics done gone bad!</t>
+        </is>
+      </c>
+      <c r="C555" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i13e1l</t>
+        </is>
+      </c>
+    </row>
+    <row r="556">
+      <c r="A556" t="inlineStr">
+        <is>
+          <t>1i13m3g</t>
+        </is>
+      </c>
+      <c r="B556" t="inlineStr">
+        <is>
+          <t>Beginner to the nail game, I need advice</t>
+        </is>
+      </c>
+      <c r="C556" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i13m3g/beginner_to_the_nail_game_i_need_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="557">
+      <c r="A557" t="inlineStr">
+        <is>
+          <t>1i165wx</t>
+        </is>
+      </c>
+      <c r="B557" t="inlineStr">
+        <is>
+          <t>Gel removal results</t>
+        </is>
+      </c>
+      <c r="C557" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1uv8znjjpyce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="558">
+      <c r="A558" t="inlineStr">
+        <is>
+          <t>1i19kl2</t>
+        </is>
+      </c>
+      <c r="B558" t="inlineStr">
+        <is>
+          <t>first time getting acrylics</t>
+        </is>
+      </c>
+      <c r="C558" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gn48ubvthzce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="559">
+      <c r="A559" t="inlineStr">
+        <is>
+          <t>1i19d4l</t>
+        </is>
+      </c>
+      <c r="B559" t="inlineStr">
+        <is>
+          <t>First time getting nails done!</t>
+        </is>
+      </c>
+      <c r="C559" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i19d4l</t>
+        </is>
+      </c>
+    </row>
+    <row r="560">
+      <c r="A560" t="inlineStr">
+        <is>
+          <t>1i19coe</t>
+        </is>
+      </c>
+      <c r="B560" t="inlineStr">
+        <is>
+          <t>Which brand full tips?</t>
+        </is>
+      </c>
+      <c r="C560" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qzpdmo63gzce1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="561">
+      <c r="A561" t="inlineStr">
+        <is>
+          <t>1i196jb</t>
+        </is>
+      </c>
+      <c r="B561" t="inlineStr">
+        <is>
+          <t>❄️💖👸🏻</t>
+        </is>
+      </c>
+      <c r="C561" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i196jb</t>
+        </is>
+      </c>
+    </row>
+    <row r="562">
+      <c r="A562" t="inlineStr">
+        <is>
+          <t>1i18f14</t>
+        </is>
+      </c>
+      <c r="B562" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Abstract squiggles </t>
+        </is>
+      </c>
+      <c r="C562" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0l0s58cq8zce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="563">
+      <c r="A563" t="inlineStr">
+        <is>
+          <t>1i189ts</t>
+        </is>
+      </c>
+      <c r="B563" t="inlineStr">
+        <is>
+          <t>Nude and Rosegold gliter .. perfect 🤩✨</t>
+        </is>
+      </c>
+      <c r="C563" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1vgma0h47zce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="564">
+      <c r="A564" t="inlineStr">
+        <is>
+          <t>1i186dh</t>
+        </is>
+      </c>
+      <c r="B564" t="inlineStr">
+        <is>
+          <t>how much would you pay for these?</t>
+        </is>
+      </c>
+      <c r="C564" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dacmyu2s6zce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="565">
+      <c r="A565" t="inlineStr">
+        <is>
+          <t>1i16cms</t>
+        </is>
+      </c>
+      <c r="B565" t="inlineStr">
+        <is>
+          <t>Simple Bday Nails</t>
+        </is>
+      </c>
+      <c r="C565" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ei6hi038ryce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="566">
+      <c r="A566" t="inlineStr">
+        <is>
+          <t>1i163ra</t>
+        </is>
+      </c>
+      <c r="B566" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DND Seascapes </t>
+        </is>
+      </c>
+      <c r="C566" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i163ra</t>
+        </is>
+      </c>
+    </row>
+    <row r="567">
+      <c r="A567" t="inlineStr">
+        <is>
+          <t>1i162f0</t>
+        </is>
+      </c>
+      <c r="B567" t="inlineStr">
+        <is>
+          <t>Hand-painted on press ons</t>
+        </is>
+      </c>
+      <c r="C567" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i162f0</t>
+        </is>
+      </c>
+    </row>
+    <row r="568">
+      <c r="A568" t="inlineStr">
+        <is>
+          <t>1i15oen</t>
+        </is>
+      </c>
+      <c r="B568" t="inlineStr">
+        <is>
+          <t>Cuticle care</t>
+        </is>
+      </c>
+      <c r="C568" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i15oen/cuticle_care/</t>
+        </is>
+      </c>
+    </row>
+    <row r="569">
+      <c r="A569" t="inlineStr">
+        <is>
+          <t>1i142op</t>
+        </is>
+      </c>
+      <c r="B569" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thoughts on the nails? </t>
+        </is>
+      </c>
+      <c r="C569" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/688effwk3yce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="570">
+      <c r="A570" t="inlineStr">
+        <is>
+          <t>1i13r1a</t>
+        </is>
+      </c>
+      <c r="B570" t="inlineStr">
+        <is>
+          <t>Where to find wide nails to make press-ons?</t>
+        </is>
+      </c>
+      <c r="C570" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i13r1a/where_to_find_wide_nails_to_make_pressons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="571">
+      <c r="A571" t="inlineStr">
+        <is>
+          <t>1i1rj97</t>
+        </is>
+      </c>
+      <c r="B571" t="inlineStr">
+        <is>
+          <t>Anyone heard of Color Swap?</t>
+        </is>
+      </c>
+      <c r="C571" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sarttbrhr3de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="572">
+      <c r="A572" t="inlineStr">
+        <is>
+          <t>1i1qtae</t>
+        </is>
+      </c>
+      <c r="B572" t="inlineStr">
+        <is>
+          <t>Recos for Regular Polish Artists</t>
+        </is>
+      </c>
+      <c r="C572" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i1qtae/recos_for_regular_polish_artists/</t>
+        </is>
+      </c>
+    </row>
+    <row r="573">
+      <c r="A573" t="inlineStr">
+        <is>
+          <t>1i1q50i</t>
+        </is>
+      </c>
+      <c r="B573" t="inlineStr">
+        <is>
+          <t>Clear Jelly Stamper Gel-ly Wraps</t>
+        </is>
+      </c>
+      <c r="C573" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i1q50i/clear_jelly_stamper_gelly_wraps/</t>
+        </is>
+      </c>
+    </row>
+    <row r="574">
+      <c r="A574" t="inlineStr">
+        <is>
+          <t>1i1pt37</t>
+        </is>
+      </c>
+      <c r="B574" t="inlineStr">
+        <is>
+          <t>Water based top coat??</t>
+        </is>
+      </c>
+      <c r="C574" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i1pt37/water_based_top_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="575">
+      <c r="A575" t="inlineStr">
+        <is>
+          <t>1i1poup</t>
+        </is>
+      </c>
+      <c r="B575" t="inlineStr">
+        <is>
+          <t>Trim all the nails or is it not really noticeable?</t>
+        </is>
+      </c>
+      <c r="C575" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1poup</t>
+        </is>
+      </c>
+    </row>
+    <row r="576">
+      <c r="A576" t="inlineStr">
+        <is>
+          <t>1i1ooq7</t>
+        </is>
+      </c>
+      <c r="B576" t="inlineStr">
+        <is>
+          <t>Dragon On and On but make it matte</t>
+        </is>
+      </c>
+      <c r="C576" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1ooq7</t>
+        </is>
+      </c>
+    </row>
+    <row r="577">
+      <c r="A577" t="inlineStr">
+        <is>
+          <t>1i1onyv</t>
+        </is>
+      </c>
+      <c r="B577" t="inlineStr">
+        <is>
+          <t>Has anyone gotten good results from these “patterned” magnets (from Amazon or elsewhere)? Any recommendations?</t>
+        </is>
+      </c>
+      <c r="C577" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j0j0ca80w2de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="578">
+      <c r="A578" t="inlineStr">
+        <is>
+          <t>1i1o8t9</t>
+        </is>
+      </c>
+      <c r="B578" t="inlineStr">
+        <is>
+          <t>Has anyone tried this magnetic nail technique?</t>
+        </is>
+      </c>
+      <c r="C578" t="inlineStr">
+        <is>
+          <t>https://www.instagram.com/reel/DEZ9cBnutd7/?igsh=MTlzenUxdW9tc2k5bg==</t>
+        </is>
+      </c>
+    </row>
+    <row r="579">
+      <c r="A579" t="inlineStr">
+        <is>
+          <t>1i1o2pl</t>
+        </is>
+      </c>
+      <c r="B579" t="inlineStr">
+        <is>
+          <t>Midnight Rider</t>
+        </is>
+      </c>
+      <c r="C579" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1o2pl</t>
+        </is>
+      </c>
+    </row>
+    <row r="580">
+      <c r="A580" t="inlineStr">
+        <is>
+          <t>1i1nsxg</t>
+        </is>
+      </c>
+      <c r="B580" t="inlineStr">
+        <is>
+          <t>My boyfriend let me paint his nails 🥰</t>
+        </is>
+      </c>
+      <c r="C580" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dwg7pldqn2de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="581">
+      <c r="A581" t="inlineStr">
+        <is>
+          <t>1i1nqrl</t>
+        </is>
+      </c>
+      <c r="B581" t="inlineStr">
+        <is>
+          <t>Skittle mani after the big chop :,)</t>
+        </is>
+      </c>
+      <c r="C581" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1nqrl</t>
+        </is>
+      </c>
+    </row>
+    <row r="582">
+      <c r="A582" t="inlineStr">
+        <is>
+          <t>1i1nqhf</t>
+        </is>
+      </c>
+      <c r="B582" t="inlineStr">
+        <is>
+          <t>Matched my drink to my nails</t>
+        </is>
+      </c>
+      <c r="C582" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1nqhf</t>
+        </is>
+      </c>
+    </row>
+    <row r="583">
+      <c r="A583" t="inlineStr">
+        <is>
+          <t>1i1nmpq</t>
+        </is>
+      </c>
+      <c r="B583" t="inlineStr">
+        <is>
+          <t>Let's have some fun 🌈</t>
+        </is>
+      </c>
+      <c r="C583" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i1nmpq/lets_have_some_fun/</t>
+        </is>
+      </c>
+    </row>
+    <row r="584">
+      <c r="A584" t="inlineStr">
+        <is>
+          <t>1i1nehh</t>
+        </is>
+      </c>
+      <c r="B584" t="inlineStr">
+        <is>
+          <t>Orly Orange Punch 🔥🦀🥵</t>
+        </is>
+      </c>
+      <c r="C584" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t4cnbsyxj2de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="585">
+      <c r="A585" t="inlineStr">
+        <is>
+          <t>1i1n6lp</t>
+        </is>
+      </c>
+      <c r="B585" t="inlineStr">
+        <is>
+          <t>The Magician v1.5 🪄💫</t>
+        </is>
+      </c>
+      <c r="C585" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/unhtmxzuh2de1</t>
+        </is>
+      </c>
+    </row>
+    <row r="586">
+      <c r="A586" t="inlineStr">
+        <is>
+          <t>1i1n2nt</t>
+        </is>
+      </c>
+      <c r="B586" t="inlineStr">
+        <is>
+          <t>Almond or square?</t>
+        </is>
+      </c>
+      <c r="C586" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1n2nt</t>
+        </is>
+      </c>
+    </row>
+    <row r="587">
+      <c r="A587" t="inlineStr">
+        <is>
+          <t>1i1mqiq</t>
+        </is>
+      </c>
+      <c r="B587" t="inlineStr">
+        <is>
+          <t>Moonfairy formula?</t>
+        </is>
+      </c>
+      <c r="C587" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i1mqiq/moonfairy_formula/</t>
+        </is>
+      </c>
+    </row>
+    <row r="588">
+      <c r="A588" t="inlineStr">
+        <is>
+          <t>1i1mi38</t>
+        </is>
+      </c>
+      <c r="B588" t="inlineStr">
+        <is>
+          <t>Bliss 💜💙💜💙💜💙</t>
+        </is>
+      </c>
+      <c r="C588" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4zaatb6mb2de1</t>
+        </is>
+      </c>
+    </row>
+    <row r="589">
+      <c r="A589" t="inlineStr">
+        <is>
+          <t>1i1ma0p</t>
+        </is>
+      </c>
+      <c r="B589" t="inlineStr">
+        <is>
+          <t>Fashion Polly</t>
+        </is>
+      </c>
+      <c r="C589" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1ma0p</t>
+        </is>
+      </c>
+    </row>
+    <row r="590">
+      <c r="A590" t="inlineStr">
+        <is>
+          <t>1i1lydr</t>
+        </is>
+      </c>
+      <c r="B590" t="inlineStr">
+        <is>
+          <t>Interview nails vs what I wore yesterday…</t>
+        </is>
+      </c>
+      <c r="C590" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1lydr</t>
+        </is>
+      </c>
+    </row>
+    <row r="591">
+      <c r="A591" t="inlineStr">
+        <is>
+          <t>1i1kzd6</t>
+        </is>
+      </c>
+      <c r="B591" t="inlineStr">
+        <is>
+          <t>ORLY offering to help restock LA salons &amp; techs</t>
+        </is>
+      </c>
+      <c r="C591" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1kzd6</t>
+        </is>
+      </c>
+    </row>
+    <row r="592">
+      <c r="A592" t="inlineStr">
+        <is>
+          <t>1i1kpfe</t>
+        </is>
+      </c>
+      <c r="B592" t="inlineStr">
+        <is>
+          <t>wug nails! (idk if anyone will get the reference but)</t>
+        </is>
+      </c>
+      <c r="C592" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/goo9iawvv1de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="593">
+      <c r="A593" t="inlineStr">
+        <is>
+          <t>1i1kon6</t>
+        </is>
+      </c>
+      <c r="B593" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tried my hand at some leopard nail art for the first time :) </t>
+        </is>
+      </c>
+      <c r="C593" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1nsxoyapv1de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="594">
+      <c r="A594" t="inlineStr">
+        <is>
+          <t>1i1kci8</t>
+        </is>
+      </c>
+      <c r="B594" t="inlineStr">
+        <is>
+          <t>I found better lighting 😆</t>
+        </is>
+      </c>
+      <c r="C594" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xuy2aapxs1de1</t>
+        </is>
+      </c>
+    </row>
+    <row r="595">
+      <c r="A595" t="inlineStr">
+        <is>
+          <t>1i1k7ap</t>
+        </is>
+      </c>
+      <c r="B595" t="inlineStr">
+        <is>
+          <t>Imperial Stormtrooper pre and post cleanup</t>
+        </is>
+      </c>
+      <c r="C595" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1k7ap</t>
+        </is>
+      </c>
+    </row>
+    <row r="596">
+      <c r="A596" t="inlineStr">
+        <is>
+          <t>1i1jsx1</t>
+        </is>
+      </c>
+      <c r="B596" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Doing a base coat experiment </t>
+        </is>
+      </c>
+      <c r="C596" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/91g9kkaao1de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="597">
+      <c r="A597" t="inlineStr">
+        <is>
+          <t>1i1jsfr</t>
+        </is>
+      </c>
+      <c r="B597" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Northern Lights 🧲 </t>
+        </is>
+      </c>
+      <c r="C597" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/xnya8vh0o1de1</t>
+        </is>
+      </c>
+    </row>
+    <row r="598">
+      <c r="A598" t="inlineStr">
+        <is>
+          <t>1i1j8ns</t>
+        </is>
+      </c>
+      <c r="B598" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Favorite warm greys???? </t>
+        </is>
+      </c>
+      <c r="C598" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i1j8ns/favorite_warm_greys/</t>
+        </is>
+      </c>
+    </row>
+    <row r="599">
+      <c r="A599" t="inlineStr">
+        <is>
+          <t>1i1j1b0</t>
+        </is>
+      </c>
+      <c r="B599" t="inlineStr">
+        <is>
+          <t>This Is a Storm Warning 😎⛈️</t>
+        </is>
+      </c>
+      <c r="C599" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/n6ayq8hwh1de1</t>
+        </is>
+      </c>
+    </row>
+    <row r="600">
+      <c r="A600" t="inlineStr">
+        <is>
+          <t>1i1htjy</t>
+        </is>
+      </c>
+      <c r="B600" t="inlineStr">
+        <is>
+          <t>blues and greens ✨✨</t>
+        </is>
+      </c>
+      <c r="C600" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1htjy</t>
+        </is>
+      </c>
+    </row>
+    <row r="601">
+      <c r="A601" t="inlineStr">
+        <is>
+          <t>1i1hnm0</t>
+        </is>
+      </c>
+      <c r="B601" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Purple on purple </t>
+        </is>
+      </c>
+      <c r="C601" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1hnm0</t>
+        </is>
+      </c>
+    </row>
+    <row r="602">
+      <c r="A602" t="inlineStr">
+        <is>
+          <t>1i1hkij</t>
+        </is>
+      </c>
+      <c r="B602" t="inlineStr">
+        <is>
+          <t>is this lamp okay?</t>
+        </is>
+      </c>
+      <c r="C602" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i1hkij/is_this_lamp_okay/</t>
+        </is>
+      </c>
+    </row>
+    <row r="603">
+      <c r="A603" t="inlineStr">
+        <is>
+          <t>1i1ha9b</t>
+        </is>
+      </c>
+      <c r="B603" t="inlineStr">
+        <is>
+          <t>When will hhc make September overstock available?</t>
+        </is>
+      </c>
+      <c r="C603" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i1ha9b/when_will_hhc_make_september_overstock_available/</t>
+        </is>
+      </c>
+    </row>
+    <row r="604">
+      <c r="A604" t="inlineStr">
+        <is>
+          <t>1i1h0ag</t>
+        </is>
+      </c>
+      <c r="B604" t="inlineStr">
+        <is>
+          <t>I feel so…exposed now 😢</t>
+        </is>
+      </c>
+      <c r="C604" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1h0ag</t>
+        </is>
+      </c>
+    </row>
+    <row r="605">
+      <c r="A605" t="inlineStr">
+        <is>
+          <t>1i1grpu</t>
+        </is>
+      </c>
+      <c r="B605" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cant stop staring at my own hands </t>
+        </is>
+      </c>
+      <c r="C605" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1grpu</t>
+        </is>
+      </c>
+    </row>
+    <row r="606">
+      <c r="A606" t="inlineStr">
+        <is>
+          <t>1i1gmar</t>
+        </is>
+      </c>
+      <c r="B606" t="inlineStr">
+        <is>
+          <t>ILNP Swatch Comparisons?</t>
+        </is>
+      </c>
+      <c r="C606" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i1gmar/ilnp_swatch_comparisons/</t>
+        </is>
+      </c>
+    </row>
+    <row r="607">
+      <c r="A607" t="inlineStr">
+        <is>
+          <t>1i1fzih</t>
+        </is>
+      </c>
+      <c r="B607" t="inlineStr">
+        <is>
+          <t>Drugstore Shorties 🖤</t>
+        </is>
+      </c>
+      <c r="C607" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1fzih</t>
+        </is>
+      </c>
+    </row>
+    <row r="608">
+      <c r="A608" t="inlineStr">
+        <is>
+          <t>1i1fxj9</t>
+        </is>
+      </c>
+      <c r="B608" t="inlineStr">
+        <is>
+          <t>devil’s advocate ✨</t>
+        </is>
+      </c>
+      <c r="C608" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1fxj9</t>
+        </is>
+      </c>
+    </row>
+    <row r="609">
+      <c r="A609" t="inlineStr">
+        <is>
+          <t>1i1frvt</t>
+        </is>
+      </c>
+      <c r="B609" t="inlineStr">
+        <is>
+          <t xml:space="preserve">*sigh* missed out on Goblins and Ghoulies.. Is Phoenix Indie duping it sorta kinda?! </t>
+        </is>
+      </c>
+      <c r="C609" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i1frvt/sigh_missed_out_on_goblins_and_ghoulies_is/</t>
+        </is>
+      </c>
+    </row>
+    <row r="610">
+      <c r="A610" t="inlineStr">
+        <is>
+          <t>1i1fh28</t>
+        </is>
+      </c>
+      <c r="B610" t="inlineStr">
+        <is>
+          <t>My toxic relationship ship with cremes continue…</t>
+        </is>
+      </c>
+      <c r="C610" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s5e35qgvp0de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="611">
+      <c r="A611" t="inlineStr">
+        <is>
+          <t>1i1fg9i</t>
+        </is>
+      </c>
+      <c r="B611" t="inlineStr">
+        <is>
+          <t>Name a more iconic duo</t>
+        </is>
+      </c>
+      <c r="C611" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1fg9i</t>
+        </is>
+      </c>
+    </row>
+    <row r="612">
+      <c r="A612" t="inlineStr">
+        <is>
+          <t>1i1f5yf</t>
+        </is>
+      </c>
+      <c r="B612" t="inlineStr">
+        <is>
+          <t>What causes this in gel nails?</t>
+        </is>
+      </c>
+      <c r="C612" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1f5yf</t>
+        </is>
+      </c>
+    </row>
+    <row r="613">
+      <c r="A613" t="inlineStr">
+        <is>
+          <t>1i1epqa</t>
+        </is>
+      </c>
+      <c r="B613" t="inlineStr">
+        <is>
+          <t>Defy &amp; Inspire Brand</t>
+        </is>
+      </c>
+      <c r="C613" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i1epqa/defy_inspire_brand/</t>
+        </is>
+      </c>
+    </row>
+    <row r="614">
+      <c r="A614" t="inlineStr">
+        <is>
+          <t>1i1em80</t>
+        </is>
+      </c>
+      <c r="B614" t="inlineStr">
+        <is>
+          <t>wow</t>
+        </is>
+      </c>
+      <c r="C614" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1em80</t>
+        </is>
+      </c>
+    </row>
+    <row r="615">
+      <c r="A615" t="inlineStr">
+        <is>
+          <t>1i1e7bg</t>
+        </is>
+      </c>
+      <c r="B615" t="inlineStr">
+        <is>
+          <t>The girlies were right</t>
+        </is>
+      </c>
+      <c r="C615" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1e7bg</t>
+        </is>
+      </c>
+    </row>
+    <row r="616">
+      <c r="A616" t="inlineStr">
+        <is>
+          <t>1i1e1u7</t>
+        </is>
+      </c>
+      <c r="B616" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cirque is having a 50% sale on their website </t>
+        </is>
+      </c>
+      <c r="C616" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i1e1u7/cirque_is_having_a_50_sale_on_their_website/</t>
+        </is>
+      </c>
+    </row>
+    <row r="617">
+      <c r="A617" t="inlineStr">
+        <is>
+          <t>1i1e1at</t>
+        </is>
+      </c>
+      <c r="B617" t="inlineStr">
+        <is>
+          <t>pink shimmers similar to Trinket?</t>
+        </is>
+      </c>
+      <c r="C617" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eqnk75q8f0de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="618">
+      <c r="A618" t="inlineStr">
+        <is>
+          <t>1i1e11y</t>
+        </is>
+      </c>
+      <c r="B618" t="inlineStr">
+        <is>
+          <t>Goddess of rot 😌</t>
+        </is>
+      </c>
+      <c r="C618" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1e11y</t>
+        </is>
+      </c>
+    </row>
+    <row r="619">
+      <c r="A619" t="inlineStr">
+        <is>
+          <t>1i1dxo6</t>
+        </is>
+      </c>
+      <c r="B619" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Momento Mori has my heart ♥️ </t>
+        </is>
+      </c>
+      <c r="C619" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/csfesoxge0de1</t>
+        </is>
+      </c>
+    </row>
+    <row r="620">
+      <c r="A620" t="inlineStr">
+        <is>
+          <t>1i1dc8f</t>
+        </is>
+      </c>
+      <c r="B620" t="inlineStr">
+        <is>
+          <t>Topping of Quick Dry Top Coat Question</t>
+        </is>
+      </c>
+      <c r="C620" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i1dc8f/topping_of_quick_dry_top_coat_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="621">
+      <c r="A621" t="inlineStr">
+        <is>
+          <t>1i1d46w</t>
+        </is>
+      </c>
+      <c r="B621" t="inlineStr">
+        <is>
+          <t>What happened here? But kinda cool?</t>
+        </is>
+      </c>
+      <c r="C621" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1d46w</t>
+        </is>
+      </c>
+    </row>
+    <row r="622">
+      <c r="A622" t="inlineStr">
+        <is>
+          <t>1i1d0hm</t>
+        </is>
+      </c>
+      <c r="B622" t="inlineStr">
+        <is>
+          <t>A bit dented, but still shifty!</t>
+        </is>
+      </c>
+      <c r="C622" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1d0hm</t>
+        </is>
+      </c>
+    </row>
+    <row r="623">
+      <c r="A623" t="inlineStr">
+        <is>
+          <t>1i1cq3f</t>
+        </is>
+      </c>
+      <c r="B623" t="inlineStr">
+        <is>
+          <t>Dupe for Mooncat Moonspell?</t>
+        </is>
+      </c>
+      <c r="C623" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1cq3f</t>
+        </is>
+      </c>
+    </row>
+    <row r="624">
+      <c r="A624" t="inlineStr">
+        <is>
+          <t>1i17xtl</t>
+        </is>
+      </c>
+      <c r="B624" t="inlineStr">
+        <is>
+          <t>Essie Matte Gel Couture vs Matte For You</t>
+        </is>
+      </c>
+      <c r="C624" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i17xtl/essie_matte_gel_couture_vs_matte_for_you/</t>
+        </is>
+      </c>
+    </row>
+    <row r="625">
+      <c r="A625" t="inlineStr">
+        <is>
+          <t>1i1bmk8</t>
+        </is>
+      </c>
+      <c r="B625" t="inlineStr">
+        <is>
+          <t>First ILNP Order!</t>
+        </is>
+      </c>
+      <c r="C625" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x4936yu6xzce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="626">
+      <c r="A626" t="inlineStr">
+        <is>
+          <t>1i1c9rj</t>
+        </is>
+      </c>
+      <c r="B626" t="inlineStr">
+        <is>
+          <t>Got two new magnetic polishes yesterday and couldn’t decide on one…</t>
+        </is>
+      </c>
+      <c r="C626" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1c9rj</t>
+        </is>
+      </c>
+    </row>
+    <row r="627">
+      <c r="A627" t="inlineStr">
+        <is>
+          <t>1i1c7n6</t>
+        </is>
+      </c>
+      <c r="B627" t="inlineStr">
+        <is>
+          <t>ILNP Petals 🌺</t>
+        </is>
+      </c>
+      <c r="C627" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qcc2jzbn10de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="628">
+      <c r="A628" t="inlineStr">
+        <is>
+          <t>1i1c3wg</t>
+        </is>
+      </c>
+      <c r="B628" t="inlineStr">
+        <is>
+          <t>✨ Like shards of mirror glass</t>
+        </is>
+      </c>
+      <c r="C628" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1c3wg</t>
+        </is>
+      </c>
+    </row>
+    <row r="629">
+      <c r="A629" t="inlineStr">
+        <is>
+          <t>1i1bed7</t>
+        </is>
+      </c>
+      <c r="B629" t="inlineStr">
+        <is>
+          <t>Polished for Days - just wow!</t>
+        </is>
+      </c>
+      <c r="C629" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qaxz771gvzce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="630">
+      <c r="A630" t="inlineStr">
+        <is>
+          <t>1i1be32</t>
+        </is>
+      </c>
+      <c r="B630" t="inlineStr">
+        <is>
+          <t>so glowy</t>
+        </is>
+      </c>
+      <c r="C630" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1be32</t>
+        </is>
+      </c>
+    </row>
+    <row r="631">
+      <c r="A631" t="inlineStr">
+        <is>
+          <t>1i1b25j</t>
+        </is>
+      </c>
+      <c r="B631" t="inlineStr">
+        <is>
+          <t>Nail always breaks in same spot</t>
+        </is>
+      </c>
+      <c r="C631" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5y30b7rvszce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="632">
+      <c r="A632" t="inlineStr">
+        <is>
+          <t>1i1avba</t>
+        </is>
+      </c>
+      <c r="B632" t="inlineStr">
+        <is>
+          <t>Decided to try a French mani for the very first time at midnight, freehand because I hate myself</t>
+        </is>
+      </c>
+      <c r="C632" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/669vxprirzce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="633">
+      <c r="A633" t="inlineStr">
+        <is>
+          <t>1i1aue6</t>
+        </is>
+      </c>
+      <c r="B633" t="inlineStr">
+        <is>
+          <t>What is your polish-related first world problem?</t>
+        </is>
+      </c>
+      <c r="C633" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i1aue6/what_is_your_polishrelated_first_world_problem/</t>
+        </is>
+      </c>
+    </row>
+    <row r="634">
+      <c r="A634" t="inlineStr">
+        <is>
+          <t>1i1atox</t>
+        </is>
+      </c>
+      <c r="B634" t="inlineStr">
+        <is>
+          <t>Can't stop staring</t>
+        </is>
+      </c>
+      <c r="C634" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/exk5pni6rzce1</t>
+        </is>
+      </c>
+    </row>
+    <row r="635">
+      <c r="A635" t="inlineStr">
+        <is>
+          <t>1i1a200</t>
+        </is>
+      </c>
+      <c r="B635" t="inlineStr">
+        <is>
+          <t>buff manicure/pedicure expectations too high?</t>
+        </is>
+      </c>
+      <c r="C635" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i1a200/buff_manicurepedicure_expectations_too_high/</t>
+        </is>
+      </c>
+    </row>
+    <row r="636">
+      <c r="A636" t="inlineStr">
+        <is>
+          <t>1i19ukt</t>
+        </is>
+      </c>
+      <c r="B636" t="inlineStr">
+        <is>
+          <t>Clionadh purchase💖</t>
+        </is>
+      </c>
+      <c r="C636" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i19ukt</t>
+        </is>
+      </c>
+    </row>
+    <row r="637">
+      <c r="A637" t="inlineStr">
+        <is>
+          <t>1i19aez</t>
+        </is>
+      </c>
+      <c r="B637" t="inlineStr">
+        <is>
+          <t>Dupe for BKL Get Lobstered?</t>
+        </is>
+      </c>
+      <c r="C637" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i19aez/dupe_for_bkl_get_lobstered/</t>
+        </is>
+      </c>
+    </row>
+    <row r="638">
+      <c r="A638" t="inlineStr">
+        <is>
+          <t>1i199vq</t>
+        </is>
+      </c>
+      <c r="B638" t="inlineStr">
+        <is>
+          <t>✨psilocin✨</t>
+        </is>
+      </c>
+      <c r="C638" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i199vq</t>
+        </is>
+      </c>
+    </row>
+    <row r="639">
+      <c r="A639" t="inlineStr">
+        <is>
+          <t>1i198br</t>
+        </is>
+      </c>
+      <c r="B639" t="inlineStr">
+        <is>
+          <t>ILNP Annabelle but blue?</t>
+        </is>
+      </c>
+      <c r="C639" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gs8xnsa6fzce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="640">
+      <c r="A640" t="inlineStr">
+        <is>
+          <t>1i18gi0</t>
+        </is>
+      </c>
+      <c r="B640" t="inlineStr">
+        <is>
+          <t>My hyponychiums are overgrown after cutting my long nails short, so I made my pinky a pencil with the extra skin as the eraser</t>
+        </is>
+      </c>
+      <c r="C640" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ha7icqk29zce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="641">
+      <c r="A641" t="inlineStr">
+        <is>
+          <t>1i17k8t</t>
+        </is>
+      </c>
+      <c r="B641" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Second polish from PPU </t>
+        </is>
+      </c>
+      <c r="C641" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i17k8t</t>
+        </is>
+      </c>
+    </row>
+    <row r="642">
+      <c r="A642" t="inlineStr">
+        <is>
+          <t>1i17f06</t>
+        </is>
+      </c>
+      <c r="B642" t="inlineStr">
+        <is>
+          <t>Holiday Nail Palette Cleanser?</t>
+        </is>
+      </c>
+      <c r="C642" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i17f06</t>
+        </is>
+      </c>
+    </row>
+    <row r="643">
+      <c r="A643" t="inlineStr">
+        <is>
+          <t>1i1733f</t>
+        </is>
+      </c>
+      <c r="B643" t="inlineStr">
+        <is>
+          <t>We have Mermaid Bait at home</t>
+        </is>
+      </c>
+      <c r="C643" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1733f</t>
+        </is>
+      </c>
+    </row>
+    <row r="644">
+      <c r="A644" t="inlineStr">
+        <is>
+          <t>1i160jz</t>
+        </is>
+      </c>
+      <c r="B644" t="inlineStr">
+        <is>
+          <t>How I swatch my magnetics</t>
+        </is>
+      </c>
+      <c r="C644" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i160jz</t>
+        </is>
+      </c>
+    </row>
+    <row r="645">
+      <c r="A645" t="inlineStr">
+        <is>
+          <t>1i15vt2</t>
+        </is>
+      </c>
+      <c r="B645" t="inlineStr">
+        <is>
+          <t>Help me find this color from the 2022 horror film Hatching</t>
+        </is>
+      </c>
+      <c r="C645" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ag8hqflvmyce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="646">
+      <c r="A646" t="inlineStr">
+        <is>
+          <t>1i15cmq</t>
+        </is>
+      </c>
+      <c r="B646" t="inlineStr">
+        <is>
+          <t>Lurid Lacquer - Hella Handmade Creations</t>
+        </is>
+      </c>
+      <c r="C646" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i15cmq/lurid_lacquer_hella_handmade_creations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="647">
+      <c r="A647" t="inlineStr">
+        <is>
+          <t>1i15c7d</t>
+        </is>
+      </c>
+      <c r="B647" t="inlineStr">
+        <is>
+          <t>The Sub Made Me Buy It - first mani of 2025</t>
+        </is>
+      </c>
+      <c r="C647" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i15c7d</t>
+        </is>
+      </c>
+    </row>
+    <row r="648">
+      <c r="A648" t="inlineStr">
+        <is>
+          <t>1i1557n</t>
+        </is>
+      </c>
+      <c r="B648" t="inlineStr">
+        <is>
+          <t>Glitter nail polish</t>
+        </is>
+      </c>
+      <c r="C648" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i1557n/glitter_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="649">
+      <c r="A649" t="inlineStr">
+        <is>
+          <t>1i14vwl</t>
+        </is>
+      </c>
+      <c r="B649" t="inlineStr">
+        <is>
+          <t>A keeper!!</t>
+        </is>
+      </c>
+      <c r="C649" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i14vwl</t>
+        </is>
+      </c>
+    </row>
+    <row r="650">
+      <c r="A650" t="inlineStr">
+        <is>
+          <t>1i142i7</t>
+        </is>
+      </c>
+      <c r="B650" t="inlineStr">
+        <is>
+          <t>Daybreak dupe?</t>
+        </is>
+      </c>
+      <c r="C650" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/009tk7oi3yce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="651">
+      <c r="A651" t="inlineStr">
+        <is>
+          <t>1i12e7i</t>
+        </is>
+      </c>
+      <c r="B651" t="inlineStr">
+        <is>
+          <t>One Year Ago vs. Now</t>
+        </is>
+      </c>
+      <c r="C651" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i12e7i</t>
+        </is>
+      </c>
+    </row>
+    <row r="652">
+      <c r="A652" t="inlineStr">
+        <is>
+          <t>1i1s87a</t>
+        </is>
+      </c>
+      <c r="B652" t="inlineStr">
+        <is>
+          <t>Some of my favorite nail art designs 🩷</t>
+        </is>
+      </c>
+      <c r="C652" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1s87a</t>
+        </is>
+      </c>
+    </row>
+    <row r="653">
+      <c r="A653" t="inlineStr">
+        <is>
+          <t>1i1q5ww</t>
+        </is>
+      </c>
+      <c r="B653" t="inlineStr">
+        <is>
+          <t>Clear Jelly Stamper Gel-ly Wraps</t>
+        </is>
+      </c>
+      <c r="C653" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1i1q5ww/clear_jelly_stamper_gelly_wraps/</t>
+        </is>
+      </c>
+    </row>
+    <row r="654">
+      <c r="A654" t="inlineStr">
+        <is>
+          <t>1i1m2e1</t>
+        </is>
+      </c>
+      <c r="B654" t="inlineStr">
+        <is>
+          <t>Painting a Simpsons Valentine Set! Starting with Homer 🤩</t>
+        </is>
+      </c>
+      <c r="C654" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xam5evkp72de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="655">
+      <c r="A655" t="inlineStr">
+        <is>
+          <t>1i1kh6n</t>
+        </is>
+      </c>
+      <c r="B655" t="inlineStr">
+        <is>
+          <t>Remove Jewels?</t>
+        </is>
+      </c>
+      <c r="C655" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wva5s6lzt1de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="656">
+      <c r="A656" t="inlineStr">
+        <is>
+          <t>1i1k80n</t>
+        </is>
+      </c>
+      <c r="B656" t="inlineStr">
+        <is>
+          <t>I DREAM OF CHROME ⛓️</t>
+        </is>
+      </c>
+      <c r="C656" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1k80n</t>
+        </is>
+      </c>
+    </row>
+    <row r="657">
+      <c r="A657" t="inlineStr">
+        <is>
+          <t>1i1jdyi</t>
+        </is>
+      </c>
+      <c r="B657" t="inlineStr">
+        <is>
+          <t xml:space="preserve">tips on aura nails </t>
+        </is>
+      </c>
+      <c r="C657" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1i1jdyi/tips_on_aura_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="658">
+      <c r="A658" t="inlineStr">
+        <is>
+          <t>1i1gk6n</t>
+        </is>
+      </c>
+      <c r="B658" t="inlineStr">
+        <is>
+          <t>Fire Emblem Fates Lady Corrin as Stained Glass Painting Nail Art!</t>
+        </is>
+      </c>
+      <c r="C658" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1gk6n</t>
+        </is>
+      </c>
+    </row>
+    <row r="659">
+      <c r="A659" t="inlineStr">
+        <is>
+          <t>1i1fv9v</t>
+        </is>
+      </c>
+      <c r="B659" t="inlineStr">
+        <is>
+          <t>Purple/lilac 💜</t>
+        </is>
+      </c>
+      <c r="C659" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dqtks85os0de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="660">
+      <c r="A660" t="inlineStr">
+        <is>
+          <t>1i1freb</t>
+        </is>
+      </c>
+      <c r="B660" t="inlineStr">
+        <is>
+          <t>Tie Dye Nail Art with Holographic Glitter</t>
+        </is>
+      </c>
+      <c r="C660" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o67nhjm4s0de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="661">
+      <c r="A661" t="inlineStr">
+        <is>
+          <t>1i1ffz9</t>
+        </is>
+      </c>
+      <c r="B661" t="inlineStr">
+        <is>
+          <t>I am just getting started making press-on nails. Any tips for the beginner?</t>
+        </is>
+      </c>
+      <c r="C661" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1i1ffz9/i_am_just_getting_started_making_presson_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="662">
+      <c r="A662" t="inlineStr">
+        <is>
+          <t>1i1ejve</t>
+        </is>
+      </c>
+      <c r="B662" t="inlineStr">
+        <is>
+          <t>Nails cute 😊💕</t>
+        </is>
+      </c>
+      <c r="C662" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qus5y9c2j0de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="663">
+      <c r="A663" t="inlineStr">
+        <is>
+          <t>1i1doqo</t>
+        </is>
+      </c>
+      <c r="B663" t="inlineStr">
+        <is>
+          <t>January, my nail tech got me</t>
+        </is>
+      </c>
+      <c r="C663" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sckw02boc0de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="664">
+      <c r="A664" t="inlineStr">
+        <is>
+          <t>1i18xxv</t>
+        </is>
+      </c>
+      <c r="B664" t="inlineStr">
+        <is>
+          <t>My nails today✨ 😍</t>
+        </is>
+      </c>
+      <c r="C664" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/83zgi1sqczce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="665">
+      <c r="A665" t="inlineStr">
+        <is>
+          <t>1i185bf</t>
+        </is>
+      </c>
+      <c r="B665" t="inlineStr">
+        <is>
+          <t>I made this set today. i´m love it! 🤩</t>
+        </is>
+      </c>
+      <c r="C665" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c2pzymxa6zce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="666">
+      <c r="A666" t="inlineStr">
+        <is>
+          <t>1i18004</t>
+        </is>
+      </c>
+      <c r="B666" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New set made by me ✨  </t>
+        </is>
+      </c>
+      <c r="C666" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/38zyedq25zce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="667">
+      <c r="A667" t="inlineStr">
+        <is>
+          <t>1i11i44</t>
+        </is>
+      </c>
+      <c r="B667" t="inlineStr">
+        <is>
+          <t>Gustav Klimt inspired nails</t>
+        </is>
+      </c>
+      <c r="C667" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nxt6sggt5xce1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="668">
+      <c r="A668" t="inlineStr">
+        <is>
+          <t>1i14pe8</t>
+        </is>
+      </c>
+      <c r="B668" t="inlineStr">
+        <is>
+          <t>throwback to an old set i painted</t>
+        </is>
+      </c>
+      <c r="C668" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ggiwqfzxayce1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Thu Jan 16 08:10:31 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_01_19.xlsx
+++ b/data/collected_data/2025_01_19.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C668"/>
+  <dimension ref="A1:C848"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11790,6 +11790,3067 @@
         </is>
       </c>
     </row>
+    <row r="669">
+      <c r="A669" t="inlineStr">
+        <is>
+          <t>1i2jzal</t>
+        </is>
+      </c>
+      <c r="B669" t="inlineStr">
+        <is>
+          <t>This set is very different for me but I'm obsessed</t>
+        </is>
+      </c>
+      <c r="C669" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2jzal</t>
+        </is>
+      </c>
+    </row>
+    <row r="670">
+      <c r="A670" t="inlineStr">
+        <is>
+          <t>1i2j2qz</t>
+        </is>
+      </c>
+      <c r="B670" t="inlineStr">
+        <is>
+          <t>My favourite color</t>
+        </is>
+      </c>
+      <c r="C670" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rhnbnzsdyade1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="671">
+      <c r="A671" t="inlineStr">
+        <is>
+          <t>1i2ij8x</t>
+        </is>
+      </c>
+      <c r="B671" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Which shape looks better? </t>
+        </is>
+      </c>
+      <c r="C671" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2ij8x</t>
+        </is>
+      </c>
+    </row>
+    <row r="672">
+      <c r="A672" t="inlineStr">
+        <is>
+          <t>1i2ic7p</t>
+        </is>
+      </c>
+      <c r="B672" t="inlineStr">
+        <is>
+          <t xml:space="preserve">try the aura cateye set for the first time👀 it’s insaneeeee! </t>
+        </is>
+      </c>
+      <c r="C672" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2ic7p</t>
+        </is>
+      </c>
+    </row>
+    <row r="673">
+      <c r="A673" t="inlineStr">
+        <is>
+          <t>1i2gncf</t>
+        </is>
+      </c>
+      <c r="B673" t="inlineStr">
+        <is>
+          <t>Am I overreacting???</t>
+        </is>
+      </c>
+      <c r="C673" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2gncf</t>
+        </is>
+      </c>
+    </row>
+    <row r="674">
+      <c r="A674" t="inlineStr">
+        <is>
+          <t>1i2hraz</t>
+        </is>
+      </c>
+      <c r="B674" t="inlineStr">
+        <is>
+          <t>Nails after removing extensions</t>
+        </is>
+      </c>
+      <c r="C674" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zfuacoeriade1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="675">
+      <c r="A675" t="inlineStr">
+        <is>
+          <t>1i2hoef</t>
+        </is>
+      </c>
+      <c r="B675" t="inlineStr">
+        <is>
+          <t>What could’ve happened?</t>
+        </is>
+      </c>
+      <c r="C675" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9shyvuiwhade1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="676">
+      <c r="A676" t="inlineStr">
+        <is>
+          <t>1i2hobx</t>
+        </is>
+      </c>
+      <c r="B676" t="inlineStr">
+        <is>
+          <t xml:space="preserve">mini junk by a new tech </t>
+        </is>
+      </c>
+      <c r="C676" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2hobx</t>
+        </is>
+      </c>
+    </row>
+    <row r="677">
+      <c r="A677" t="inlineStr">
+        <is>
+          <t>1i2h0a3</t>
+        </is>
+      </c>
+      <c r="B677" t="inlineStr">
+        <is>
+          <t>Satisfying af</t>
+        </is>
+      </c>
+      <c r="C677" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2h0a3</t>
+        </is>
+      </c>
+    </row>
+    <row r="678">
+      <c r="A678" t="inlineStr">
+        <is>
+          <t>1i2gtyi</t>
+        </is>
+      </c>
+      <c r="B678" t="inlineStr">
+        <is>
+          <t>This is another one of my technicatures, what do you think? I love mermaids</t>
+        </is>
+      </c>
+      <c r="C678" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2gtyi</t>
+        </is>
+      </c>
+    </row>
+    <row r="679">
+      <c r="A679" t="inlineStr">
+        <is>
+          <t>1i2gqzk</t>
+        </is>
+      </c>
+      <c r="B679" t="inlineStr">
+        <is>
+          <t>New year new nails (and length!)</t>
+        </is>
+      </c>
+      <c r="C679" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f3p2jy368ade1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="680">
+      <c r="A680" t="inlineStr">
+        <is>
+          <t>1i2cjfd</t>
+        </is>
+      </c>
+      <c r="B680" t="inlineStr">
+        <is>
+          <t>Am I overreacting , are these bad?</t>
+        </is>
+      </c>
+      <c r="C680" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2cjfd</t>
+        </is>
+      </c>
+    </row>
+    <row r="681">
+      <c r="A681" t="inlineStr">
+        <is>
+          <t>1i2gc7z</t>
+        </is>
+      </c>
+      <c r="B681" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first design </t>
+        </is>
+      </c>
+      <c r="C681" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/86tfx6e34ade1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="682">
+      <c r="A682" t="inlineStr">
+        <is>
+          <t>1i2g7hn</t>
+        </is>
+      </c>
+      <c r="B682" t="inlineStr">
+        <is>
+          <t>Not super complex but possibly the best I’ve ever done!</t>
+        </is>
+      </c>
+      <c r="C682" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fgps3yqr2ade1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="683">
+      <c r="A683" t="inlineStr">
+        <is>
+          <t>1i2cgir</t>
+        </is>
+      </c>
+      <c r="B683" t="inlineStr">
+        <is>
+          <t xml:space="preserve">HELP! My nails feel destroyed, Nail tech ruined my nails! </t>
+        </is>
+      </c>
+      <c r="C683" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i2cgir/help_my_nails_feel_destroyed_nail_tech_ruined_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="684">
+      <c r="A684" t="inlineStr">
+        <is>
+          <t>1i2dzrc</t>
+        </is>
+      </c>
+      <c r="B684" t="inlineStr">
+        <is>
+          <t>Help! I want a fill with builder gel, what mani would that be here?</t>
+        </is>
+      </c>
+      <c r="C684" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rbfpztgdi9de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="685">
+      <c r="A685" t="inlineStr">
+        <is>
+          <t>1i2fxjm</t>
+        </is>
+      </c>
+      <c r="B685" t="inlineStr">
+        <is>
+          <t>Shellac/gel on tips only</t>
+        </is>
+      </c>
+      <c r="C685" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i2fxjm/shellacgel_on_tips_only/</t>
+        </is>
+      </c>
+    </row>
+    <row r="686">
+      <c r="A686" t="inlineStr">
+        <is>
+          <t>1i2bfvo</t>
+        </is>
+      </c>
+      <c r="B686" t="inlineStr">
+        <is>
+          <t>Does anyone know where to get Gel X tips that match Olive &amp; June’s sizes?</t>
+        </is>
+      </c>
+      <c r="C686" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zussn7cwv8de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="687">
+      <c r="A687" t="inlineStr">
+        <is>
+          <t>1i2bgup</t>
+        </is>
+      </c>
+      <c r="B687" t="inlineStr">
+        <is>
+          <t>Trying something different (for me)</t>
+        </is>
+      </c>
+      <c r="C687" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2bgup</t>
+        </is>
+      </c>
+    </row>
+    <row r="688">
+      <c r="A688" t="inlineStr">
+        <is>
+          <t>1i2czd5</t>
+        </is>
+      </c>
+      <c r="B688" t="inlineStr">
+        <is>
+          <t>Entering my Boho Era✌️</t>
+        </is>
+      </c>
+      <c r="C688" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tf23bzs899de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="689">
+      <c r="A689" t="inlineStr">
+        <is>
+          <t>1i2fud7</t>
+        </is>
+      </c>
+      <c r="B689" t="inlineStr">
+        <is>
+          <t xml:space="preserve">gems have me obsessed </t>
+        </is>
+      </c>
+      <c r="C689" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zjtrth19z9de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="690">
+      <c r="A690" t="inlineStr">
+        <is>
+          <t>1i2fqel</t>
+        </is>
+      </c>
+      <c r="B690" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Almond shape? It was recommended that I try a shape to elongate my nails, any advice or do they look okay? </t>
+        </is>
+      </c>
+      <c r="C690" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7styjbx6y9de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="691">
+      <c r="A691" t="inlineStr">
+        <is>
+          <t>1i2fp4g</t>
+        </is>
+      </c>
+      <c r="B691" t="inlineStr">
+        <is>
+          <t>What should I improve on in shaping?</t>
+        </is>
+      </c>
+      <c r="C691" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2fp4g</t>
+        </is>
+      </c>
+    </row>
+    <row r="692">
+      <c r="A692" t="inlineStr">
+        <is>
+          <t>1i2foqw</t>
+        </is>
+      </c>
+      <c r="B692" t="inlineStr">
+        <is>
+          <t>Keyboards?</t>
+        </is>
+      </c>
+      <c r="C692" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i2foqw/keyboards/</t>
+        </is>
+      </c>
+    </row>
+    <row r="693">
+      <c r="A693" t="inlineStr">
+        <is>
+          <t>1i2fl9e</t>
+        </is>
+      </c>
+      <c r="B693" t="inlineStr">
+        <is>
+          <t>Nail lamps recs</t>
+        </is>
+      </c>
+      <c r="C693" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i2fl9e/nail_lamps_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="694">
+      <c r="A694" t="inlineStr">
+        <is>
+          <t>1i2erxr</t>
+        </is>
+      </c>
+      <c r="B694" t="inlineStr">
+        <is>
+          <t>Spacey GelX nails done by me</t>
+        </is>
+      </c>
+      <c r="C694" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/83cqpjvfp9de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="695">
+      <c r="A695" t="inlineStr">
+        <is>
+          <t>1i2eb5c</t>
+        </is>
+      </c>
+      <c r="B695" t="inlineStr">
+        <is>
+          <t>black french with a little ✨flavor✨</t>
+        </is>
+      </c>
+      <c r="C695" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/or2rd1e7l9de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="696">
+      <c r="A696" t="inlineStr">
+        <is>
+          <t>1i2e0me</t>
+        </is>
+      </c>
+      <c r="B696" t="inlineStr">
+        <is>
+          <t>What do you think about black french? Like or not?✨</t>
+        </is>
+      </c>
+      <c r="C696" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2e0me</t>
+        </is>
+      </c>
+    </row>
+    <row r="697">
+      <c r="A697" t="inlineStr">
+        <is>
+          <t>1i2dn6f</t>
+        </is>
+      </c>
+      <c r="B697" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lightning Strikes! </t>
+        </is>
+      </c>
+      <c r="C697" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cvjay6v6f9de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="698">
+      <c r="A698" t="inlineStr">
+        <is>
+          <t>1i2djvq</t>
+        </is>
+      </c>
+      <c r="B698" t="inlineStr">
+        <is>
+          <t>Outer space 🚀✨🌙</t>
+        </is>
+      </c>
+      <c r="C698" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2djvq</t>
+        </is>
+      </c>
+    </row>
+    <row r="699">
+      <c r="A699" t="inlineStr">
+        <is>
+          <t>1i2dhle</t>
+        </is>
+      </c>
+      <c r="B699" t="inlineStr">
+        <is>
+          <t>What's something you didn't mean to knick with your e-file? I'll go first</t>
+        </is>
+      </c>
+      <c r="C699" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1rvco8zrd9de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="700">
+      <c r="A700" t="inlineStr">
+        <is>
+          <t>1i2dh9g</t>
+        </is>
+      </c>
+      <c r="B700" t="inlineStr">
+        <is>
+          <t>Fun 420 themed nails 💚</t>
+        </is>
+      </c>
+      <c r="C700" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2dh9g</t>
+        </is>
+      </c>
+    </row>
+    <row r="701">
+      <c r="A701" t="inlineStr">
+        <is>
+          <t>1i2cuhr</t>
+        </is>
+      </c>
+      <c r="B701" t="inlineStr">
+        <is>
+          <t>First time going for the clean girl aesthetic 🫧</t>
+        </is>
+      </c>
+      <c r="C701" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2cuhr</t>
+        </is>
+      </c>
+    </row>
+    <row r="702">
+      <c r="A702" t="inlineStr">
+        <is>
+          <t>1i2cp6t</t>
+        </is>
+      </c>
+      <c r="B702" t="inlineStr">
+        <is>
+          <t>first time using metal charms!!</t>
+        </is>
+      </c>
+      <c r="C702" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qrm9tp0r69de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="703">
+      <c r="A703" t="inlineStr">
+        <is>
+          <t>1i2bzbg</t>
+        </is>
+      </c>
+      <c r="B703" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do I protect my nails while working in food service? </t>
+        </is>
+      </c>
+      <c r="C703" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i2bzbg/how_do_i_protect_my_nails_while_working_in_food/</t>
+        </is>
+      </c>
+    </row>
+    <row r="704">
+      <c r="A704" t="inlineStr">
+        <is>
+          <t>1i2c132</t>
+        </is>
+      </c>
+      <c r="B704" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Me gusta, es elegante y bonito </t>
+        </is>
+      </c>
+      <c r="C704" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ippsm5wx09de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="705">
+      <c r="A705" t="inlineStr">
+        <is>
+          <t>1i2bsh7</t>
+        </is>
+      </c>
+      <c r="B705" t="inlineStr">
+        <is>
+          <t>First time doing gel at home</t>
+        </is>
+      </c>
+      <c r="C705" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xotja5qwy8de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="706">
+      <c r="A706" t="inlineStr">
+        <is>
+          <t>1i2brll</t>
+        </is>
+      </c>
+      <c r="B706" t="inlineStr">
+        <is>
+          <t>This girl I like is gonna let me do her nails and I wanna do a good job!</t>
+        </is>
+      </c>
+      <c r="C706" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i2brll/this_girl_i_like_is_gonna_let_me_do_her_nails_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="707">
+      <c r="A707" t="inlineStr">
+        <is>
+          <t>1i2bkmb</t>
+        </is>
+      </c>
+      <c r="B707" t="inlineStr">
+        <is>
+          <t>incapacitated with the flu but atleast i love my nails 🥹</t>
+        </is>
+      </c>
+      <c r="C707" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2bkmb</t>
+        </is>
+      </c>
+    </row>
+    <row r="708">
+      <c r="A708" t="inlineStr">
+        <is>
+          <t>1i2bfah</t>
+        </is>
+      </c>
+      <c r="B708" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first time trying solar polish
+</t>
+        </is>
+      </c>
+      <c r="C708" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2bfah</t>
+        </is>
+      </c>
+    </row>
+    <row r="709">
+      <c r="A709" t="inlineStr">
+        <is>
+          <t>1i2b6jf</t>
+        </is>
+      </c>
+      <c r="B709" t="inlineStr">
+        <is>
+          <t>I may like crazy but…</t>
+        </is>
+      </c>
+      <c r="C709" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/43mcdufpt8de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="710">
+      <c r="A710" t="inlineStr">
+        <is>
+          <t>1i2b63g</t>
+        </is>
+      </c>
+      <c r="B710" t="inlineStr">
+        <is>
+          <t>I’m trying new effects, this is cat’s eye, what do you think?</t>
+        </is>
+      </c>
+      <c r="C710" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jsdyozglt8de1</t>
+        </is>
+      </c>
+    </row>
+    <row r="711">
+      <c r="A711" t="inlineStr">
+        <is>
+          <t>1i2alme</t>
+        </is>
+      </c>
+      <c r="B711" t="inlineStr">
+        <is>
+          <t>🧧🍊</t>
+        </is>
+      </c>
+      <c r="C711" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2alme</t>
+        </is>
+      </c>
+    </row>
+    <row r="712">
+      <c r="A712" t="inlineStr">
+        <is>
+          <t>1i2aiut</t>
+        </is>
+      </c>
+      <c r="B712" t="inlineStr">
+        <is>
+          <t>Cat eye polish</t>
+        </is>
+      </c>
+      <c r="C712" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i2aiut/cat_eye_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="713">
+      <c r="A713" t="inlineStr">
+        <is>
+          <t>1i2a5wi</t>
+        </is>
+      </c>
+      <c r="B713" t="inlineStr">
+        <is>
+          <t>I am in love with these nails but is this pricey? I’m not familiar with gel overlay</t>
+        </is>
+      </c>
+      <c r="C713" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2a5wi</t>
+        </is>
+      </c>
+    </row>
+    <row r="714">
+      <c r="A714" t="inlineStr">
+        <is>
+          <t>1i29qc1</t>
+        </is>
+      </c>
+      <c r="B714" t="inlineStr">
+        <is>
+          <t>Question for Nail techs: Extra charge for inspo?</t>
+        </is>
+      </c>
+      <c r="C714" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i29qc1/question_for_nail_techs_extra_charge_for_inspo/</t>
+        </is>
+      </c>
+    </row>
+    <row r="715">
+      <c r="A715" t="inlineStr">
+        <is>
+          <t>1i2aa19</t>
+        </is>
+      </c>
+      <c r="B715" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beginner nails! </t>
+        </is>
+      </c>
+      <c r="C715" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vlzvueocm8de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="716">
+      <c r="A716" t="inlineStr">
+        <is>
+          <t>1i2a6fb</t>
+        </is>
+      </c>
+      <c r="B716" t="inlineStr">
+        <is>
+          <t>Where can I get my nails done like this in Toronto?</t>
+        </is>
+      </c>
+      <c r="C716" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2a6fb</t>
+        </is>
+      </c>
+    </row>
+    <row r="717">
+      <c r="A717" t="inlineStr">
+        <is>
+          <t>1i2a2rd</t>
+        </is>
+      </c>
+      <c r="B717" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hyperrealistic stilettos </t>
+        </is>
+      </c>
+      <c r="C717" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2a2rd</t>
+        </is>
+      </c>
+    </row>
+    <row r="718">
+      <c r="A718" t="inlineStr">
+        <is>
+          <t>1i29xpd</t>
+        </is>
+      </c>
+      <c r="B718" t="inlineStr">
+        <is>
+          <t>Give it to me straight x&lt;3</t>
+        </is>
+      </c>
+      <c r="C718" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i29xpd</t>
+        </is>
+      </c>
+    </row>
+    <row r="719">
+      <c r="A719" t="inlineStr">
+        <is>
+          <t>1i29uvw</t>
+        </is>
+      </c>
+      <c r="B719" t="inlineStr">
+        <is>
+          <t>Butterfly press ons</t>
+        </is>
+      </c>
+      <c r="C719" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xh72gjsyi8de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="720">
+      <c r="A720" t="inlineStr">
+        <is>
+          <t>1i29kpd</t>
+        </is>
+      </c>
+      <c r="B720" t="inlineStr">
+        <is>
+          <t>I painted my nails for the first time</t>
+        </is>
+      </c>
+      <c r="C720" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lz9dpp3qg8de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="721">
+      <c r="A721" t="inlineStr">
+        <is>
+          <t>1i29k0r</t>
+        </is>
+      </c>
+      <c r="B721" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just classic French tips </t>
+        </is>
+      </c>
+      <c r="C721" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i29k0r</t>
+        </is>
+      </c>
+    </row>
+    <row r="722">
+      <c r="A722" t="inlineStr">
+        <is>
+          <t>1i29fd5</t>
+        </is>
+      </c>
+      <c r="B722" t="inlineStr">
+        <is>
+          <t>It has taken me a lot of work. What do you think of the result? It's just a demonstration</t>
+        </is>
+      </c>
+      <c r="C722" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i29fd5</t>
+        </is>
+      </c>
+    </row>
+    <row r="723">
+      <c r="A723" t="inlineStr">
+        <is>
+          <t>1i28xcs</t>
+        </is>
+      </c>
+      <c r="B723" t="inlineStr">
+        <is>
+          <t>Nails in memory of my husky</t>
+        </is>
+      </c>
+      <c r="C723" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i28xcs</t>
+        </is>
+      </c>
+    </row>
+    <row r="724">
+      <c r="A724" t="inlineStr">
+        <is>
+          <t>1i25v6a</t>
+        </is>
+      </c>
+      <c r="B724" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anyone post photos of their nails and then get weird messages immediately after? </t>
+        </is>
+      </c>
+      <c r="C724" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i25v6a/anyone_post_photos_of_their_nails_and_then_get/</t>
+        </is>
+      </c>
+    </row>
+    <row r="725">
+      <c r="A725" t="inlineStr">
+        <is>
+          <t>1i28926</t>
+        </is>
+      </c>
+      <c r="B725" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Silver nailart </t>
+        </is>
+      </c>
+      <c r="C725" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lqujaclg68de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="726">
+      <c r="A726" t="inlineStr">
+        <is>
+          <t>1i286gt</t>
+        </is>
+      </c>
+      <c r="B726" t="inlineStr">
+        <is>
+          <t>💜💜💜</t>
+        </is>
+      </c>
+      <c r="C726" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2n6qg2xt58de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="727">
+      <c r="A727" t="inlineStr">
+        <is>
+          <t>1i285xe</t>
+        </is>
+      </c>
+      <c r="B727" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Viva Las Vegas. </t>
+        </is>
+      </c>
+      <c r="C727" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tcgvnmsr58de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="728">
+      <c r="A728" t="inlineStr">
+        <is>
+          <t>1i284ws</t>
+        </is>
+      </c>
+      <c r="B728" t="inlineStr">
+        <is>
+          <t>For nail techs- where do you operate your business?</t>
+        </is>
+      </c>
+      <c r="C728" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i284ws/for_nail_techs_where_do_you_operate_your_business/</t>
+        </is>
+      </c>
+    </row>
+    <row r="729">
+      <c r="A729" t="inlineStr">
+        <is>
+          <t>1i22yl0</t>
+        </is>
+      </c>
+      <c r="B729" t="inlineStr">
+        <is>
+          <t>Detachable Fake Nail Extensions</t>
+        </is>
+      </c>
+      <c r="C729" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i22yl0/detachable_fake_nail_extensions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="730">
+      <c r="A730" t="inlineStr">
+        <is>
+          <t>1i27rnp</t>
+        </is>
+      </c>
+      <c r="B730" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Layered colors </t>
+        </is>
+      </c>
+      <c r="C730" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kjsr8f4r28de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="731">
+      <c r="A731" t="inlineStr">
+        <is>
+          <t>1i27ovh</t>
+        </is>
+      </c>
+      <c r="B731" t="inlineStr">
+        <is>
+          <t>Our matching vacation nails</t>
+        </is>
+      </c>
+      <c r="C731" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i27ovh</t>
+        </is>
+      </c>
+    </row>
+    <row r="732">
+      <c r="A732" t="inlineStr">
+        <is>
+          <t>1i27nyz</t>
+        </is>
+      </c>
+      <c r="B732" t="inlineStr">
+        <is>
+          <t>Accidentally used dip powder as acrylic powder. Is this an option?</t>
+        </is>
+      </c>
+      <c r="C732" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i27nyz/accidentally_used_dip_powder_as_acrylic_powder_is/</t>
+        </is>
+      </c>
+    </row>
+    <row r="733">
+      <c r="A733" t="inlineStr">
+        <is>
+          <t>1i27g6x</t>
+        </is>
+      </c>
+      <c r="B733" t="inlineStr">
+        <is>
+          <t>Absolutely in love with my nails! (Done at Naturally Nails in Clayton, BC)</t>
+        </is>
+      </c>
+      <c r="C733" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zrsfzg3808de1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="734">
+      <c r="A734" t="inlineStr">
+        <is>
+          <t>1i27cpg</t>
+        </is>
+      </c>
+      <c r="B734" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Manicure advice </t>
+        </is>
+      </c>
+      <c r="C734" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i27cpg/manicure_advice/</t>
+        </is>
+      </c>
+    </row>
+    <row r="735">
+      <c r="A735" t="inlineStr">
+        <is>
+          <t>1i274nz</t>
+        </is>
+      </c>
+      <c r="B735" t="inlineStr">
+        <is>
+          <t>WEEKLY NAIL GROWTH RATE</t>
+        </is>
+      </c>
+      <c r="C735" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rwolexrrx7de1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="736">
+      <c r="A736" t="inlineStr">
+        <is>
+          <t>1i273yi</t>
+        </is>
+      </c>
+      <c r="B736" t="inlineStr">
+        <is>
+          <t xml:space="preserve">usahana nails~ </t>
+        </is>
+      </c>
+      <c r="C736" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i273yi</t>
+        </is>
+      </c>
+    </row>
+    <row r="737">
+      <c r="A737" t="inlineStr">
+        <is>
+          <t>1i26xhw</t>
+        </is>
+      </c>
+      <c r="B737" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kiss Magnetic Velvet gel press on nails 10/10 </t>
+        </is>
+      </c>
+      <c r="C737" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i26xhw/kiss_magnetic_velvet_gel_press_on_nails_1010/</t>
+        </is>
+      </c>
+    </row>
+    <row r="738">
+      <c r="A738" t="inlineStr">
+        <is>
+          <t>1i26que</t>
+        </is>
+      </c>
+      <c r="B738" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Builder gel or acrylic nails? </t>
+        </is>
+      </c>
+      <c r="C738" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i26que/builder_gel_or_acrylic_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="739">
+      <c r="A739" t="inlineStr">
+        <is>
+          <t>1i25w3m</t>
+        </is>
+      </c>
+      <c r="B739" t="inlineStr">
+        <is>
+          <t>Skin under nails?</t>
+        </is>
+      </c>
+      <c r="C739" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i25w3m/skin_under_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="740">
+      <c r="A740" t="inlineStr">
+        <is>
+          <t>1i26iek</t>
+        </is>
+      </c>
+      <c r="B740" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Plus size nails </t>
+        </is>
+      </c>
+      <c r="C740" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i26iek/plus_size_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="741">
+      <c r="A741" t="inlineStr">
+        <is>
+          <t>1i263a9</t>
+        </is>
+      </c>
+      <c r="B741" t="inlineStr">
+        <is>
+          <t>my fishing lure nails!!</t>
+        </is>
+      </c>
+      <c r="C741" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i263a9</t>
+        </is>
+      </c>
+    </row>
+    <row r="742">
+      <c r="A742" t="inlineStr">
+        <is>
+          <t>1i25sp5</t>
+        </is>
+      </c>
+      <c r="B742" t="inlineStr">
+        <is>
+          <t>My first set of 2025. What do you think? ☃️</t>
+        </is>
+      </c>
+      <c r="C742" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1qkxhoafn7de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="743">
+      <c r="A743" t="inlineStr">
+        <is>
+          <t>1i25m27</t>
+        </is>
+      </c>
+      <c r="B743" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Worth it? </t>
+        </is>
+      </c>
+      <c r="C743" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4uzyd9o0m7de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="744">
+      <c r="A744" t="inlineStr">
+        <is>
+          <t>1i25j4z</t>
+        </is>
+      </c>
+      <c r="B744" t="inlineStr">
+        <is>
+          <t>Kokoist system</t>
+        </is>
+      </c>
+      <c r="C744" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ecqnkj2fl7de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="745">
+      <c r="A745" t="inlineStr">
+        <is>
+          <t>1i24oaq</t>
+        </is>
+      </c>
+      <c r="B745" t="inlineStr">
+        <is>
+          <t>Recovering from nail biting</t>
+        </is>
+      </c>
+      <c r="C745" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i24oaq/recovering_from_nail_biting/</t>
+        </is>
+      </c>
+    </row>
+    <row r="746">
+      <c r="A746" t="inlineStr">
+        <is>
+          <t>1i24b2c</t>
+        </is>
+      </c>
+      <c r="B746" t="inlineStr">
+        <is>
+          <t>Rotary nail file</t>
+        </is>
+      </c>
+      <c r="C746" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i24b2c/rotary_nail_file/</t>
+        </is>
+      </c>
+    </row>
+    <row r="747">
+      <c r="A747" t="inlineStr">
+        <is>
+          <t>1i24iue</t>
+        </is>
+      </c>
+      <c r="B747" t="inlineStr">
+        <is>
+          <t>Looking for Garden Path Lacquers in Europe</t>
+        </is>
+      </c>
+      <c r="C747" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i24iue/looking_for_garden_path_lacquers_in_europe/</t>
+        </is>
+      </c>
+    </row>
+    <row r="748">
+      <c r="A748" t="inlineStr">
+        <is>
+          <t>1i24gvb</t>
+        </is>
+      </c>
+      <c r="B748" t="inlineStr">
+        <is>
+          <t>First nails of 2025💁🏼‍♀️</t>
+        </is>
+      </c>
+      <c r="C748" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hx6kkbgkd7de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="749">
+      <c r="A749" t="inlineStr">
+        <is>
+          <t>1i2484u</t>
+        </is>
+      </c>
+      <c r="B749" t="inlineStr">
+        <is>
+          <t>Kokoist gel and nail lamp</t>
+        </is>
+      </c>
+      <c r="C749" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8yj82smpb7de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="750">
+      <c r="A750" t="inlineStr">
+        <is>
+          <t>1i240p7</t>
+        </is>
+      </c>
+      <c r="B750" t="inlineStr">
+        <is>
+          <t>Had to start over :’(</t>
+        </is>
+      </c>
+      <c r="C750" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i240p7</t>
+        </is>
+      </c>
+    </row>
+    <row r="751">
+      <c r="A751" t="inlineStr">
+        <is>
+          <t>1i23u3e</t>
+        </is>
+      </c>
+      <c r="B751" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just a few of the sets I started making for friends! </t>
+        </is>
+      </c>
+      <c r="C751" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i23u3e</t>
+        </is>
+      </c>
+    </row>
+    <row r="752">
+      <c r="A752" t="inlineStr">
+        <is>
+          <t>1i23sto</t>
+        </is>
+      </c>
+      <c r="B752" t="inlineStr">
+        <is>
+          <t>Bought my first cute press on nails</t>
+        </is>
+      </c>
+      <c r="C752" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xk15p2qg87de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="753">
+      <c r="A753" t="inlineStr">
+        <is>
+          <t>1i23hen</t>
+        </is>
+      </c>
+      <c r="B753" t="inlineStr">
+        <is>
+          <t>This mug inspired my press ons I made hehe 😋</t>
+        </is>
+      </c>
+      <c r="C753" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i23hen</t>
+        </is>
+      </c>
+    </row>
+    <row r="754">
+      <c r="A754" t="inlineStr">
+        <is>
+          <t>1i23mro</t>
+        </is>
+      </c>
+      <c r="B754" t="inlineStr">
+        <is>
+          <t>January nails🥀</t>
+        </is>
+      </c>
+      <c r="C754" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kz61q71577de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="755">
+      <c r="A755" t="inlineStr">
+        <is>
+          <t>1i22o3h</t>
+        </is>
+      </c>
+      <c r="B755" t="inlineStr">
+        <is>
+          <t>Skin Around My Nails Look Bad</t>
+        </is>
+      </c>
+      <c r="C755" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i22o3h</t>
+        </is>
+      </c>
+    </row>
+    <row r="756">
+      <c r="A756" t="inlineStr">
+        <is>
+          <t>1i22fvc</t>
+        </is>
+      </c>
+      <c r="B756" t="inlineStr">
+        <is>
+          <t>First time fake nails 💅(love them)!</t>
+        </is>
+      </c>
+      <c r="C756" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i22fvc</t>
+        </is>
+      </c>
+    </row>
+    <row r="757">
+      <c r="A757" t="inlineStr">
+        <is>
+          <t>1i22c3g</t>
+        </is>
+      </c>
+      <c r="B757" t="inlineStr">
+        <is>
+          <t>365, party girl 💚💅</t>
+        </is>
+      </c>
+      <c r="C757" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uf9qfo4ix6de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="758">
+      <c r="A758" t="inlineStr">
+        <is>
+          <t>1i22asa</t>
+        </is>
+      </c>
+      <c r="B758" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did my own nails 💅 </t>
+        </is>
+      </c>
+      <c r="C758" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i22asa</t>
+        </is>
+      </c>
+    </row>
+    <row r="759">
+      <c r="A759" t="inlineStr">
+        <is>
+          <t>1i21wcf</t>
+        </is>
+      </c>
+      <c r="B759" t="inlineStr">
+        <is>
+          <t>Genshin impact nails</t>
+        </is>
+      </c>
+      <c r="C759" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wbbgpfjau6de1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="760">
+      <c r="A760" t="inlineStr">
+        <is>
+          <t>1i224s3</t>
+        </is>
+      </c>
+      <c r="B760" t="inlineStr">
+        <is>
+          <t>New nails to match my new bag!</t>
+        </is>
+      </c>
+      <c r="C760" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d74yoxfzv6de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="761">
+      <c r="A761" t="inlineStr">
+        <is>
+          <t>1i224ch</t>
+        </is>
+      </c>
+      <c r="B761" t="inlineStr">
+        <is>
+          <t>Making Press Ons - Does brand matter?</t>
+        </is>
+      </c>
+      <c r="C761" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i224ch/making_press_ons_does_brand_matter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="762">
+      <c r="A762" t="inlineStr">
+        <is>
+          <t>1i21ile</t>
+        </is>
+      </c>
+      <c r="B762" t="inlineStr">
+        <is>
+          <t>give these nails a caption! ⭐️</t>
+        </is>
+      </c>
+      <c r="C762" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i21ile</t>
+        </is>
+      </c>
+    </row>
+    <row r="763">
+      <c r="A763" t="inlineStr">
+        <is>
+          <t>1i21nf5</t>
+        </is>
+      </c>
+      <c r="B763" t="inlineStr">
+        <is>
+          <t>First nails of 2025 ! In love with them 💗</t>
+        </is>
+      </c>
+      <c r="C763" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hx9mcrpds6de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="764">
+      <c r="A764" t="inlineStr">
+        <is>
+          <t>1i21djl</t>
+        </is>
+      </c>
+      <c r="B764" t="inlineStr">
+        <is>
+          <t xml:space="preserve">January 💙 </t>
+        </is>
+      </c>
+      <c r="C764" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/to2nydo9q6de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="765">
+      <c r="A765" t="inlineStr">
+        <is>
+          <t>1i1vfus</t>
+        </is>
+      </c>
+      <c r="B765" t="inlineStr">
+        <is>
+          <t>It’s been a while, talk to me about shape and gel risk</t>
+        </is>
+      </c>
+      <c r="C765" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i1vfus/its_been_a_while_talk_to_me_about_shape_and_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="766">
+      <c r="A766" t="inlineStr">
+        <is>
+          <t>1i1wj59</t>
+        </is>
+      </c>
+      <c r="B766" t="inlineStr">
+        <is>
+          <t>Blending tips after or before base coat? Help with Switching to Fill-Ins</t>
+        </is>
+      </c>
+      <c r="C766" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i1wj59/blending_tips_after_or_before_base_coat_help_with/</t>
+        </is>
+      </c>
+    </row>
+    <row r="767">
+      <c r="A767" t="inlineStr">
+        <is>
+          <t>1i211lc</t>
+        </is>
+      </c>
+      <c r="B767" t="inlineStr">
+        <is>
+          <t>Clean Shimmer on Short Nails</t>
+        </is>
+      </c>
+      <c r="C767" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bnq3l0jpn6de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="768">
+      <c r="A768" t="inlineStr">
+        <is>
+          <t>1i20qfi</t>
+        </is>
+      </c>
+      <c r="B768" t="inlineStr">
+        <is>
+          <t xml:space="preserve">it’s always a dopamine boost when I get my nails done ♡ </t>
+        </is>
+      </c>
+      <c r="C768" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vcara0lbl6de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="769">
+      <c r="A769" t="inlineStr">
+        <is>
+          <t>1i2ipux</t>
+        </is>
+      </c>
+      <c r="B769" t="inlineStr">
+        <is>
+          <t xml:space="preserve">To whoever shared that BK Choose Life is back in stock. Holy wow. New favorite polish. Thank you. </t>
+        </is>
+      </c>
+      <c r="C769" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/9ul7lbowtade1</t>
+        </is>
+      </c>
+    </row>
+    <row r="770">
+      <c r="A770" t="inlineStr">
+        <is>
+          <t>1i2ikqj</t>
+        </is>
+      </c>
+      <c r="B770" t="inlineStr">
+        <is>
+          <t>Let's talk solar polish 🌞</t>
+        </is>
+      </c>
+      <c r="C770" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6kjhpim6sade1</t>
+        </is>
+      </c>
+    </row>
+    <row r="771">
+      <c r="A771" t="inlineStr">
+        <is>
+          <t>1i2i9v6</t>
+        </is>
+      </c>
+      <c r="B771" t="inlineStr">
+        <is>
+          <t>Does anyone have recommendations for glowy shimmer toppers, or do they not exist?</t>
+        </is>
+      </c>
+      <c r="C771" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2i9v6</t>
+        </is>
+      </c>
+    </row>
+    <row r="772">
+      <c r="A772" t="inlineStr">
+        <is>
+          <t>1i2i2nc</t>
+        </is>
+      </c>
+      <c r="B772" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Accidentally made a combo that almost dupes Mooncat Dragon Scales--maybe I can take it off my wish list?? </t>
+        </is>
+      </c>
+      <c r="C772" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2i2nc</t>
+        </is>
+      </c>
+    </row>
+    <row r="773">
+      <c r="A773" t="inlineStr">
+        <is>
+          <t>1i2hlpy</t>
+        </is>
+      </c>
+      <c r="B773" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did OPI discontinue their lacquer thinner??? </t>
+        </is>
+      </c>
+      <c r="C773" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i2hlpy/did_opi_discontinue_their_lacquer_thinner/</t>
+        </is>
+      </c>
+    </row>
+    <row r="774">
+      <c r="A774" t="inlineStr">
+        <is>
+          <t>1i2gnys</t>
+        </is>
+      </c>
+      <c r="B774" t="inlineStr">
+        <is>
+          <t>Attempting to dupe Sassy Sauce's Cock A Doodle Doom</t>
+        </is>
+      </c>
+      <c r="C774" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2gnys</t>
+        </is>
+      </c>
+    </row>
+    <row r="775">
+      <c r="A775" t="inlineStr">
+        <is>
+          <t>1i2gl70</t>
+        </is>
+      </c>
+      <c r="B775" t="inlineStr">
+        <is>
+          <t xml:space="preserve">BEHOLD - a star is born. </t>
+        </is>
+      </c>
+      <c r="C775" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2gl70</t>
+        </is>
+      </c>
+    </row>
+    <row r="776">
+      <c r="A776" t="inlineStr">
+        <is>
+          <t>1i2ghwz</t>
+        </is>
+      </c>
+      <c r="B776" t="inlineStr">
+        <is>
+          <t>I'm in love 💗</t>
+        </is>
+      </c>
+      <c r="C776" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2ghwz</t>
+        </is>
+      </c>
+    </row>
+    <row r="777">
+      <c r="A777" t="inlineStr">
+        <is>
+          <t>1i2g8oy</t>
+        </is>
+      </c>
+      <c r="B777" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Solidarity Inspired </t>
+        </is>
+      </c>
+      <c r="C777" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2g8oy</t>
+        </is>
+      </c>
+    </row>
+    <row r="778">
+      <c r="A778" t="inlineStr">
+        <is>
+          <t>1i2g5rf</t>
+        </is>
+      </c>
+      <c r="B778" t="inlineStr">
+        <is>
+          <t>Matte Top Coat</t>
+        </is>
+      </c>
+      <c r="C778" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2g5rf</t>
+        </is>
+      </c>
+    </row>
+    <row r="779">
+      <c r="A779" t="inlineStr">
+        <is>
+          <t>1i2fnbk</t>
+        </is>
+      </c>
+      <c r="B779" t="inlineStr">
+        <is>
+          <t>Love/hate relationship with ILNP</t>
+        </is>
+      </c>
+      <c r="C779" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i2fnbk/lovehate_relationship_with_ilnp/</t>
+        </is>
+      </c>
+    </row>
+    <row r="780">
+      <c r="A780" t="inlineStr">
+        <is>
+          <t>1i2fmmp</t>
+        </is>
+      </c>
+      <c r="B780" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does anyone know how to get this effect? </t>
+        </is>
+      </c>
+      <c r="C780" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2fmmp</t>
+        </is>
+      </c>
+    </row>
+    <row r="781">
+      <c r="A781" t="inlineStr">
+        <is>
+          <t>1i2fbmm</t>
+        </is>
+      </c>
+      <c r="B781" t="inlineStr">
+        <is>
+          <t>Lūmen Haunted Melody</t>
+        </is>
+      </c>
+      <c r="C781" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u8amewkbu9de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="782">
+      <c r="A782" t="inlineStr">
+        <is>
+          <t>1i2et6q</t>
+        </is>
+      </c>
+      <c r="B782" t="inlineStr">
+        <is>
+          <t>Husband asked if he could paint my nails 🥹</t>
+        </is>
+      </c>
+      <c r="C782" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2et6q</t>
+        </is>
+      </c>
+    </row>
+    <row r="783">
+      <c r="A783" t="inlineStr">
+        <is>
+          <t>1i2el5u</t>
+        </is>
+      </c>
+      <c r="B783" t="inlineStr">
+        <is>
+          <t>Nude Color Favs &amp; Recs?</t>
+        </is>
+      </c>
+      <c r="C783" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i2el5u/nude_color_favs_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="784">
+      <c r="A784" t="inlineStr">
+        <is>
+          <t>1i2e8lm</t>
+        </is>
+      </c>
+      <c r="B784" t="inlineStr">
+        <is>
+          <t>layering colors&gt;&gt;&gt;&gt;</t>
+        </is>
+      </c>
+      <c r="C784" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j2sjytmjk9de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="785">
+      <c r="A785" t="inlineStr">
+        <is>
+          <t>1i2cv44</t>
+        </is>
+      </c>
+      <c r="B785" t="inlineStr">
+        <is>
+          <t>When is it a bad batch?</t>
+        </is>
+      </c>
+      <c r="C785" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2cv44</t>
+        </is>
+      </c>
+    </row>
+    <row r="786">
+      <c r="A786" t="inlineStr">
+        <is>
+          <t>1i2cq77</t>
+        </is>
+      </c>
+      <c r="B786" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sissi gel does it again 👏 </t>
+        </is>
+      </c>
+      <c r="C786" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/rs5sywyz69de1</t>
+        </is>
+      </c>
+    </row>
+    <row r="787">
+      <c r="A787" t="inlineStr">
+        <is>
+          <t>1i2cm0e</t>
+        </is>
+      </c>
+      <c r="B787" t="inlineStr">
+        <is>
+          <t>Dupe for Glo Worm by Danglefoot</t>
+        </is>
+      </c>
+      <c r="C787" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hcnclbuz59de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="788">
+      <c r="A788" t="inlineStr">
+        <is>
+          <t>1i2cjco</t>
+        </is>
+      </c>
+      <c r="B788" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Update: Polish Sorting </t>
+        </is>
+      </c>
+      <c r="C788" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2cjco</t>
+        </is>
+      </c>
+    </row>
+    <row r="789">
+      <c r="A789" t="inlineStr">
+        <is>
+          <t>1i2cb6j</t>
+        </is>
+      </c>
+      <c r="B789" t="inlineStr">
+        <is>
+          <t>Sassy Sauce and Starrily-a rave and a moderate and surprising disappointment</t>
+        </is>
+      </c>
+      <c r="C789" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d102fmad39de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="790">
+      <c r="A790" t="inlineStr">
+        <is>
+          <t>1i2c4vg</t>
+        </is>
+      </c>
+      <c r="B790" t="inlineStr">
+        <is>
+          <t xml:space="preserve">glitter grabber/smoother. kbshimmer or glisten and glow?  </t>
+        </is>
+      </c>
+      <c r="C790" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i2c4vg/glitter_grabbersmoother_kbshimmer_or_glisten_and/</t>
+        </is>
+      </c>
+    </row>
+    <row r="791">
+      <c r="A791" t="inlineStr">
+        <is>
+          <t>1i2bwrp</t>
+        </is>
+      </c>
+      <c r="B791" t="inlineStr">
+        <is>
+          <t>first mani of the year! congrats it's a dumpster fire</t>
+        </is>
+      </c>
+      <c r="C791" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2bwrp</t>
+        </is>
+      </c>
+    </row>
+    <row r="792">
+      <c r="A792" t="inlineStr">
+        <is>
+          <t>1i2bi28</t>
+        </is>
+      </c>
+      <c r="B792" t="inlineStr">
+        <is>
+          <t>Why does the 100% acetone I get from Sally or the drugstore not work as well as salon acetone? Is it user error? If not, where do you get the real deal?</t>
+        </is>
+      </c>
+      <c r="C792" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i2bi28/why_does_the_100_acetone_i_get_from_sally_or_the/</t>
+        </is>
+      </c>
+    </row>
+    <row r="793">
+      <c r="A793" t="inlineStr">
+        <is>
+          <t>1i2badb</t>
+        </is>
+      </c>
+      <c r="B793" t="inlineStr">
+        <is>
+          <t>A brown blue look 💙🟫</t>
+        </is>
+      </c>
+      <c r="C793" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2badb</t>
+        </is>
+      </c>
+    </row>
+    <row r="794">
+      <c r="A794" t="inlineStr">
+        <is>
+          <t>1i2ag0c</t>
+        </is>
+      </c>
+      <c r="B794" t="inlineStr">
+        <is>
+          <t>Help looking for a specific lavender jelly colour?</t>
+        </is>
+      </c>
+      <c r="C794" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i2ag0c/help_looking_for_a_specific_lavender_jelly_colour/</t>
+        </is>
+      </c>
+    </row>
+    <row r="795">
+      <c r="A795" t="inlineStr">
+        <is>
+          <t>1i2aes5</t>
+        </is>
+      </c>
+      <c r="B795" t="inlineStr">
+        <is>
+          <t>What should I purchase from KBShimmer in my upcoming order??</t>
+        </is>
+      </c>
+      <c r="C795" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i2aes5/what_should_i_purchase_from_kbshimmer_in_my/</t>
+        </is>
+      </c>
+    </row>
+    <row r="796">
+      <c r="A796" t="inlineStr">
+        <is>
+          <t>1i29xhp</t>
+        </is>
+      </c>
+      <c r="B796" t="inlineStr">
+        <is>
+          <t xml:space="preserve">PFD &amp; SAMMICH ON RING </t>
+        </is>
+      </c>
+      <c r="C796" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/4okzyc7ej8de1</t>
+        </is>
+      </c>
+    </row>
+    <row r="797">
+      <c r="A797" t="inlineStr">
+        <is>
+          <t>1i29w8e</t>
+        </is>
+      </c>
+      <c r="B797" t="inlineStr">
+        <is>
+          <t>A bluer mermaid bait?</t>
+        </is>
+      </c>
+      <c r="C797" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pl5omqi9j8de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="798">
+      <c r="A798" t="inlineStr">
+        <is>
+          <t>1i28w04</t>
+        </is>
+      </c>
+      <c r="B798" t="inlineStr">
+        <is>
+          <t>LA Polish Donations</t>
+        </is>
+      </c>
+      <c r="C798" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i28w04/la_polish_donations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="799">
+      <c r="A799" t="inlineStr">
+        <is>
+          <t>1i28vj0</t>
+        </is>
+      </c>
+      <c r="B799" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Emily de Molly - 4 Hours </t>
+        </is>
+      </c>
+      <c r="C799" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i28vj0</t>
+        </is>
+      </c>
+    </row>
+    <row r="800">
+      <c r="A800" t="inlineStr">
+        <is>
+          <t>1i28oxi</t>
+        </is>
+      </c>
+      <c r="B800" t="inlineStr">
+        <is>
+          <t>Mooncat Triceratops (matte and glossy)</t>
+        </is>
+      </c>
+      <c r="C800" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tzvd593x98de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="801">
+      <c r="A801" t="inlineStr">
+        <is>
+          <t>1i28loj</t>
+        </is>
+      </c>
+      <c r="B801" t="inlineStr">
+        <is>
+          <t>Her name is Faun, but it should be Shiny New Penny</t>
+        </is>
+      </c>
+      <c r="C801" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i28loj</t>
+        </is>
+      </c>
+    </row>
+    <row r="802">
+      <c r="A802" t="inlineStr">
+        <is>
+          <t>1i28chi</t>
+        </is>
+      </c>
+      <c r="B802" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ILNP 30# Horseshoe Magnets Restocked! 🧲 </t>
+        </is>
+      </c>
+      <c r="C802" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sb55a65778de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="803">
+      <c r="A803" t="inlineStr">
+        <is>
+          <t>1i28bw3</t>
+        </is>
+      </c>
+      <c r="B803" t="inlineStr">
+        <is>
+          <t>My SO found polishes he hid away to give me in roughly 2018-2019 (fun time capsule)</t>
+        </is>
+      </c>
+      <c r="C803" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/du44fp9278de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="804">
+      <c r="A804" t="inlineStr">
+        <is>
+          <t>1i27z0l</t>
+        </is>
+      </c>
+      <c r="B804" t="inlineStr">
+        <is>
+          <t>I hate how sharp the edges of my nails feel when not polished (after edge wear). Is there anything I can do that isn't more polish?</t>
+        </is>
+      </c>
+      <c r="C804" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i27z0l/i_hate_how_sharp_the_edges_of_my_nails_feel_when/</t>
+        </is>
+      </c>
+    </row>
+    <row r="805">
+      <c r="A805" t="inlineStr">
+        <is>
+          <t>1i26qac</t>
+        </is>
+      </c>
+      <c r="B805" t="inlineStr">
+        <is>
+          <t>Ummm ok After Hours!!!</t>
+        </is>
+      </c>
+      <c r="C805" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/2lh1d4cnu7de1</t>
+        </is>
+      </c>
+    </row>
+    <row r="806">
+      <c r="A806" t="inlineStr">
+        <is>
+          <t>1i26kwn</t>
+        </is>
+      </c>
+      <c r="B806" t="inlineStr">
+        <is>
+          <t>Its like a favorite pair of jeans but on my nails ✨</t>
+        </is>
+      </c>
+      <c r="C806" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i26kwn</t>
+        </is>
+      </c>
+    </row>
+    <row r="807">
+      <c r="A807" t="inlineStr">
+        <is>
+          <t>1i26gt9</t>
+        </is>
+      </c>
+      <c r="B807" t="inlineStr">
+        <is>
+          <t>THIS IS SO DANG CUTE! Cardcaptor Sakura-themed polish included a mini clow card 😭</t>
+        </is>
+      </c>
+      <c r="C807" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i26gt9</t>
+        </is>
+      </c>
+    </row>
+    <row r="808">
+      <c r="A808" t="inlineStr">
+        <is>
+          <t>1i25tym</t>
+        </is>
+      </c>
+      <c r="B808" t="inlineStr">
+        <is>
+          <t>ILNP - Grapevine</t>
+        </is>
+      </c>
+      <c r="C808" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i25tym</t>
+        </is>
+      </c>
+    </row>
+    <row r="809">
+      <c r="A809" t="inlineStr">
+        <is>
+          <t>1i25f44</t>
+        </is>
+      </c>
+      <c r="B809" t="inlineStr">
+        <is>
+          <t>I couldn't stop looking at my nails 💙🦋</t>
+        </is>
+      </c>
+      <c r="C809" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ysjl6nzjk7de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="810">
+      <c r="A810" t="inlineStr">
+        <is>
+          <t>1i2541a</t>
+        </is>
+      </c>
+      <c r="B810" t="inlineStr">
+        <is>
+          <t>Winter Fire 🔥🕯️</t>
+        </is>
+      </c>
+      <c r="C810" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m56u0apci7de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="811">
+      <c r="A811" t="inlineStr">
+        <is>
+          <t>1i241d5</t>
+        </is>
+      </c>
+      <c r="B811" t="inlineStr">
+        <is>
+          <t>Glass Ceiling + Illusion = Absolute Magic</t>
+        </is>
+      </c>
+      <c r="C811" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/zjj96s58a7de1</t>
+        </is>
+      </c>
+    </row>
+    <row r="812">
+      <c r="A812" t="inlineStr">
+        <is>
+          <t>1i23ydg</t>
+        </is>
+      </c>
+      <c r="B812" t="inlineStr">
+        <is>
+          <t>G&amp;G Told ya I wasn't FULL vs HT Chameleon Coat?</t>
+        </is>
+      </c>
+      <c r="C812" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i23ydg/gg_told_ya_i_wasnt_full_vs_ht_chameleon_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="813">
+      <c r="A813" t="inlineStr">
+        <is>
+          <t>1i23m72</t>
+        </is>
+      </c>
+      <c r="B813" t="inlineStr">
+        <is>
+          <t>Heavy nail curve?</t>
+        </is>
+      </c>
+      <c r="C813" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i23m72</t>
+        </is>
+      </c>
+    </row>
+    <row r="814">
+      <c r="A814" t="inlineStr">
+        <is>
+          <t>1i22q3e</t>
+        </is>
+      </c>
+      <c r="B814" t="inlineStr">
+        <is>
+          <t>Sparking magic 🪄</t>
+        </is>
+      </c>
+      <c r="C814" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fylbvcib07de1.gif</t>
+        </is>
+      </c>
+    </row>
+    <row r="815">
+      <c r="A815" t="inlineStr">
+        <is>
+          <t>1i21s9w</t>
+        </is>
+      </c>
+      <c r="B815" t="inlineStr">
+        <is>
+          <t>I know y’all love a Blurple shift</t>
+        </is>
+      </c>
+      <c r="C815" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qxn35k9ft6de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="816">
+      <c r="A816" t="inlineStr">
+        <is>
+          <t>1i21rmx</t>
+        </is>
+      </c>
+      <c r="B816" t="inlineStr">
+        <is>
+          <t>Brand Brag Thread</t>
+        </is>
+      </c>
+      <c r="C816" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i21rmx/brand_brag_thread/</t>
+        </is>
+      </c>
+    </row>
+    <row r="817">
+      <c r="A817" t="inlineStr">
+        <is>
+          <t>1i21qaw</t>
+        </is>
+      </c>
+      <c r="B817" t="inlineStr">
+        <is>
+          <t>Foggy and rainy morning? No problem!</t>
+        </is>
+      </c>
+      <c r="C817" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i21qaw</t>
+        </is>
+      </c>
+    </row>
+    <row r="818">
+      <c r="A818" t="inlineStr">
+        <is>
+          <t>1i21mnc</t>
+        </is>
+      </c>
+      <c r="B818" t="inlineStr">
+        <is>
+          <t>Why does my chrome look glittery and not chrome?</t>
+        </is>
+      </c>
+      <c r="C818" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i21mnc</t>
+        </is>
+      </c>
+    </row>
+    <row r="819">
+      <c r="A819" t="inlineStr">
+        <is>
+          <t>1i21fa0</t>
+        </is>
+      </c>
+      <c r="B819" t="inlineStr">
+        <is>
+          <t>Stunned by Norpsilocin</t>
+        </is>
+      </c>
+      <c r="C819" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/6a4jl4inq6de1</t>
+        </is>
+      </c>
+    </row>
+    <row r="820">
+      <c r="A820" t="inlineStr">
+        <is>
+          <t>1i2125a</t>
+        </is>
+      </c>
+      <c r="B820" t="inlineStr">
+        <is>
+          <t>Yeah so like, this polish really is the best ever</t>
+        </is>
+      </c>
+      <c r="C820" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/q72iehdsn6de1</t>
+        </is>
+      </c>
+    </row>
+    <row r="821">
+      <c r="A821" t="inlineStr">
+        <is>
+          <t>1i202pf</t>
+        </is>
+      </c>
+      <c r="B821" t="inlineStr">
+        <is>
+          <t>Has anyone used these silicone tips for an oil soak?</t>
+        </is>
+      </c>
+      <c r="C821" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6b0syn95g6de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="822">
+      <c r="A822" t="inlineStr">
+        <is>
+          <t>1i1xcus</t>
+        </is>
+      </c>
+      <c r="B822" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Magnetic skittles </t>
+        </is>
+      </c>
+      <c r="C822" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h951lac6t5de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="823">
+      <c r="A823" t="inlineStr">
+        <is>
+          <t>1i1x7cm</t>
+        </is>
+      </c>
+      <c r="B823" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Second attempt at ombré </t>
+        </is>
+      </c>
+      <c r="C823" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uin2jrepr5de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="824">
+      <c r="A824" t="inlineStr">
+        <is>
+          <t>1i1wgx2</t>
+        </is>
+      </c>
+      <c r="B824" t="inlineStr">
+        <is>
+          <t>Anyone else having this problem?</t>
+        </is>
+      </c>
+      <c r="C824" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h2hr2q8dk5de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="825">
+      <c r="A825" t="inlineStr">
+        <is>
+          <t>1i1wdx9</t>
+        </is>
+      </c>
+      <c r="B825" t="inlineStr">
+        <is>
+          <t>🩵Turquoise🩵</t>
+        </is>
+      </c>
+      <c r="C825" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1wdx9</t>
+        </is>
+      </c>
+    </row>
+    <row r="826">
+      <c r="A826" t="inlineStr">
+        <is>
+          <t>1i1wclw</t>
+        </is>
+      </c>
+      <c r="B826" t="inlineStr">
+        <is>
+          <t>Swatch request: Hot Syrup, Iscreamnails</t>
+        </is>
+      </c>
+      <c r="C826" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i1wclw/swatch_request_hot_syrup_iscreamnails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="827">
+      <c r="A827" t="inlineStr">
+        <is>
+          <t>1i1v5tm</t>
+        </is>
+      </c>
+      <c r="B827" t="inlineStr">
+        <is>
+          <t>My first post here - some of the oldies in my stash!</t>
+        </is>
+      </c>
+      <c r="C827" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i1v5tm/my_first_post_here_some_of_the_oldies_in_my_stash/</t>
+        </is>
+      </c>
+    </row>
+    <row r="828">
+      <c r="A828" t="inlineStr">
+        <is>
+          <t>1i1tw9l</t>
+        </is>
+      </c>
+      <c r="B828" t="inlineStr">
+        <is>
+          <t>Love this vampy red! Perfect for office and outside</t>
+        </is>
+      </c>
+      <c r="C828" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/plqsrh01o4de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="829">
+      <c r="A829" t="inlineStr">
+        <is>
+          <t>1i1kgla</t>
+        </is>
+      </c>
+      <c r="B829" t="inlineStr">
+        <is>
+          <t>Dam polish tat</t>
+        </is>
+      </c>
+      <c r="C829" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i1kgla/dam_polish_tat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="830">
+      <c r="A830" t="inlineStr">
+        <is>
+          <t>1i1lkw6</t>
+        </is>
+      </c>
+      <c r="B830" t="inlineStr">
+        <is>
+          <t>Are Helios Luminor colors identified by the stamp on the bottom of the bottle?</t>
+        </is>
+      </c>
+      <c r="C830" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1lkw6</t>
+        </is>
+      </c>
+    </row>
+    <row r="831">
+      <c r="A831" t="inlineStr">
+        <is>
+          <t>1i1neo9</t>
+        </is>
+      </c>
+      <c r="B831" t="inlineStr">
+        <is>
+          <t>BEST RED</t>
+        </is>
+      </c>
+      <c r="C831" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i1neo9/best_red/</t>
+        </is>
+      </c>
+    </row>
+    <row r="832">
+      <c r="A832" t="inlineStr">
+        <is>
+          <t>1i1pktt</t>
+        </is>
+      </c>
+      <c r="B832" t="inlineStr">
+        <is>
+          <t xml:space="preserve">dents in gel nails </t>
+        </is>
+      </c>
+      <c r="C832" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i1pktt/dents_in_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="833">
+      <c r="A833" t="inlineStr">
+        <is>
+          <t>1i1sy1b</t>
+        </is>
+      </c>
+      <c r="B833" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I'm obsessed </t>
+        </is>
+      </c>
+      <c r="C833" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1sy1b</t>
+        </is>
+      </c>
+    </row>
+    <row r="834">
+      <c r="A834" t="inlineStr">
+        <is>
+          <t>1i2j3jc</t>
+        </is>
+      </c>
+      <c r="B834" t="inlineStr">
+        <is>
+          <t>January 💙</t>
+        </is>
+      </c>
+      <c r="C834" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z142sdvpyade1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="835">
+      <c r="A835" t="inlineStr">
+        <is>
+          <t>1i2fgap</t>
+        </is>
+      </c>
+      <c r="B835" t="inlineStr">
+        <is>
+          <t>First post here</t>
+        </is>
+      </c>
+      <c r="C835" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fgik5qlmv9de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="836">
+      <c r="A836" t="inlineStr">
+        <is>
+          <t>1i2dyw0</t>
+        </is>
+      </c>
+      <c r="B836" t="inlineStr">
+        <is>
+          <t>Nails for the week</t>
+        </is>
+      </c>
+      <c r="C836" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y1vzckn5i9de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="837">
+      <c r="A837" t="inlineStr">
+        <is>
+          <t>1i2d5dg</t>
+        </is>
+      </c>
+      <c r="B837" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Queen jewels </t>
+        </is>
+      </c>
+      <c r="C837" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2d5dg</t>
+        </is>
+      </c>
+    </row>
+    <row r="838">
+      <c r="A838" t="inlineStr">
+        <is>
+          <t>1i2ccxw</t>
+        </is>
+      </c>
+      <c r="B838" t="inlineStr">
+        <is>
+          <t>Strawberry nail set 🍓</t>
+        </is>
+      </c>
+      <c r="C838" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2ccxw</t>
+        </is>
+      </c>
+    </row>
+    <row r="839">
+      <c r="A839" t="inlineStr">
+        <is>
+          <t>1i2a4nk</t>
+        </is>
+      </c>
+      <c r="B839" t="inlineStr">
+        <is>
+          <t>Blooming gel - 1st attempt ever</t>
+        </is>
+      </c>
+      <c r="C839" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2a4nk</t>
+        </is>
+      </c>
+    </row>
+    <row r="840">
+      <c r="A840" t="inlineStr">
+        <is>
+          <t>1i2a1xe</t>
+        </is>
+      </c>
+      <c r="B840" t="inlineStr">
+        <is>
+          <t>Butterfly nails</t>
+        </is>
+      </c>
+      <c r="C840" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x1equxkjk8de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="841">
+      <c r="A841" t="inlineStr">
+        <is>
+          <t>1i286xn</t>
+        </is>
+      </c>
+      <c r="B841" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Working on a new set! </t>
+        </is>
+      </c>
+      <c r="C841" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i286xn</t>
+        </is>
+      </c>
+    </row>
+    <row r="842">
+      <c r="A842" t="inlineStr">
+        <is>
+          <t>1i23zhs</t>
+        </is>
+      </c>
+      <c r="B842" t="inlineStr">
+        <is>
+          <t>VALENTINES DAY SET ⟡ ݁₊ .</t>
+        </is>
+      </c>
+      <c r="C842" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i23zhs</t>
+        </is>
+      </c>
+    </row>
+    <row r="843">
+      <c r="A843" t="inlineStr">
+        <is>
+          <t>1i22rh1</t>
+        </is>
+      </c>
+      <c r="B843" t="inlineStr">
+        <is>
+          <t>Rate my progress/tips or critiques</t>
+        </is>
+      </c>
+      <c r="C843" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i22rh1</t>
+        </is>
+      </c>
+    </row>
+    <row r="844">
+      <c r="A844" t="inlineStr">
+        <is>
+          <t>1i22jym</t>
+        </is>
+      </c>
+      <c r="B844" t="inlineStr">
+        <is>
+          <t>How to recreate this look</t>
+        </is>
+      </c>
+      <c r="C844" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1i22jym/how_to_recreate_this_look/</t>
+        </is>
+      </c>
+    </row>
+    <row r="845">
+      <c r="A845" t="inlineStr">
+        <is>
+          <t>1i21zrf</t>
+        </is>
+      </c>
+      <c r="B845" t="inlineStr">
+        <is>
+          <t>Edgy Barbie</t>
+        </is>
+      </c>
+      <c r="C845" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1i21zrf/edgy_barbie/</t>
+        </is>
+      </c>
+    </row>
+    <row r="846">
+      <c r="A846" t="inlineStr">
+        <is>
+          <t>1i217e2</t>
+        </is>
+      </c>
+      <c r="B846" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Recent 3D nail art </t>
+        </is>
+      </c>
+      <c r="C846" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i217e2</t>
+        </is>
+      </c>
+    </row>
+    <row r="847">
+      <c r="A847" t="inlineStr">
+        <is>
+          <t>1i20qdr</t>
+        </is>
+      </c>
+      <c r="B847" t="inlineStr">
+        <is>
+          <t xml:space="preserve">In a scale of 1-10 how much you give for this design? </t>
+        </is>
+      </c>
+      <c r="C847" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w5ttgr9bl6de1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="848">
+      <c r="A848" t="inlineStr">
+        <is>
+          <t>1i1wy3i</t>
+        </is>
+      </c>
+      <c r="B848" t="inlineStr">
+        <is>
+          <t>Beginner set</t>
+        </is>
+      </c>
+      <c r="C848" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i1wy3i</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Fri Jan 17 08:10:26 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_01_19.xlsx
+++ b/data/collected_data/2025_01_19.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C848"/>
+  <dimension ref="A1:C1052"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14851,6 +14851,3474 @@
         </is>
       </c>
     </row>
+    <row r="849">
+      <c r="A849" t="inlineStr">
+        <is>
+          <t>1i3bnk2</t>
+        </is>
+      </c>
+      <c r="B849" t="inlineStr">
+        <is>
+          <t>first character nails!</t>
+        </is>
+      </c>
+      <c r="C849" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3bnk2</t>
+        </is>
+      </c>
+    </row>
+    <row r="850">
+      <c r="A850" t="inlineStr">
+        <is>
+          <t>1i3b9em</t>
+        </is>
+      </c>
+      <c r="B850" t="inlineStr">
+        <is>
+          <t>Ready for my birthday</t>
+        </is>
+      </c>
+      <c r="C850" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lyhouf0tcide1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="851">
+      <c r="A851" t="inlineStr">
+        <is>
+          <t>1i3araq</t>
+        </is>
+      </c>
+      <c r="B851" t="inlineStr">
+        <is>
+          <t>Chartreuse and ume blossoms for the new year</t>
+        </is>
+      </c>
+      <c r="C851" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0m9obly16ide1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" t="inlineStr">
+        <is>
+          <t>1i3alte</t>
+        </is>
+      </c>
+      <c r="B852" t="inlineStr">
+        <is>
+          <t>First time getting my nails done💅🏻✨</t>
+        </is>
+      </c>
+      <c r="C852" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cqt973134ide1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" t="inlineStr">
+        <is>
+          <t>1i3aa9d</t>
+        </is>
+      </c>
+      <c r="B853" t="inlineStr">
+        <is>
+          <t>Natural French Tips</t>
+        </is>
+      </c>
+      <c r="C853" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/a5eyvq1uzhde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" t="inlineStr">
+        <is>
+          <t>1i39vrc</t>
+        </is>
+      </c>
+      <c r="B854" t="inlineStr">
+        <is>
+          <t>in love with my new nails! but....</t>
+        </is>
+      </c>
+      <c r="C854" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i39vrc</t>
+        </is>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" t="inlineStr">
+        <is>
+          <t>1i38x0m</t>
+        </is>
+      </c>
+      <c r="B855" t="inlineStr">
+        <is>
+          <t>IG @ra3creat3s 💅🏼</t>
+        </is>
+      </c>
+      <c r="C855" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i38x0m</t>
+        </is>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" t="inlineStr">
+        <is>
+          <t>1i39h0k</t>
+        </is>
+      </c>
+      <c r="B856" t="inlineStr">
+        <is>
+          <t>Nails selected by potential bf</t>
+        </is>
+      </c>
+      <c r="C856" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7nhb4z1cqhde1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" t="inlineStr">
+        <is>
+          <t>1i39d2i</t>
+        </is>
+      </c>
+      <c r="B857" t="inlineStr">
+        <is>
+          <t>light pink acrylics turning brown-ish</t>
+        </is>
+      </c>
+      <c r="C857" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i39d2i/light_pink_acrylics_turning_brownish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" t="inlineStr">
+        <is>
+          <t>1i394kg</t>
+        </is>
+      </c>
+      <c r="B858" t="inlineStr">
+        <is>
+          <t>Fav set I've done so far</t>
+        </is>
+      </c>
+      <c r="C858" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i394kg</t>
+        </is>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" t="inlineStr">
+        <is>
+          <t>1i391fx</t>
+        </is>
+      </c>
+      <c r="B859" t="inlineStr">
+        <is>
+          <t>Kaws set</t>
+        </is>
+      </c>
+      <c r="C859" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i391fx</t>
+        </is>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" t="inlineStr">
+        <is>
+          <t>1i36gmf</t>
+        </is>
+      </c>
+      <c r="B860" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Polish help </t>
+        </is>
+      </c>
+      <c r="C860" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eooxd1zzvgde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" t="inlineStr">
+        <is>
+          <t>1i38ukl</t>
+        </is>
+      </c>
+      <c r="B861" t="inlineStr">
+        <is>
+          <t>i wanted something plain but funky , been embracing pink lately as an “i only wear black” girly :) 🩷🖤⭐️</t>
+        </is>
+      </c>
+      <c r="C861" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i38ukl</t>
+        </is>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" t="inlineStr">
+        <is>
+          <t>1i383nf</t>
+        </is>
+      </c>
+      <c r="B862" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Need color suggestions for black and gold dress </t>
+        </is>
+      </c>
+      <c r="C862" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v5er5q6xbhde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" t="inlineStr">
+        <is>
+          <t>1i37r1o</t>
+        </is>
+      </c>
+      <c r="B863" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can I use regular “super glue” on these soft tips? </t>
+        </is>
+      </c>
+      <c r="C863" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7isff9me8hde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" t="inlineStr">
+        <is>
+          <t>1i36r5f</t>
+        </is>
+      </c>
+      <c r="B864" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Birthday nails!! 💅🏼 </t>
+        </is>
+      </c>
+      <c r="C864" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i36r5f</t>
+        </is>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" t="inlineStr">
+        <is>
+          <t>1i36ptj</t>
+        </is>
+      </c>
+      <c r="B865" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Opinions? </t>
+        </is>
+      </c>
+      <c r="C865" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i36ptj/opinions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" t="inlineStr">
+        <is>
+          <t>1i36l3c</t>
+        </is>
+      </c>
+      <c r="B866" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Gel X Nails </t>
+        </is>
+      </c>
+      <c r="C866" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i36l3c/gel_x_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" t="inlineStr">
+        <is>
+          <t>1i36jrq</t>
+        </is>
+      </c>
+      <c r="B867" t="inlineStr">
+        <is>
+          <t>Recommendations for extra short press on nails- short &amp; wide nail beds</t>
+        </is>
+      </c>
+      <c r="C867" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9dg1knjtwgde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" t="inlineStr">
+        <is>
+          <t>1i36dx4</t>
+        </is>
+      </c>
+      <c r="B868" t="inlineStr">
+        <is>
+          <t>NEUTRAL CHIC</t>
+        </is>
+      </c>
+      <c r="C868" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/c6mtrw4avgde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" t="inlineStr">
+        <is>
+          <t>1i35tcz</t>
+        </is>
+      </c>
+      <c r="B869" t="inlineStr">
+        <is>
+          <t>First Nails of the Year</t>
+        </is>
+      </c>
+      <c r="C869" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i35tcz</t>
+        </is>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" t="inlineStr">
+        <is>
+          <t>1i35qc1</t>
+        </is>
+      </c>
+      <c r="B870" t="inlineStr">
+        <is>
+          <t>Decided to get acrylics again after a long break. 🔮✨</t>
+        </is>
+      </c>
+      <c r="C870" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i35qc1</t>
+        </is>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" t="inlineStr">
+        <is>
+          <t>1i358ot</t>
+        </is>
+      </c>
+      <c r="B871" t="inlineStr">
+        <is>
+          <t>Trying to choose the best nail shape and hoping for suggestions?</t>
+        </is>
+      </c>
+      <c r="C871" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i358ot</t>
+        </is>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" t="inlineStr">
+        <is>
+          <t>1i34fso</t>
+        </is>
+      </c>
+      <c r="B872" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Purple glitter ombre </t>
+        </is>
+      </c>
+      <c r="C872" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i34fso</t>
+        </is>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" t="inlineStr">
+        <is>
+          <t>1i352br</t>
+        </is>
+      </c>
+      <c r="B873" t="inlineStr">
+        <is>
+          <t>My nail tech gave me the best nails I’ve ever had yesterday!</t>
+        </is>
+      </c>
+      <c r="C873" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kw519794jgde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" t="inlineStr">
+        <is>
+          <t>1i351ro</t>
+        </is>
+      </c>
+      <c r="B874" t="inlineStr">
+        <is>
+          <t>nails ready to go to the beach</t>
+        </is>
+      </c>
+      <c r="C874" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i351ro</t>
+        </is>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" t="inlineStr">
+        <is>
+          <t>1i34qv9</t>
+        </is>
+      </c>
+      <c r="B875" t="inlineStr">
+        <is>
+          <t>doing my nails is always a days long project</t>
+        </is>
+      </c>
+      <c r="C875" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i34qv9</t>
+        </is>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" t="inlineStr">
+        <is>
+          <t>1i34oea</t>
+        </is>
+      </c>
+      <c r="B876" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How about this design? </t>
+        </is>
+      </c>
+      <c r="C876" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3x17xsxnfgde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" t="inlineStr">
+        <is>
+          <t>1i34n66</t>
+        </is>
+      </c>
+      <c r="B877" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Painting a Creature Commandos Nails Set 💕 Starting with "The Bride" </t>
+        </is>
+      </c>
+      <c r="C877" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/an6jcl1cfgde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" t="inlineStr">
+        <is>
+          <t>1i33sfl</t>
+        </is>
+      </c>
+      <c r="B878" t="inlineStr">
+        <is>
+          <t xml:space="preserve">nail curing question </t>
+        </is>
+      </c>
+      <c r="C878" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i33sfl/nail_curing_question/</t>
+        </is>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" t="inlineStr">
+        <is>
+          <t>1i33pto</t>
+        </is>
+      </c>
+      <c r="B879" t="inlineStr">
+        <is>
+          <t>Birthday Naillsss</t>
+        </is>
+      </c>
+      <c r="C879" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ktwtdog97gde1</t>
+        </is>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" t="inlineStr">
+        <is>
+          <t>1i33nid</t>
+        </is>
+      </c>
+      <c r="B880" t="inlineStr">
+        <is>
+          <t>First set of the new year!  🔥</t>
+        </is>
+      </c>
+      <c r="C880" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/715ezoxp6gde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" t="inlineStr">
+        <is>
+          <t>1i33iov</t>
+        </is>
+      </c>
+      <c r="B881" t="inlineStr">
+        <is>
+          <t>First time getting gel acrylics, thoughts?</t>
+        </is>
+      </c>
+      <c r="C881" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m91ltubj5gde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" t="inlineStr">
+        <is>
+          <t>1i33eu1</t>
+        </is>
+      </c>
+      <c r="B882" t="inlineStr">
+        <is>
+          <t>some of my work recently:)</t>
+        </is>
+      </c>
+      <c r="C882" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i33eu1</t>
+        </is>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" t="inlineStr">
+        <is>
+          <t>1i334ke</t>
+        </is>
+      </c>
+      <c r="B883" t="inlineStr">
+        <is>
+          <t>Beginner here can you tell me what can fix. I need criticism</t>
+        </is>
+      </c>
+      <c r="C883" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/60cmxz362gde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" t="inlineStr">
+        <is>
+          <t>1i337do</t>
+        </is>
+      </c>
+      <c r="B884" t="inlineStr">
+        <is>
+          <t>How to recreate pink glass nails?</t>
+        </is>
+      </c>
+      <c r="C884" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f1rdmbgw2gde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" t="inlineStr">
+        <is>
+          <t>1i32q8u</t>
+        </is>
+      </c>
+      <c r="B885" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This is a design with Turkish eyes, with the effect of melted. How Dali watches </t>
+        </is>
+      </c>
+      <c r="C885" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tglned9vyfde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" t="inlineStr">
+        <is>
+          <t>1i32oz6</t>
+        </is>
+      </c>
+      <c r="B886" t="inlineStr">
+        <is>
+          <t>How can I improve this without buying the pearls?</t>
+        </is>
+      </c>
+      <c r="C886" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i32oz6</t>
+        </is>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" t="inlineStr">
+        <is>
+          <t>1i325sn</t>
+        </is>
+      </c>
+      <c r="B887" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Made for my manicurist </t>
+        </is>
+      </c>
+      <c r="C887" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/w76qnmj3ufde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" t="inlineStr">
+        <is>
+          <t>1i320t2</t>
+        </is>
+      </c>
+      <c r="B888" t="inlineStr">
+        <is>
+          <t>Nail Polish Remover</t>
+        </is>
+      </c>
+      <c r="C888" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i320t2/nail_polish_remover/</t>
+        </is>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" t="inlineStr">
+        <is>
+          <t>1i31xpg</t>
+        </is>
+      </c>
+      <c r="B889" t="inlineStr">
+        <is>
+          <t>I got them redone 🥺</t>
+        </is>
+      </c>
+      <c r="C889" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2dp9yuh8sfde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" t="inlineStr">
+        <is>
+          <t>1i30746</t>
+        </is>
+      </c>
+      <c r="B890" t="inlineStr">
+        <is>
+          <t>I think it turned out nice 💗</t>
+        </is>
+      </c>
+      <c r="C890" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i30746</t>
+        </is>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" t="inlineStr">
+        <is>
+          <t>1i31gjh</t>
+        </is>
+      </c>
+      <c r="B891" t="inlineStr">
+        <is>
+          <t>Zebra nails with charms, I’m in love!!</t>
+        </is>
+      </c>
+      <c r="C891" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/cuntkleeofde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" t="inlineStr">
+        <is>
+          <t>1i31g79</t>
+        </is>
+      </c>
+      <c r="B892" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Base coat </t>
+        </is>
+      </c>
+      <c r="C892" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i31g79/base_coat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" t="inlineStr">
+        <is>
+          <t>1i31cjy</t>
+        </is>
+      </c>
+      <c r="B893" t="inlineStr">
+        <is>
+          <t>Last Halloween</t>
+        </is>
+      </c>
+      <c r="C893" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/foeukq7hnfde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" t="inlineStr">
+        <is>
+          <t>1i315g9</t>
+        </is>
+      </c>
+      <c r="B894" t="inlineStr">
+        <is>
+          <t>Barbie Blue French nails</t>
+        </is>
+      </c>
+      <c r="C894" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zvxjieixlfde1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" t="inlineStr">
+        <is>
+          <t>1i313lq</t>
+        </is>
+      </c>
+      <c r="B895" t="inlineStr">
+        <is>
+          <t>nail care advice?</t>
+        </is>
+      </c>
+      <c r="C895" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i313lq</t>
+        </is>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" t="inlineStr">
+        <is>
+          <t>1i30ve3</t>
+        </is>
+      </c>
+      <c r="B896" t="inlineStr">
+        <is>
+          <t>January recommendation?</t>
+        </is>
+      </c>
+      <c r="C896" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i30ve3/january_recommendation/</t>
+        </is>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" t="inlineStr">
+        <is>
+          <t>1i2zt6s</t>
+        </is>
+      </c>
+      <c r="B897" t="inlineStr">
+        <is>
+          <t>Adding to the chrome collection with gel X from a nail salon $80 🫠💕</t>
+        </is>
+      </c>
+      <c r="C897" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/d5ttr2ucbfde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" t="inlineStr">
+        <is>
+          <t>1i2z475</t>
+        </is>
+      </c>
+      <c r="B898" t="inlineStr">
+        <is>
+          <t xml:space="preserve">full tips for nail recovery </t>
+        </is>
+      </c>
+      <c r="C898" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i2z475/full_tips_for_nail_recovery/</t>
+        </is>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" t="inlineStr">
+        <is>
+          <t>1i2zlgi</t>
+        </is>
+      </c>
+      <c r="B899" t="inlineStr">
+        <is>
+          <t>🩵🩷 Wintery Skittle 🩶🤍 ❄️Playing around with some of my icy winter shades. Index - ILNP Snow Angel. Middle - ILNP Sled Day. Ring - ILNP Rosewater. Thumb and pinky - Rogue Laquer Snow Be It. All topped with ILNP Spotlight ✨</t>
+        </is>
+      </c>
+      <c r="C899" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2zlgi</t>
+        </is>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" t="inlineStr">
+        <is>
+          <t>1i2z1ym</t>
+        </is>
+      </c>
+      <c r="B900" t="inlineStr">
+        <is>
+          <t>Brown “cat eye”</t>
+        </is>
+      </c>
+      <c r="C900" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2z1ym</t>
+        </is>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" t="inlineStr">
+        <is>
+          <t>1i2xll9</t>
+        </is>
+      </c>
+      <c r="B901" t="inlineStr">
+        <is>
+          <t>Are these too grown out/can I get away with these nails for another 10-days while on vacation?</t>
+        </is>
+      </c>
+      <c r="C901" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rp2feakeuede1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" t="inlineStr">
+        <is>
+          <t>1i2ygsx</t>
+        </is>
+      </c>
+      <c r="B902" t="inlineStr">
+        <is>
+          <t>$5 Press ons from Amazon</t>
+        </is>
+      </c>
+      <c r="C902" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hyy00dpz0fde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" t="inlineStr">
+        <is>
+          <t>1i2yqwj</t>
+        </is>
+      </c>
+      <c r="B903" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My nail beds are changing shape  </t>
+        </is>
+      </c>
+      <c r="C903" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/232pawv43fde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" t="inlineStr">
+        <is>
+          <t>1i2ywr9</t>
+        </is>
+      </c>
+      <c r="B904" t="inlineStr">
+        <is>
+          <t>My first at-home magnetic gel mani</t>
+        </is>
+      </c>
+      <c r="C904" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/iq6r6kdd4fde1</t>
+        </is>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" t="inlineStr">
+        <is>
+          <t>1i2yc9u</t>
+        </is>
+      </c>
+      <c r="B905" t="inlineStr">
+        <is>
+          <t>Found myself a new nail tech!</t>
+        </is>
+      </c>
+      <c r="C905" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2yc9u</t>
+        </is>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" t="inlineStr">
+        <is>
+          <t>1i2y87h</t>
+        </is>
+      </c>
+      <c r="B906" t="inlineStr">
+        <is>
+          <t>Vday mani💌</t>
+        </is>
+      </c>
+      <c r="C906" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2y87h</t>
+        </is>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" t="inlineStr">
+        <is>
+          <t>1i2y5tu</t>
+        </is>
+      </c>
+      <c r="B907" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What causes gel polish to crinkle up? </t>
+        </is>
+      </c>
+      <c r="C907" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1d5g96bnyede1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" t="inlineStr">
+        <is>
+          <t>1i2xqfv</t>
+        </is>
+      </c>
+      <c r="B908" t="inlineStr">
+        <is>
+          <t>New icy set ❄️💙</t>
+        </is>
+      </c>
+      <c r="C908" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/sa24ig1gvede1</t>
+        </is>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" t="inlineStr">
+        <is>
+          <t>1i2x10f</t>
+        </is>
+      </c>
+      <c r="B909" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What shape anf nail color(s) would suit me? </t>
+        </is>
+      </c>
+      <c r="C909" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kqh3bbv2qede1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" t="inlineStr">
+        <is>
+          <t>1i2wu7g</t>
+        </is>
+      </c>
+      <c r="B910" t="inlineStr">
+        <is>
+          <t>Product suggestion for "well used" nails</t>
+        </is>
+      </c>
+      <c r="C910" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i2wu7g/product_suggestion_for_well_used_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" t="inlineStr">
+        <is>
+          <t>1i2wqt0</t>
+        </is>
+      </c>
+      <c r="B911" t="inlineStr">
+        <is>
+          <t>Trying to remove acrylics but the nail tips aren't going anywhere. Any tips???</t>
+        </is>
+      </c>
+      <c r="C911" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i2wqt0/trying_to_remove_acrylics_but_the_nail_tips_arent/</t>
+        </is>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" t="inlineStr">
+        <is>
+          <t>1i2w1nu</t>
+        </is>
+      </c>
+      <c r="B912" t="inlineStr">
+        <is>
+          <t>Tips lifting from natural nail</t>
+        </is>
+      </c>
+      <c r="C912" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2w1nu</t>
+        </is>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" t="inlineStr">
+        <is>
+          <t>1i2vy2z</t>
+        </is>
+      </c>
+      <c r="B913" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nail care help! </t>
+        </is>
+      </c>
+      <c r="C913" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i2vy2z/nail_care_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" t="inlineStr">
+        <is>
+          <t>1i2vtea</t>
+        </is>
+      </c>
+      <c r="B914" t="inlineStr">
+        <is>
+          <t>Lady butchered my nails so I had to fix them myself</t>
+        </is>
+      </c>
+      <c r="C914" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2vtea</t>
+        </is>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" t="inlineStr">
+        <is>
+          <t>1i2vrkn</t>
+        </is>
+      </c>
+      <c r="B915" t="inlineStr">
+        <is>
+          <t>Cherry Blossom Nails</t>
+        </is>
+      </c>
+      <c r="C915" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oxiwqmmigede1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" t="inlineStr">
+        <is>
+          <t>1i2tvix</t>
+        </is>
+      </c>
+      <c r="B916" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tips welcome to improve </t>
+        </is>
+      </c>
+      <c r="C916" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q6bit6qg2ede1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" t="inlineStr">
+        <is>
+          <t>1i2iehs</t>
+        </is>
+      </c>
+      <c r="B917" t="inlineStr">
+        <is>
+          <t>Help with very poor manicure…</t>
+        </is>
+      </c>
+      <c r="C917" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jeto52g9qade1</t>
+        </is>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" t="inlineStr">
+        <is>
+          <t>1i2vopr</t>
+        </is>
+      </c>
+      <c r="B918" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What shape would suit my nails best </t>
+        </is>
+      </c>
+      <c r="C918" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7nqsjehyfede1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" t="inlineStr">
+        <is>
+          <t>1i2v3s5</t>
+        </is>
+      </c>
+      <c r="B919" t="inlineStr">
+        <is>
+          <t>new nails 😍</t>
+        </is>
+      </c>
+      <c r="C919" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fy4p4qqlbede1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" t="inlineStr">
+        <is>
+          <t>1i2ustm</t>
+        </is>
+      </c>
+      <c r="B920" t="inlineStr">
+        <is>
+          <t>What do you use for an at home manicure?</t>
+        </is>
+      </c>
+      <c r="C920" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i2ustm/what_do_you_use_for_an_at_home_manicure/</t>
+        </is>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" t="inlineStr">
+        <is>
+          <t>1i2udfk</t>
+        </is>
+      </c>
+      <c r="B921" t="inlineStr">
+        <is>
+          <t>Dupes for this gel polish? (Gelcare Rosehip Oil)</t>
+        </is>
+      </c>
+      <c r="C921" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9bpdhka56ede1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" t="inlineStr">
+        <is>
+          <t>1i2u8zw</t>
+        </is>
+      </c>
+      <c r="B922" t="inlineStr">
+        <is>
+          <t>I fell in love! You can tell it by my nails</t>
+        </is>
+      </c>
+      <c r="C922" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/z902uoy35ede1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" t="inlineStr">
+        <is>
+          <t>1i2u4l2</t>
+        </is>
+      </c>
+      <c r="B923" t="inlineStr">
+        <is>
+          <t>How can I improve my nails</t>
+        </is>
+      </c>
+      <c r="C923" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m2ckjmkb4ede1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" t="inlineStr">
+        <is>
+          <t>1i2u14u</t>
+        </is>
+      </c>
+      <c r="B924" t="inlineStr">
+        <is>
+          <t>Doing my own set</t>
+        </is>
+      </c>
+      <c r="C924" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zi67k8sl3ede1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" t="inlineStr">
+        <is>
+          <t>1i2tzso</t>
+        </is>
+      </c>
+      <c r="B925" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Goth nails </t>
+        </is>
+      </c>
+      <c r="C925" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9b9tm99b3ede1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" t="inlineStr">
+        <is>
+          <t>1i2tyr2</t>
+        </is>
+      </c>
+      <c r="B926" t="inlineStr">
+        <is>
+          <t>Favorite set so far</t>
+        </is>
+      </c>
+      <c r="C926" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2tyr2</t>
+        </is>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" t="inlineStr">
+        <is>
+          <t>1i2tgsr</t>
+        </is>
+      </c>
+      <c r="B927" t="inlineStr">
+        <is>
+          <t>Clean girl aesthetic, but for an elder emo. 🖤</t>
+        </is>
+      </c>
+      <c r="C927" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2tgsr</t>
+        </is>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" t="inlineStr">
+        <is>
+          <t>1i2swhj</t>
+        </is>
+      </c>
+      <c r="B928" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Dear all of you, you have been amazed by my portfolio works. Thank you so much for your support! I really love doing this. This is another presentation of a module I have recently approved </t>
+        </is>
+      </c>
+      <c r="C928" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ekjj7ly2vdde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" t="inlineStr">
+        <is>
+          <t>1i2sv36</t>
+        </is>
+      </c>
+      <c r="B929" t="inlineStr">
+        <is>
+          <t xml:space="preserve">hand painted </t>
+        </is>
+      </c>
+      <c r="C929" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2sv36</t>
+        </is>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" t="inlineStr">
+        <is>
+          <t>1i2rtl8</t>
+        </is>
+      </c>
+      <c r="B930" t="inlineStr">
+        <is>
+          <t>Miro Inspired</t>
+        </is>
+      </c>
+      <c r="C930" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2rtl8</t>
+        </is>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" t="inlineStr">
+        <is>
+          <t>1i2r2x7</t>
+        </is>
+      </c>
+      <c r="B931" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do you deal with it when gel/acrylics start to lift off of the nail? Nail glue? </t>
+        </is>
+      </c>
+      <c r="C931" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i2r2x7/how_do_you_deal_with_it_when_gelacrylics_start_to/</t>
+        </is>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" t="inlineStr">
+        <is>
+          <t>1i2pzkt</t>
+        </is>
+      </c>
+      <c r="B932" t="inlineStr">
+        <is>
+          <t>My DIY nails. I really aimed for narrow or narrow looking nails and I had to find the hard way that nails like that cannot withstand my everyday life. Latest set (glitter/pink) was the one, sturdy, not bulky and pretty</t>
+        </is>
+      </c>
+      <c r="C932" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2pzkt</t>
+        </is>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" t="inlineStr">
+        <is>
+          <t>1i2skk9</t>
+        </is>
+      </c>
+      <c r="B933" t="inlineStr">
+        <is>
+          <t>Not bright, but stylish</t>
+        </is>
+      </c>
+      <c r="C933" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hrq8x36gsdde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" t="inlineStr">
+        <is>
+          <t>1i2rz7k</t>
+        </is>
+      </c>
+      <c r="B934" t="inlineStr">
+        <is>
+          <t>something subtle</t>
+        </is>
+      </c>
+      <c r="C934" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hgshtoa3odde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" t="inlineStr">
+        <is>
+          <t>1i2ru5s</t>
+        </is>
+      </c>
+      <c r="B935" t="inlineStr">
+        <is>
+          <t>natural🪐</t>
+        </is>
+      </c>
+      <c r="C935" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/35do76jymdde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" t="inlineStr">
+        <is>
+          <t>1i2rkan</t>
+        </is>
+      </c>
+      <c r="B936" t="inlineStr">
+        <is>
+          <t>Love the color, not so Sure about the shape, thoughts……</t>
+        </is>
+      </c>
+      <c r="C936" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x1cygmyskdde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" t="inlineStr">
+        <is>
+          <t>1i2rirp</t>
+        </is>
+      </c>
+      <c r="B937" t="inlineStr">
+        <is>
+          <t>Nintendo Switch 2 nails!!!</t>
+        </is>
+      </c>
+      <c r="C937" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2rirp</t>
+        </is>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" t="inlineStr">
+        <is>
+          <t>1i2pck8</t>
+        </is>
+      </c>
+      <c r="B938" t="inlineStr">
+        <is>
+          <t>Got new nails with hearts today ❤️</t>
+        </is>
+      </c>
+      <c r="C938" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2pck8</t>
+        </is>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" t="inlineStr">
+        <is>
+          <t>1i2p4b9</t>
+        </is>
+      </c>
+      <c r="B939" t="inlineStr">
+        <is>
+          <t>It this a bruise? Can I still do extensions?</t>
+        </is>
+      </c>
+      <c r="C939" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xr0nj0180dde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" t="inlineStr">
+        <is>
+          <t>1i2oi6m</t>
+        </is>
+      </c>
+      <c r="B940" t="inlineStr">
+        <is>
+          <t>First set of 2025💅</t>
+        </is>
+      </c>
+      <c r="C940" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7e5h7vqlucde1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" t="inlineStr">
+        <is>
+          <t>1i2o3m3</t>
+        </is>
+      </c>
+      <c r="B941" t="inlineStr">
+        <is>
+          <t>Line faces</t>
+        </is>
+      </c>
+      <c r="C941" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2o3m3</t>
+        </is>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" t="inlineStr">
+        <is>
+          <t>1i2nzg5</t>
+        </is>
+      </c>
+      <c r="B942" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My amazing nail tech smashed it as always! </t>
+        </is>
+      </c>
+      <c r="C942" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2nzg5</t>
+        </is>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" t="inlineStr">
+        <is>
+          <t>1i2ncmd</t>
+        </is>
+      </c>
+      <c r="B943" t="inlineStr">
+        <is>
+          <t>First time getting my nails done 💕💕</t>
+        </is>
+      </c>
+      <c r="C943" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/brh5h1chicde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" t="inlineStr">
+        <is>
+          <t>1i2n07v</t>
+        </is>
+      </c>
+      <c r="B944" t="inlineStr">
+        <is>
+          <t>I envy myself</t>
+        </is>
+      </c>
+      <c r="C944" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ayjoxg79ecde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" t="inlineStr">
+        <is>
+          <t>1i2lugr</t>
+        </is>
+      </c>
+      <c r="B945" t="inlineStr">
+        <is>
+          <t>started regularly taking vitamins, stopped biting my nails, the obvious difference in growth is 🤯</t>
+        </is>
+      </c>
+      <c r="C945" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2lugr</t>
+        </is>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" t="inlineStr">
+        <is>
+          <t>1i2lo01</t>
+        </is>
+      </c>
+      <c r="B946" t="inlineStr">
+        <is>
+          <t>Been working on my nuance</t>
+        </is>
+      </c>
+      <c r="C946" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2lo01</t>
+        </is>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" t="inlineStr">
+        <is>
+          <t>1i2l7y2</t>
+        </is>
+      </c>
+      <c r="B947" t="inlineStr">
+        <is>
+          <t>Pink - yay or nay?</t>
+        </is>
+      </c>
+      <c r="C947" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2l7y2</t>
+        </is>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" t="inlineStr">
+        <is>
+          <t>1i2ko0h</t>
+        </is>
+      </c>
+      <c r="B948" t="inlineStr">
+        <is>
+          <t>Can I go back if I genuinely hate them?</t>
+        </is>
+      </c>
+      <c r="C948" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2ko0h</t>
+        </is>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" t="inlineStr">
+        <is>
+          <t>1i3bi7t</t>
+        </is>
+      </c>
+      <c r="B949" t="inlineStr">
+        <is>
+          <t>Do you ever accidentally do a mismatched accent nail?</t>
+        </is>
+      </c>
+      <c r="C949" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3bi7t</t>
+        </is>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" t="inlineStr">
+        <is>
+          <t>1i3b7a5</t>
+        </is>
+      </c>
+      <c r="B950" t="inlineStr">
+        <is>
+          <t>I need a purple like the shade in this pic! A cool-toned, neon, venomous purple creme</t>
+        </is>
+      </c>
+      <c r="C950" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wvhjkcg1cide1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" t="inlineStr">
+        <is>
+          <t>1i3al8d</t>
+        </is>
+      </c>
+      <c r="B951" t="inlineStr">
+        <is>
+          <t>Horse shoe magnets: 10 lb. vs. 30 lb. pull</t>
+        </is>
+      </c>
+      <c r="C951" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1npciy0v3ide1</t>
+        </is>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" t="inlineStr">
+        <is>
+          <t>1i3aaou</t>
+        </is>
+      </c>
+      <c r="B952" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Does anybody have a 3D printer and the 30lb nail art magnet? </t>
+        </is>
+      </c>
+      <c r="C952" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i3aaou/does_anybody_have_a_3d_printer_and_the_30lb_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" t="inlineStr">
+        <is>
+          <t>1i3a45m</t>
+        </is>
+      </c>
+      <c r="B953" t="inlineStr">
+        <is>
+          <t>120 swatches later... 😅</t>
+        </is>
+      </c>
+      <c r="C953" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3a45m</t>
+        </is>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" t="inlineStr">
+        <is>
+          <t>1i39mq4</t>
+        </is>
+      </c>
+      <c r="B954" t="inlineStr">
+        <is>
+          <t>Pink-with-green-shimmer indie comparison!</t>
+        </is>
+      </c>
+      <c r="C954" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i39mq4</t>
+        </is>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" t="inlineStr">
+        <is>
+          <t>1i38qsj</t>
+        </is>
+      </c>
+      <c r="B955" t="inlineStr">
+        <is>
+          <t>Blue Velvet in honor of David Lynch 💔</t>
+        </is>
+      </c>
+      <c r="C955" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/1j8v743hihde1</t>
+        </is>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" t="inlineStr">
+        <is>
+          <t>1i38pik</t>
+        </is>
+      </c>
+      <c r="B956" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ISO dupes for lights lacquer angel baby </t>
+        </is>
+      </c>
+      <c r="C956" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i38pik</t>
+        </is>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" t="inlineStr">
+        <is>
+          <t>1i38p7u</t>
+        </is>
+      </c>
+      <c r="B957" t="inlineStr">
+        <is>
+          <t>Gel X Help</t>
+        </is>
+      </c>
+      <c r="C957" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/idluzwe3ihde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" t="inlineStr">
+        <is>
+          <t>1i38d6l</t>
+        </is>
+      </c>
+      <c r="B958" t="inlineStr">
+        <is>
+          <t>The Most Perfect Blue</t>
+        </is>
+      </c>
+      <c r="C958" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i38d6l</t>
+        </is>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" t="inlineStr">
+        <is>
+          <t>1i380iz</t>
+        </is>
+      </c>
+      <c r="B959" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Loving this thermal from Mooncat </t>
+        </is>
+      </c>
+      <c r="C959" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/ag7a8080bhde1</t>
+        </is>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" t="inlineStr">
+        <is>
+          <t>1i37xxb</t>
+        </is>
+      </c>
+      <c r="B960" t="inlineStr">
+        <is>
+          <t>Could anyone help me identify the name of this OPI mini bottle?</t>
+        </is>
+      </c>
+      <c r="C960" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i37xxb</t>
+        </is>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" t="inlineStr">
+        <is>
+          <t>1i37tzu</t>
+        </is>
+      </c>
+      <c r="B961" t="inlineStr">
+        <is>
+          <t>A dog needs attention - tell me something I don’t know!</t>
+        </is>
+      </c>
+      <c r="C961" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i37tzu</t>
+        </is>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" t="inlineStr">
+        <is>
+          <t>1i378xa</t>
+        </is>
+      </c>
+      <c r="B962" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Whimsical multichrome butterflies for my first reverse stamping attempt </t>
+        </is>
+      </c>
+      <c r="C962" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i378xa</t>
+        </is>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" t="inlineStr">
+        <is>
+          <t>1i36727</t>
+        </is>
+      </c>
+      <c r="B963" t="inlineStr">
+        <is>
+          <t>Hobbit hole inspired mani</t>
+        </is>
+      </c>
+      <c r="C963" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i36727</t>
+        </is>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" t="inlineStr">
+        <is>
+          <t>1i3630z</t>
+        </is>
+      </c>
+      <c r="B964" t="inlineStr">
+        <is>
+          <t>Sparkly shorties✨</t>
+        </is>
+      </c>
+      <c r="C964" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r2bmpicgsgde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" t="inlineStr">
+        <is>
+          <t>1i360hw</t>
+        </is>
+      </c>
+      <c r="B965" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pink lava set🦩🩷 💎 </t>
+        </is>
+      </c>
+      <c r="C965" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/4f8x7bjtrgde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" t="inlineStr">
+        <is>
+          <t>1i35w9i</t>
+        </is>
+      </c>
+      <c r="B966" t="inlineStr">
+        <is>
+          <t>Nails getting ruined at work</t>
+        </is>
+      </c>
+      <c r="C966" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i35w9i/nails_getting_ruined_at_work/</t>
+        </is>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" t="inlineStr">
+        <is>
+          <t>1i35h2a</t>
+        </is>
+      </c>
+      <c r="B967" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ethereal comparison/swatch help needed </t>
+        </is>
+      </c>
+      <c r="C967" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i35h2a/ethereal_comparisonswatch_help_needed/</t>
+        </is>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" t="inlineStr">
+        <is>
+          <t>1i35ev0</t>
+        </is>
+      </c>
+      <c r="B968" t="inlineStr">
+        <is>
+          <t>Reverse Velvet</t>
+        </is>
+      </c>
+      <c r="C968" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i35ev0/reverse_velvet/</t>
+        </is>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" t="inlineStr">
+        <is>
+          <t>1i35dss</t>
+        </is>
+      </c>
+      <c r="B969" t="inlineStr">
+        <is>
+          <t>Ambitious request, this has never been done</t>
+        </is>
+      </c>
+      <c r="C969" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i35dss/ambitious_request_this_has_never_been_done/</t>
+        </is>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" t="inlineStr">
+        <is>
+          <t>1i35bav</t>
+        </is>
+      </c>
+      <c r="B970" t="inlineStr">
+        <is>
+          <t>Quick dry top coats that don't stain from black clothes?</t>
+        </is>
+      </c>
+      <c r="C970" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i35bav/quick_dry_top_coats_that_dont_stain_from_black/</t>
+        </is>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" t="inlineStr">
+        <is>
+          <t>1i35am6</t>
+        </is>
+      </c>
+      <c r="B971" t="inlineStr">
+        <is>
+          <t>I call this Neapolitan ice cream 🍦</t>
+        </is>
+      </c>
+      <c r="C971" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i35am6</t>
+        </is>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" t="inlineStr">
+        <is>
+          <t>1i33hbf</t>
+        </is>
+      </c>
+      <c r="B972" t="inlineStr">
+        <is>
+          <t>January bluesss 💙💙💙</t>
+        </is>
+      </c>
+      <c r="C972" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i33hbf</t>
+        </is>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" t="inlineStr">
+        <is>
+          <t>1i33ddt</t>
+        </is>
+      </c>
+      <c r="B973" t="inlineStr">
+        <is>
+          <t>Cowgirl nails? 🤠</t>
+        </is>
+      </c>
+      <c r="C973" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i33ddt/cowgirl_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" t="inlineStr">
+        <is>
+          <t>1i331o7</t>
+        </is>
+      </c>
+      <c r="B974" t="inlineStr">
+        <is>
+          <t>Mooncat's House of Hades vs ILNP's midnight kiss: almost dupes?</t>
+        </is>
+      </c>
+      <c r="C974" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i331o7</t>
+        </is>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" t="inlineStr">
+        <is>
+          <t>1i3301m</t>
+        </is>
+      </c>
+      <c r="B975" t="inlineStr">
+        <is>
+          <t>Best metallics?</t>
+        </is>
+      </c>
+      <c r="C975" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i3301m/best_metallics/</t>
+        </is>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" t="inlineStr">
+        <is>
+          <t>1i32pxt</t>
+        </is>
+      </c>
+      <c r="B976" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Thermal + matching (??) gradient </t>
+        </is>
+      </c>
+      <c r="C976" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i32pxt</t>
+        </is>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" t="inlineStr">
+        <is>
+          <t>1i32mzh</t>
+        </is>
+      </c>
+      <c r="B977" t="inlineStr">
+        <is>
+          <t>I can’t believe this has been untried for a year!</t>
+        </is>
+      </c>
+      <c r="C977" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i32mzh</t>
+        </is>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" t="inlineStr">
+        <is>
+          <t>1i32jzy</t>
+        </is>
+      </c>
+      <c r="B978" t="inlineStr">
+        <is>
+          <t>How to recreate this look</t>
+        </is>
+      </c>
+      <c r="C978" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i32jzy/how_to_recreate_this_look/</t>
+        </is>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" t="inlineStr">
+        <is>
+          <t>1i31nhl</t>
+        </is>
+      </c>
+      <c r="B979" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I turn into a cat chasing sun puddles whenever I wear a sparkly polish. </t>
+        </is>
+      </c>
+      <c r="C979" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i31nhl</t>
+        </is>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" t="inlineStr">
+        <is>
+          <t>1i2w94q</t>
+        </is>
+      </c>
+      <c r="B980" t="inlineStr">
+        <is>
+          <t>Table lighting recs?</t>
+        </is>
+      </c>
+      <c r="C980" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i2w94q/table_lighting_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" t="inlineStr">
+        <is>
+          <t>1i2z22i</t>
+        </is>
+      </c>
+      <c r="B981" t="inlineStr">
+        <is>
+          <t>cirque hearth jelly</t>
+        </is>
+      </c>
+      <c r="C981" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2z22i</t>
+        </is>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" t="inlineStr">
+        <is>
+          <t>1i308c8</t>
+        </is>
+      </c>
+      <c r="B982" t="inlineStr">
+        <is>
+          <t>So glad I saw that post</t>
+        </is>
+      </c>
+      <c r="C982" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i308c8</t>
+        </is>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" t="inlineStr">
+        <is>
+          <t>1i2zitd</t>
+        </is>
+      </c>
+      <c r="B983" t="inlineStr">
+        <is>
+          <t>🩵🩷 Wintery Skittle 🩶🤍 ❄️Playing around with some of my icy winter shades. Index - ILNP Snow Angel. Middle - ILNP Sled Day. Ring - ILNP Rosewater. Thumb and pinky - Rogue Laquer Snow Be It. All topped with ILNP Spotlight ✨</t>
+        </is>
+      </c>
+      <c r="C983" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2zitd</t>
+        </is>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" t="inlineStr">
+        <is>
+          <t>1i2z7jf</t>
+        </is>
+      </c>
+      <c r="B984" t="inlineStr">
+        <is>
+          <t>Sugar &amp; ice and everything nice :)</t>
+        </is>
+      </c>
+      <c r="C984" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2z7jf</t>
+        </is>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" t="inlineStr">
+        <is>
+          <t>1i2z6jm</t>
+        </is>
+      </c>
+      <c r="B985" t="inlineStr">
+        <is>
+          <t>Recommend me your weirdest/most unique orange polish</t>
+        </is>
+      </c>
+      <c r="C985" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i2z6jm/recommend_me_your_weirdestmost_unique_orange/</t>
+        </is>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" t="inlineStr">
+        <is>
+          <t>1i2z48a</t>
+        </is>
+      </c>
+      <c r="B986" t="inlineStr">
+        <is>
+          <t>Brown “cat eye”</t>
+        </is>
+      </c>
+      <c r="C986" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2z48a</t>
+        </is>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" t="inlineStr">
+        <is>
+          <t>1i2ypid</t>
+        </is>
+      </c>
+      <c r="B987" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Help with stamped French tips </t>
+        </is>
+      </c>
+      <c r="C987" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i2ypid/help_with_stamped_french_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" t="inlineStr">
+        <is>
+          <t>1i2ykyu</t>
+        </is>
+      </c>
+      <c r="B988" t="inlineStr">
+        <is>
+          <t>Looking to find pink like this</t>
+        </is>
+      </c>
+      <c r="C988" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/59bwf53w1fde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" t="inlineStr">
+        <is>
+          <t>1i2ydbe</t>
+        </is>
+      </c>
+      <c r="B989" t="inlineStr">
+        <is>
+          <t>Mooncat Moonrise</t>
+        </is>
+      </c>
+      <c r="C989" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2ydbe</t>
+        </is>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" t="inlineStr">
+        <is>
+          <t>1i2y25r</t>
+        </is>
+      </c>
+      <c r="B990" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Wawa wee wa! this color certainly lives up to its hype- I’m in love! </t>
+        </is>
+      </c>
+      <c r="C990" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2y25r</t>
+        </is>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" t="inlineStr">
+        <is>
+          <t>1i2xnaw</t>
+        </is>
+      </c>
+      <c r="B991" t="inlineStr">
+        <is>
+          <t>First time using ILNP Pixie Party 🧚</t>
+        </is>
+      </c>
+      <c r="C991" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jlajowtpuede1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" t="inlineStr">
+        <is>
+          <t>1i2xhhs</t>
+        </is>
+      </c>
+      <c r="B992" t="inlineStr">
+        <is>
+          <t>I didn’t expect this one to practically ✨ GLOW ✨</t>
+        </is>
+      </c>
+      <c r="C992" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dtxqqiojtede1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" t="inlineStr">
+        <is>
+          <t>1i2xf94</t>
+        </is>
+      </c>
+      <c r="B993" t="inlineStr">
+        <is>
+          <t>Bright orange-red nails to bring me good luck on the certification exam that I took today</t>
+        </is>
+      </c>
+      <c r="C993" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2xf94</t>
+        </is>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" t="inlineStr">
+        <is>
+          <t>1i2x8no</t>
+        </is>
+      </c>
+      <c r="B994" t="inlineStr">
+        <is>
+          <t>Forever my go to combo 🩸</t>
+        </is>
+      </c>
+      <c r="C994" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t7o2dg1prede1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" t="inlineStr">
+        <is>
+          <t>1i2x3i7</t>
+        </is>
+      </c>
+      <c r="B995" t="inlineStr">
+        <is>
+          <t>Verdigris</t>
+        </is>
+      </c>
+      <c r="C995" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7eep8uwlqede1</t>
+        </is>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" t="inlineStr">
+        <is>
+          <t>1i2wxzo</t>
+        </is>
+      </c>
+      <c r="B996" t="inlineStr">
+        <is>
+          <t>Party Popper by ILNP is such a gorgeous topper</t>
+        </is>
+      </c>
+      <c r="C996" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2wxzo</t>
+        </is>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" t="inlineStr">
+        <is>
+          <t>1i2wxm2</t>
+        </is>
+      </c>
+      <c r="B997" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sometimes you just want a nice creme. </t>
+        </is>
+      </c>
+      <c r="C997" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8j4xj94dpede1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" t="inlineStr">
+        <is>
+          <t>1i2wmns</t>
+        </is>
+      </c>
+      <c r="B998" t="inlineStr">
+        <is>
+          <t>I've really been into the crushed metallics this season so I made my own</t>
+        </is>
+      </c>
+      <c r="C998" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2wmns</t>
+        </is>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" t="inlineStr">
+        <is>
+          <t>1i2wfz7</t>
+        </is>
+      </c>
+      <c r="B999" t="inlineStr">
+        <is>
+          <t>catfished 🐟💙</t>
+        </is>
+      </c>
+      <c r="C999" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/71k5hb4nlede1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" t="inlineStr">
+        <is>
+          <t>1i2wfnt</t>
+        </is>
+      </c>
+      <c r="B1000" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I need help </t>
+        </is>
+      </c>
+      <c r="C1000" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i2wfnt/i_need_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" t="inlineStr">
+        <is>
+          <t>1i2w52l</t>
+        </is>
+      </c>
+      <c r="B1001" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ISO a longer replacement brush </t>
+        </is>
+      </c>
+      <c r="C1001" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i2w52l/iso_a_longer_replacement_brush/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" t="inlineStr">
+        <is>
+          <t>1i2tpyy</t>
+        </is>
+      </c>
+      <c r="B1002" t="inlineStr">
+        <is>
+          <t>First Ever at Home Gel-X mani 🥳</t>
+        </is>
+      </c>
+      <c r="C1002" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2tpyy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" t="inlineStr">
+        <is>
+          <t>1i2vzr1</t>
+        </is>
+      </c>
+      <c r="B1003" t="inlineStr">
+        <is>
+          <t>What/where do I buy uv gel polish for a total newbie?</t>
+        </is>
+      </c>
+      <c r="C1003" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i2vzr1/whatwhere_do_i_buy_uv_gel_polish_for_a_total/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" t="inlineStr">
+        <is>
+          <t>1i2vtgd</t>
+        </is>
+      </c>
+      <c r="B1004" t="inlineStr">
+        <is>
+          <t>Blurring base coats</t>
+        </is>
+      </c>
+      <c r="C1004" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i2vtgd/blurring_base_coats/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" t="inlineStr">
+        <is>
+          <t>1i2vd79</t>
+        </is>
+      </c>
+      <c r="B1005" t="inlineStr">
+        <is>
+          <t>My first indie polish mani is also my first multichrome AND first magnetic - I’m hooked!</t>
+        </is>
+      </c>
+      <c r="C1005" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/y6t04pyidede1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" t="inlineStr">
+        <is>
+          <t>1i2v8k3</t>
+        </is>
+      </c>
+      <c r="B1006" t="inlineStr">
+        <is>
+          <t>Any dangers with nail polish and kids?</t>
+        </is>
+      </c>
+      <c r="C1006" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i2v8k3/any_dangers_with_nail_polish_and_kids/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" t="inlineStr">
+        <is>
+          <t>1i2v6gu</t>
+        </is>
+      </c>
+      <c r="B1007" t="inlineStr">
+        <is>
+          <t>👷‍♂️🚗Road Work Ahead🚧👷‍♀️</t>
+        </is>
+      </c>
+      <c r="C1007" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2v6gu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" t="inlineStr">
+        <is>
+          <t>1i2utl2</t>
+        </is>
+      </c>
+      <c r="B1008" t="inlineStr">
+        <is>
+          <t>Hard reset for the new year 🎊</t>
+        </is>
+      </c>
+      <c r="C1008" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kogi6lrh9ede1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" t="inlineStr">
+        <is>
+          <t>1i2ummi</t>
+        </is>
+      </c>
+      <c r="B1009" t="inlineStr">
+        <is>
+          <t>Dupes for this gel polish? (Gelcare rosehip oil)</t>
+        </is>
+      </c>
+      <c r="C1009" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hj5ak3t28ede1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" t="inlineStr">
+        <is>
+          <t>1i2ukce</t>
+        </is>
+      </c>
+      <c r="B1010" t="inlineStr">
+        <is>
+          <t>Do you redo your polish after the smallest chip starts?</t>
+        </is>
+      </c>
+      <c r="C1010" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i2ukce/do_you_redo_your_polish_after_the_smallest_chip/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" t="inlineStr">
+        <is>
+          <t>1i2u4l5</t>
+        </is>
+      </c>
+      <c r="B1011" t="inlineStr">
+        <is>
+          <t>I need this colour back in my life 🥹</t>
+        </is>
+      </c>
+      <c r="C1011" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tk9qs1hb4ede1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" t="inlineStr">
+        <is>
+          <t>1i2twwn</t>
+        </is>
+      </c>
+      <c r="B1012" t="inlineStr">
+        <is>
+          <t>Where to start with Sassy Sauce?</t>
+        </is>
+      </c>
+      <c r="C1012" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i2twwn/where_to_start_with_sassy_sauce/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" t="inlineStr">
+        <is>
+          <t>1i2tr15</t>
+        </is>
+      </c>
+      <c r="B1013" t="inlineStr">
+        <is>
+          <t>Accidental dupe?</t>
+        </is>
+      </c>
+      <c r="C1013" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2tr15</t>
+        </is>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" t="inlineStr">
+        <is>
+          <t>1i2tnpn</t>
+        </is>
+      </c>
+      <c r="B1014" t="inlineStr">
+        <is>
+          <t>Where did all of Cirque's créme colors go??? Am I just off trend?</t>
+        </is>
+      </c>
+      <c r="C1014" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i2tnpn/where_did_all_of_cirques_créme_colors_go_am_i/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" t="inlineStr">
+        <is>
+          <t>1i2tcfd</t>
+        </is>
+      </c>
+      <c r="B1015" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My first time trying stamping! </t>
+        </is>
+      </c>
+      <c r="C1015" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2tcfd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" t="inlineStr">
+        <is>
+          <t>1i2t7p9</t>
+        </is>
+      </c>
+      <c r="B1016" t="inlineStr">
+        <is>
+          <t>I am growing my nails out for the first time in 13 years….can I use fake nails during the “awkward” phase?</t>
+        </is>
+      </c>
+      <c r="C1016" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i2t7p9/i_am_growing_my_nails_out_for_the_first_time_in/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" t="inlineStr">
+        <is>
+          <t>1i2sz8b</t>
+        </is>
+      </c>
+      <c r="B1017" t="inlineStr">
+        <is>
+          <t>My wife picks my mani pt 3</t>
+        </is>
+      </c>
+      <c r="C1017" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2sz8b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1018">
+      <c r="A1018" t="inlineStr">
+        <is>
+          <t>1i2sqhd</t>
+        </is>
+      </c>
+      <c r="B1018" t="inlineStr">
+        <is>
+          <t>Ordering from Zoya</t>
+        </is>
+      </c>
+      <c r="C1018" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i2sqhd/ordering_from_zoya/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1019">
+      <c r="A1019" t="inlineStr">
+        <is>
+          <t>1i2s4dr</t>
+        </is>
+      </c>
+      <c r="B1019" t="inlineStr">
+        <is>
+          <t>shopping my stash!</t>
+        </is>
+      </c>
+      <c r="C1019" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2s4dr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1020">
+      <c r="A1020" t="inlineStr">
+        <is>
+          <t>1i2rwsc</t>
+        </is>
+      </c>
+      <c r="B1020" t="inlineStr">
+        <is>
+          <t>Lavender with pink shimmer?</t>
+        </is>
+      </c>
+      <c r="C1020" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/v4yb1fcjndde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1021">
+      <c r="A1021" t="inlineStr">
+        <is>
+          <t>1i2rw8c</t>
+        </is>
+      </c>
+      <c r="B1021" t="inlineStr">
+        <is>
+          <t>My coworker thinks ladies shouldn't wear glitter polish cuz men hates it</t>
+        </is>
+      </c>
+      <c r="C1021" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2rw8c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1022">
+      <c r="A1022" t="inlineStr">
+        <is>
+          <t>1i2ru9o</t>
+        </is>
+      </c>
+      <c r="B1022" t="inlineStr">
+        <is>
+          <t>Looking for dupe for BKL Kikimora</t>
+        </is>
+      </c>
+      <c r="C1022" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mq6rpmbzmdde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1023">
+      <c r="A1023" t="inlineStr">
+        <is>
+          <t>1i2rfbb</t>
+        </is>
+      </c>
+      <c r="B1023" t="inlineStr">
+        <is>
+          <t>This is your friendly reminder to shop your collection ✨</t>
+        </is>
+      </c>
+      <c r="C1023" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2rfbb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1024">
+      <c r="A1024" t="inlineStr">
+        <is>
+          <t>1i2raqc</t>
+        </is>
+      </c>
+      <c r="B1024" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ethereal Alien </t>
+        </is>
+      </c>
+      <c r="C1024" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lw5a9uloidde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1025">
+      <c r="A1025" t="inlineStr">
+        <is>
+          <t>1i2qtg1</t>
+        </is>
+      </c>
+      <c r="B1025" t="inlineStr">
+        <is>
+          <t>Best gel so far. Cuticles need help.</t>
+        </is>
+      </c>
+      <c r="C1025" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2txbzpqtedde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1026">
+      <c r="A1026" t="inlineStr">
+        <is>
+          <t>1i2qq71</t>
+        </is>
+      </c>
+      <c r="B1026" t="inlineStr">
+        <is>
+          <t>Chrome Powder vs Sally Hanson</t>
+        </is>
+      </c>
+      <c r="C1026" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/senf4ca4edde1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1027">
+      <c r="A1027" t="inlineStr">
+        <is>
+          <t>1i2qi13</t>
+        </is>
+      </c>
+      <c r="B1027" t="inlineStr">
+        <is>
+          <t>What are you favorites from Cupcake?</t>
+        </is>
+      </c>
+      <c r="C1027" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i2qi13/what_are_you_favorites_from_cupcake/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1028">
+      <c r="A1028" t="inlineStr">
+        <is>
+          <t>1i2qcdj</t>
+        </is>
+      </c>
+      <c r="B1028" t="inlineStr">
+        <is>
+          <t>Green eyed monster 👽🧪👁</t>
+        </is>
+      </c>
+      <c r="C1028" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2qcdj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1029">
+      <c r="A1029" t="inlineStr">
+        <is>
+          <t>1i2q32q</t>
+        </is>
+      </c>
+      <c r="B1029" t="inlineStr">
+        <is>
+          <t xml:space="preserve">So shifty !! </t>
+        </is>
+      </c>
+      <c r="C1029" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/69a1wlao8dde1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1030">
+      <c r="A1030" t="inlineStr">
+        <is>
+          <t>1i2nw1x</t>
+        </is>
+      </c>
+      <c r="B1030" t="inlineStr">
+        <is>
+          <t>The Unbridled Rage</t>
+        </is>
+      </c>
+      <c r="C1030" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2nw1x</t>
+        </is>
+      </c>
+    </row>
+    <row r="1031">
+      <c r="A1031" t="inlineStr">
+        <is>
+          <t>1i2mz7g</t>
+        </is>
+      </c>
+      <c r="B1031" t="inlineStr">
+        <is>
+          <t>When thermal polishes "die" - which color do they take?</t>
+        </is>
+      </c>
+      <c r="C1031" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i2mz7g/when_thermal_polishes_die_which_color_do_they_take/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1032">
+      <c r="A1032" t="inlineStr">
+        <is>
+          <t>1i2lrtu</t>
+        </is>
+      </c>
+      <c r="B1032" t="inlineStr">
+        <is>
+          <t>How to change colour on already done gel nails?</t>
+        </is>
+      </c>
+      <c r="C1032" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i2lrtu/how_to_change_colour_on_already_done_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1033">
+      <c r="A1033" t="inlineStr">
+        <is>
+          <t>1i22b6n</t>
+        </is>
+      </c>
+      <c r="B1033" t="inlineStr">
+        <is>
+          <t>Any tips on doing gel nails at home?</t>
+        </is>
+      </c>
+      <c r="C1033" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i22b6n/any_tips_on_doing_gel_nails_at_home/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1034">
+      <c r="A1034" t="inlineStr">
+        <is>
+          <t>1i3b7ig</t>
+        </is>
+      </c>
+      <c r="B1034" t="inlineStr">
+        <is>
+          <t>Ready for my birthday</t>
+        </is>
+      </c>
+      <c r="C1034" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/feoah5tubide1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1035">
+      <c r="A1035" t="inlineStr">
+        <is>
+          <t>1i38yq1</t>
+        </is>
+      </c>
+      <c r="B1035" t="inlineStr">
+        <is>
+          <t>IG @ra3creat3s 💅🏼</t>
+        </is>
+      </c>
+      <c r="C1035" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i38yq1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1036">
+      <c r="A1036" t="inlineStr">
+        <is>
+          <t>1i37q5o</t>
+        </is>
+      </c>
+      <c r="B1036" t="inlineStr">
+        <is>
+          <t>Fourth Wing/ Iron Flame set</t>
+        </is>
+      </c>
+      <c r="C1036" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i37q5o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1037">
+      <c r="A1037" t="inlineStr">
+        <is>
+          <t>1i369nf</t>
+        </is>
+      </c>
+      <c r="B1037" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My take on mob wife nails </t>
+        </is>
+      </c>
+      <c r="C1037" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/96edl2a5ugde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1038">
+      <c r="A1038" t="inlineStr">
+        <is>
+          <t>1i35hqr</t>
+        </is>
+      </c>
+      <c r="B1038" t="inlineStr">
+        <is>
+          <t>Any good recommendations for a glossy top coat! I'm struggling with air bubbles in mine and it's so irritating 😭</t>
+        </is>
+      </c>
+      <c r="C1038" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i35hqr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1039">
+      <c r="A1039" t="inlineStr">
+        <is>
+          <t>1i355wx</t>
+        </is>
+      </c>
+      <c r="B1039" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Valentine’s Day ready 💌 </t>
+        </is>
+      </c>
+      <c r="C1039" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i355wx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1040">
+      <c r="A1040" t="inlineStr">
+        <is>
+          <t>1i34nga</t>
+        </is>
+      </c>
+      <c r="B1040" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Painting a Creature Commandos Nails Set 💕 Starting with "The Bride" </t>
+        </is>
+      </c>
+      <c r="C1040" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/b9p0vdiffgde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1041">
+      <c r="A1041" t="inlineStr">
+        <is>
+          <t>1i33bbi</t>
+        </is>
+      </c>
+      <c r="B1041" t="inlineStr">
+        <is>
+          <t>some of my nail art recently</t>
+        </is>
+      </c>
+      <c r="C1041" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i33bbi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1042">
+      <c r="A1042" t="inlineStr">
+        <is>
+          <t>1i308qp</t>
+        </is>
+      </c>
+      <c r="B1042" t="inlineStr">
+        <is>
+          <t>Infinity Nikki Inspired Nails</t>
+        </is>
+      </c>
+      <c r="C1042" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lrsuh1tsefde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1043">
+      <c r="A1043" t="inlineStr">
+        <is>
+          <t>1i2xdca</t>
+        </is>
+      </c>
+      <c r="B1043" t="inlineStr">
+        <is>
+          <t>🌺🌸</t>
+        </is>
+      </c>
+      <c r="C1043" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ltb38xoosede1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1044">
+      <c r="A1044" t="inlineStr">
+        <is>
+          <t>1i2usq0</t>
+        </is>
+      </c>
+      <c r="B1044" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Finished them! </t>
+        </is>
+      </c>
+      <c r="C1044" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2usq0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1045">
+      <c r="A1045" t="inlineStr">
+        <is>
+          <t>1i2u9yc</t>
+        </is>
+      </c>
+      <c r="B1045" t="inlineStr">
+        <is>
+          <t>I fell in love! You can tell it by my nails</t>
+        </is>
+      </c>
+      <c r="C1045" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/evcg4g8d5ede1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1046">
+      <c r="A1046" t="inlineStr">
+        <is>
+          <t>1i2s1sb</t>
+        </is>
+      </c>
+      <c r="B1046" t="inlineStr">
+        <is>
+          <t>For the Disney fans ✨🐭</t>
+        </is>
+      </c>
+      <c r="C1046" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mlh8m1pnodde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1047">
+      <c r="A1047" t="inlineStr">
+        <is>
+          <t>1i2re1r</t>
+        </is>
+      </c>
+      <c r="B1047" t="inlineStr">
+        <is>
+          <t>Casual valentines nails</t>
+        </is>
+      </c>
+      <c r="C1047" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7mmuy9hfjdde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1048">
+      <c r="A1048" t="inlineStr">
+        <is>
+          <t>1i2oz01</t>
+        </is>
+      </c>
+      <c r="B1048" t="inlineStr">
+        <is>
+          <t>First cateye set! 💅</t>
+        </is>
+      </c>
+      <c r="C1048" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xmr1r0lxycde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1049">
+      <c r="A1049" t="inlineStr">
+        <is>
+          <t>1i2o34o</t>
+        </is>
+      </c>
+      <c r="B1049" t="inlineStr">
+        <is>
+          <t>Line faces</t>
+        </is>
+      </c>
+      <c r="C1049" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2o34o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1050">
+      <c r="A1050" t="inlineStr">
+        <is>
+          <t>1i2n1t4</t>
+        </is>
+      </c>
+      <c r="B1050" t="inlineStr">
+        <is>
+          <t>I envy myself</t>
+        </is>
+      </c>
+      <c r="C1050" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8vpdba7mecde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1051">
+      <c r="A1051" t="inlineStr">
+        <is>
+          <t>1i2mw2e</t>
+        </is>
+      </c>
+      <c r="B1051" t="inlineStr">
+        <is>
+          <t>How hard or easy is something like this? (See text)</t>
+        </is>
+      </c>
+      <c r="C1051" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gf8pwxd1dcde1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1052">
+      <c r="A1052" t="inlineStr">
+        <is>
+          <t>1i2lmxk</t>
+        </is>
+      </c>
+      <c r="B1052" t="inlineStr">
+        <is>
+          <t>Nuance</t>
+        </is>
+      </c>
+      <c r="C1052" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i2lmxk</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sat Jan 18 08:08:47 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_01_19.xlsx
+++ b/data/collected_data/2025_01_19.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1052"/>
+  <dimension ref="A1:C1253"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -18319,6 +18319,3423 @@
         </is>
       </c>
     </row>
+    <row r="1053">
+      <c r="A1053" t="inlineStr">
+        <is>
+          <t>1i42ohf</t>
+        </is>
+      </c>
+      <c r="B1053" t="inlineStr">
+        <is>
+          <t>We just finished building our beach house... so NOW I no longer feel guilty for having two of everything!!! Frigging expensive way to de guilt myself of my nail habit!!!</t>
+        </is>
+      </c>
+      <c r="C1053" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/43welimwjpde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1054">
+      <c r="A1054" t="inlineStr">
+        <is>
+          <t>1i41pxp</t>
+        </is>
+      </c>
+      <c r="B1054" t="inlineStr">
+        <is>
+          <t>Removal</t>
+        </is>
+      </c>
+      <c r="C1054" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i41pxp/removal/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1055">
+      <c r="A1055" t="inlineStr">
+        <is>
+          <t>1i41ht2</t>
+        </is>
+      </c>
+      <c r="B1055" t="inlineStr">
+        <is>
+          <t>There so bad 😭</t>
+        </is>
+      </c>
+      <c r="C1055" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i41ht2</t>
+        </is>
+      </c>
+    </row>
+    <row r="1056">
+      <c r="A1056" t="inlineStr">
+        <is>
+          <t>1i41hoy</t>
+        </is>
+      </c>
+      <c r="B1056" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My favorite nail art. </t>
+        </is>
+      </c>
+      <c r="C1056" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i41hoy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1057">
+      <c r="A1057" t="inlineStr">
+        <is>
+          <t>1i40ujn</t>
+        </is>
+      </c>
+      <c r="B1057" t="inlineStr">
+        <is>
+          <t>it took me forever but im happy with them</t>
+        </is>
+      </c>
+      <c r="C1057" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i40ujn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1058">
+      <c r="A1058" t="inlineStr">
+        <is>
+          <t>1i3ywhf</t>
+        </is>
+      </c>
+      <c r="B1058" t="inlineStr">
+        <is>
+          <t>New to this</t>
+        </is>
+      </c>
+      <c r="C1058" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3ywhf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1059">
+      <c r="A1059" t="inlineStr">
+        <is>
+          <t>1i40qjw</t>
+        </is>
+      </c>
+      <c r="B1059" t="inlineStr">
+        <is>
+          <t>OPI Xpress/on Nails discolored?</t>
+        </is>
+      </c>
+      <c r="C1059" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i40qjw</t>
+        </is>
+      </c>
+    </row>
+    <row r="1060">
+      <c r="A1060" t="inlineStr">
+        <is>
+          <t>1i40drc</t>
+        </is>
+      </c>
+      <c r="B1060" t="inlineStr">
+        <is>
+          <t>My first time long nails, harder than it seems. U know?</t>
+        </is>
+      </c>
+      <c r="C1060" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/69wb4vjtrode1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1061">
+      <c r="A1061" t="inlineStr">
+        <is>
+          <t>1i40dps</t>
+        </is>
+      </c>
+      <c r="B1061" t="inlineStr">
+        <is>
+          <t>Love this color!!</t>
+        </is>
+      </c>
+      <c r="C1061" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/88331o7rrode1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1062">
+      <c r="A1062" t="inlineStr">
+        <is>
+          <t>1i405po</t>
+        </is>
+      </c>
+      <c r="B1062" t="inlineStr">
+        <is>
+          <t>🫐 nails 😍</t>
+        </is>
+      </c>
+      <c r="C1062" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/j78zfuhfpode1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1063">
+      <c r="A1063" t="inlineStr">
+        <is>
+          <t>1i4025j</t>
+        </is>
+      </c>
+      <c r="B1063" t="inlineStr">
+        <is>
+          <t>black luvvvv</t>
+        </is>
+      </c>
+      <c r="C1063" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r5tafyjeoode1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1064">
+      <c r="A1064" t="inlineStr">
+        <is>
+          <t>1i3ytim</t>
+        </is>
+      </c>
+      <c r="B1064" t="inlineStr">
+        <is>
+          <t xml:space="preserve">If it doesn't require a lamp, is it really gel? </t>
+        </is>
+      </c>
+      <c r="C1064" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i3ytim/if_it_doesnt_require_a_lamp_is_it_really_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1065">
+      <c r="A1065" t="inlineStr">
+        <is>
+          <t>1i3ywzh</t>
+        </is>
+      </c>
+      <c r="B1065" t="inlineStr">
+        <is>
+          <t>Help I broke my nail badly!</t>
+        </is>
+      </c>
+      <c r="C1065" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i3ywzh/help_i_broke_my_nail_badly/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1066">
+      <c r="A1066" t="inlineStr">
+        <is>
+          <t>1i3zpj6</t>
+        </is>
+      </c>
+      <c r="B1066" t="inlineStr">
+        <is>
+          <t>Please help a girl out!</t>
+        </is>
+      </c>
+      <c r="C1066" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3zpj6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1067">
+      <c r="A1067" t="inlineStr">
+        <is>
+          <t>1i3zbwd</t>
+        </is>
+      </c>
+      <c r="B1067" t="inlineStr">
+        <is>
+          <t>OPI Bubble Bath??</t>
+        </is>
+      </c>
+      <c r="C1067" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3zbwd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1068">
+      <c r="A1068" t="inlineStr">
+        <is>
+          <t>1i3xjah</t>
+        </is>
+      </c>
+      <c r="B1068" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can I get my nail fixed or is that unsafe </t>
+        </is>
+      </c>
+      <c r="C1068" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u18onw5jynde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1069">
+      <c r="A1069" t="inlineStr">
+        <is>
+          <t>1i3wxce</t>
+        </is>
+      </c>
+      <c r="B1069" t="inlineStr">
+        <is>
+          <t>Unicorn inspired nails by my bestfriend</t>
+        </is>
+      </c>
+      <c r="C1069" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oq95ytbpsnde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1070">
+      <c r="A1070" t="inlineStr">
+        <is>
+          <t>1i400j0</t>
+        </is>
+      </c>
+      <c r="B1070" t="inlineStr">
+        <is>
+          <t>Soft pink marble 🤍</t>
+        </is>
+      </c>
+      <c r="C1070" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i400j0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1071">
+      <c r="A1071" t="inlineStr">
+        <is>
+          <t>1i3zxkk</t>
+        </is>
+      </c>
+      <c r="B1071" t="inlineStr">
+        <is>
+          <t>out of budget?</t>
+        </is>
+      </c>
+      <c r="C1071" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i3zxkk/out_of_budget/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1072">
+      <c r="A1072" t="inlineStr">
+        <is>
+          <t>1i3zmfb</t>
+        </is>
+      </c>
+      <c r="B1072" t="inlineStr">
+        <is>
+          <t>Thinking about getting acrylics and not sure what the best nail shape &amp; length is for my hand?</t>
+        </is>
+      </c>
+      <c r="C1072" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xwxa3blkjode1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1073">
+      <c r="A1073" t="inlineStr">
+        <is>
+          <t>1i3zf7m</t>
+        </is>
+      </c>
+      <c r="B1073" t="inlineStr">
+        <is>
+          <t>Almond to stiletto- are these long enough?</t>
+        </is>
+      </c>
+      <c r="C1073" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3zf7m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1074">
+      <c r="A1074" t="inlineStr">
+        <is>
+          <t>1i3zb02</t>
+        </is>
+      </c>
+      <c r="B1074" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cat eye butterfly's </t>
+        </is>
+      </c>
+      <c r="C1074" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tj73dk27gode1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1075">
+      <c r="A1075" t="inlineStr">
+        <is>
+          <t>1i3z95b</t>
+        </is>
+      </c>
+      <c r="B1075" t="inlineStr">
+        <is>
+          <t>Haunting color shift</t>
+        </is>
+      </c>
+      <c r="C1075" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3z95b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1076">
+      <c r="A1076" t="inlineStr">
+        <is>
+          <t>1i3z8ob</t>
+        </is>
+      </c>
+      <c r="B1076" t="inlineStr">
+        <is>
+          <t>is it ok to put gel on the underside?</t>
+        </is>
+      </c>
+      <c r="C1076" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i3z8ob/is_it_ok_to_put_gel_on_the_underside/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1077">
+      <c r="A1077" t="inlineStr">
+        <is>
+          <t>1i3wu95</t>
+        </is>
+      </c>
+      <c r="B1077" t="inlineStr">
+        <is>
+          <t>inspired by my banana</t>
+        </is>
+      </c>
+      <c r="C1077" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6n1xcmzzrnde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1078">
+      <c r="A1078" t="inlineStr">
+        <is>
+          <t>1i3ym89</t>
+        </is>
+      </c>
+      <c r="B1078" t="inlineStr">
+        <is>
+          <t>Ready for the FREEZE ❄️🥶</t>
+        </is>
+      </c>
+      <c r="C1078" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3ym89</t>
+        </is>
+      </c>
+    </row>
+    <row r="1079">
+      <c r="A1079" t="inlineStr">
+        <is>
+          <t>1i3ym0d</t>
+        </is>
+      </c>
+      <c r="B1079" t="inlineStr">
+        <is>
+          <t>tengo ms uñas naturales maltratadas!</t>
+        </is>
+      </c>
+      <c r="C1079" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i3ym0d/tengo_ms_uñas_naturales_maltratadas/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1080">
+      <c r="A1080" t="inlineStr">
+        <is>
+          <t>1i3ylba</t>
+        </is>
+      </c>
+      <c r="B1080" t="inlineStr">
+        <is>
+          <t>$1 per small gem??</t>
+        </is>
+      </c>
+      <c r="C1080" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aey0etwy8ode1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1081">
+      <c r="A1081" t="inlineStr">
+        <is>
+          <t>1i3ycdr</t>
+        </is>
+      </c>
+      <c r="B1081" t="inlineStr">
+        <is>
+          <t>I love a dark color</t>
+        </is>
+      </c>
+      <c r="C1081" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1b5g5qdh6ode1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1082">
+      <c r="A1082" t="inlineStr">
+        <is>
+          <t>1i3xpff</t>
+        </is>
+      </c>
+      <c r="B1082" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Convince me my nails aren't too short </t>
+        </is>
+      </c>
+      <c r="C1082" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3xpff</t>
+        </is>
+      </c>
+    </row>
+    <row r="1083">
+      <c r="A1083" t="inlineStr">
+        <is>
+          <t>1i3xeyj</t>
+        </is>
+      </c>
+      <c r="B1083" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I took off my press ons and… </t>
+        </is>
+      </c>
+      <c r="C1083" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3xeyj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1084">
+      <c r="A1084" t="inlineStr">
+        <is>
+          <t>1i3wyyn</t>
+        </is>
+      </c>
+      <c r="B1084" t="inlineStr">
+        <is>
+          <t>swipe for a surprise -&gt;</t>
+        </is>
+      </c>
+      <c r="C1084" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3wyyn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1085">
+      <c r="A1085" t="inlineStr">
+        <is>
+          <t>1i3ww8k</t>
+        </is>
+      </c>
+      <c r="B1085" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Should the other hand look better painted identical or opposite? </t>
+        </is>
+      </c>
+      <c r="C1085" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qsrf9w2isnde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1086">
+      <c r="A1086" t="inlineStr">
+        <is>
+          <t>1i3wtkf</t>
+        </is>
+      </c>
+      <c r="B1086" t="inlineStr">
+        <is>
+          <t>Chrome nails I did today</t>
+        </is>
+      </c>
+      <c r="C1086" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ueda629srnde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1087">
+      <c r="A1087" t="inlineStr">
+        <is>
+          <t>1i3wows</t>
+        </is>
+      </c>
+      <c r="B1087" t="inlineStr">
+        <is>
+          <t>New set for my vacation 💅🏾</t>
+        </is>
+      </c>
+      <c r="C1087" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ufe1lcylqnde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1088">
+      <c r="A1088" t="inlineStr">
+        <is>
+          <t>1i3vfzb</t>
+        </is>
+      </c>
+      <c r="B1088" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Which one is your favorite? </t>
+        </is>
+      </c>
+      <c r="C1088" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3vfzb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1089">
+      <c r="A1089" t="inlineStr">
+        <is>
+          <t>1i3txf1</t>
+        </is>
+      </c>
+      <c r="B1089" t="inlineStr">
+        <is>
+          <t>Yall please help me - gel x</t>
+        </is>
+      </c>
+      <c r="C1089" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3txf1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1090">
+      <c r="A1090" t="inlineStr">
+        <is>
+          <t>1i3v6xu</t>
+        </is>
+      </c>
+      <c r="B1090" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New Set </t>
+        </is>
+      </c>
+      <c r="C1090" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3v6xu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1091">
+      <c r="A1091" t="inlineStr">
+        <is>
+          <t>1i3vrak</t>
+        </is>
+      </c>
+      <c r="B1091" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Took me forever but I did it </t>
+        </is>
+      </c>
+      <c r="C1091" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/gmnvkot5inde1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1092">
+      <c r="A1092" t="inlineStr">
+        <is>
+          <t>1i3v39a</t>
+        </is>
+      </c>
+      <c r="B1092" t="inlineStr">
+        <is>
+          <t>Love this stiletto nail design 🥰</t>
+        </is>
+      </c>
+      <c r="C1092" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jiql2789cnde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1093">
+      <c r="A1093" t="inlineStr">
+        <is>
+          <t>1i3v14a</t>
+        </is>
+      </c>
+      <c r="B1093" t="inlineStr">
+        <is>
+          <t>How do people do services as a nail tech without a license?</t>
+        </is>
+      </c>
+      <c r="C1093" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i3v14a/how_do_people_do_services_as_a_nail_tech_without/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1094">
+      <c r="A1094" t="inlineStr">
+        <is>
+          <t>1i3v01q</t>
+        </is>
+      </c>
+      <c r="B1094" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New nails </t>
+        </is>
+      </c>
+      <c r="C1094" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/12xvh4ugbnde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1095">
+      <c r="A1095" t="inlineStr">
+        <is>
+          <t>1i3uzeo</t>
+        </is>
+      </c>
+      <c r="B1095" t="inlineStr">
+        <is>
+          <t>My favorite Nail Color</t>
+        </is>
+      </c>
+      <c r="C1095" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/swy3cf2bbnde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1096">
+      <c r="A1096" t="inlineStr">
+        <is>
+          <t>1i3u0a1</t>
+        </is>
+      </c>
+      <c r="B1096" t="inlineStr">
+        <is>
+          <t>Gel 💅🏽 🩷💙</t>
+        </is>
+      </c>
+      <c r="C1096" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xxw0ok553nde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1097">
+      <c r="A1097" t="inlineStr">
+        <is>
+          <t>1i3t0bu</t>
+        </is>
+      </c>
+      <c r="B1097" t="inlineStr">
+        <is>
+          <t>Nail art channel content farms copying nail art channels' designs and video format</t>
+        </is>
+      </c>
+      <c r="C1097" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i3t0bu/nail_art_channel_content_farms_copying_nail_art/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1098">
+      <c r="A1098" t="inlineStr">
+        <is>
+          <t>1i3tm1o</t>
+        </is>
+      </c>
+      <c r="B1098" t="inlineStr">
+        <is>
+          <t>Valentine’s Day love notes 🩷📝 nail set done by my magical nail tech 💗✉️</t>
+        </is>
+      </c>
+      <c r="C1098" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/myy71c0tzmde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1099">
+      <c r="A1099" t="inlineStr">
+        <is>
+          <t>1i3tflr</t>
+        </is>
+      </c>
+      <c r="B1099" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Honest opinions?? </t>
+        </is>
+      </c>
+      <c r="C1099" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3tflr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1100">
+      <c r="A1100" t="inlineStr">
+        <is>
+          <t>1i3t79t</t>
+        </is>
+      </c>
+      <c r="B1100" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Am I being too picky? </t>
+        </is>
+      </c>
+      <c r="C1100" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3t79t</t>
+        </is>
+      </c>
+    </row>
+    <row r="1101">
+      <c r="A1101" t="inlineStr">
+        <is>
+          <t>1i3rowu</t>
+        </is>
+      </c>
+      <c r="B1101" t="inlineStr">
+        <is>
+          <t>What do you think of my chrome nails?</t>
+        </is>
+      </c>
+      <c r="C1101" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jhacomoakmde1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1102">
+      <c r="A1102" t="inlineStr">
+        <is>
+          <t>1i3rls9</t>
+        </is>
+      </c>
+      <c r="B1102" t="inlineStr">
+        <is>
+          <t>She Was Cold As Ice 🥶</t>
+        </is>
+      </c>
+      <c r="C1102" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/yj4n06imjmde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1103">
+      <c r="A1103" t="inlineStr">
+        <is>
+          <t>1i3qynq</t>
+        </is>
+      </c>
+      <c r="B1103" t="inlineStr">
+        <is>
+          <t>acrylic nail pain</t>
+        </is>
+      </c>
+      <c r="C1103" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/44k5i3ijemde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1104">
+      <c r="A1104" t="inlineStr">
+        <is>
+          <t>1i3r3gh</t>
+        </is>
+      </c>
+      <c r="B1104" t="inlineStr">
+        <is>
+          <t>Self-taught nail techs: what do you wish you knew when you first started?</t>
+        </is>
+      </c>
+      <c r="C1104" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i3r3gh/selftaught_nail_techs_what_do_you_wish_you_knew/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1105">
+      <c r="A1105" t="inlineStr">
+        <is>
+          <t>1i3r29w</t>
+        </is>
+      </c>
+      <c r="B1105" t="inlineStr">
+        <is>
+          <t>Matte black 💕</t>
+        </is>
+      </c>
+      <c r="C1105" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/uqvlcdlbfmde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1106">
+      <c r="A1106" t="inlineStr">
+        <is>
+          <t>1i3qw8q</t>
+        </is>
+      </c>
+      <c r="B1106" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This Is more my style. </t>
+        </is>
+      </c>
+      <c r="C1106" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i6b3dw90emde1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1107">
+      <c r="A1107" t="inlineStr">
+        <is>
+          <t>1i3qhjz</t>
+        </is>
+      </c>
+      <c r="B1107" t="inlineStr">
+        <is>
+          <t>My new nails!</t>
+        </is>
+      </c>
+      <c r="C1107" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jh3s4rgqamde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1108">
+      <c r="A1108" t="inlineStr">
+        <is>
+          <t>1i3qgxr</t>
+        </is>
+      </c>
+      <c r="B1108" t="inlineStr">
+        <is>
+          <t>Recent nails</t>
+        </is>
+      </c>
+      <c r="C1108" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3qgxr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1109">
+      <c r="A1109" t="inlineStr">
+        <is>
+          <t>1i3qbd1</t>
+        </is>
+      </c>
+      <c r="B1109" t="inlineStr">
+        <is>
+          <t>Best falsies for soft nails?</t>
+        </is>
+      </c>
+      <c r="C1109" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i3qbd1/best_falsies_for_soft_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1110">
+      <c r="A1110" t="inlineStr">
+        <is>
+          <t>1i3pl2p</t>
+        </is>
+      </c>
+      <c r="B1110" t="inlineStr">
+        <is>
+          <t>Uneven gel polish</t>
+        </is>
+      </c>
+      <c r="C1110" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3pl2p</t>
+        </is>
+      </c>
+    </row>
+    <row r="1111">
+      <c r="A1111" t="inlineStr">
+        <is>
+          <t>1i3pqoy</t>
+        </is>
+      </c>
+      <c r="B1111" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Is it bad to have back-to-back gels? </t>
+        </is>
+      </c>
+      <c r="C1111" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i3pqoy/is_it_bad_to_have_backtoback_gels/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1112">
+      <c r="A1112" t="inlineStr">
+        <is>
+          <t>1i3p88l</t>
+        </is>
+      </c>
+      <c r="B1112" t="inlineStr">
+        <is>
+          <t>Birthday nails -tried something new!</t>
+        </is>
+      </c>
+      <c r="C1112" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mpwbqgrv0mde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1113">
+      <c r="A1113" t="inlineStr">
+        <is>
+          <t>1i3ou3n</t>
+        </is>
+      </c>
+      <c r="B1113" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Feb purple nail inspo </t>
+        </is>
+      </c>
+      <c r="C1113" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gpy8wxltxlde1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1114">
+      <c r="A1114" t="inlineStr">
+        <is>
+          <t>1i3p0zg</t>
+        </is>
+      </c>
+      <c r="B1114" t="inlineStr">
+        <is>
+          <t>My first set</t>
+        </is>
+      </c>
+      <c r="C1114" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rxpzrzjazlde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1115">
+      <c r="A1115" t="inlineStr">
+        <is>
+          <t>1i3ooux</t>
+        </is>
+      </c>
+      <c r="B1115" t="inlineStr">
+        <is>
+          <t>Finally tried “cat eye”</t>
+        </is>
+      </c>
+      <c r="C1115" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5ti9q7tpwlde1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1116">
+      <c r="A1116" t="inlineStr">
+        <is>
+          <t>1i3ol5j</t>
+        </is>
+      </c>
+      <c r="B1116" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Butterfly nails </t>
+        </is>
+      </c>
+      <c r="C1116" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3ol5j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1117">
+      <c r="A1117" t="inlineStr">
+        <is>
+          <t>1i3oc5r</t>
+        </is>
+      </c>
+      <c r="B1117" t="inlineStr">
+        <is>
+          <t>Friday to pamper myself 🖤❤️❤️‍🔥🧛🏻‍♀️</t>
+        </is>
+      </c>
+      <c r="C1117" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3oc5r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1118">
+      <c r="A1118" t="inlineStr">
+        <is>
+          <t>1i3o21p</t>
+        </is>
+      </c>
+      <c r="B1118" t="inlineStr">
+        <is>
+          <t>Cat eye effect? What do you think?</t>
+        </is>
+      </c>
+      <c r="C1118" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vrw4j96trlde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1119">
+      <c r="A1119" t="inlineStr">
+        <is>
+          <t>1i3nxml</t>
+        </is>
+      </c>
+      <c r="B1119" t="inlineStr">
+        <is>
+          <t>First set of nails I made</t>
+        </is>
+      </c>
+      <c r="C1119" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3nxml</t>
+        </is>
+      </c>
+    </row>
+    <row r="1120">
+      <c r="A1120" t="inlineStr">
+        <is>
+          <t>1i3no39</t>
+        </is>
+      </c>
+      <c r="B1120" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What chrome powder do you guys use? </t>
+        </is>
+      </c>
+      <c r="C1120" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i3no39/what_chrome_powder_do_you_guys_use/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1121">
+      <c r="A1121" t="inlineStr">
+        <is>
+          <t>1i3njmu</t>
+        </is>
+      </c>
+      <c r="B1121" t="inlineStr">
+        <is>
+          <t>French with chrome</t>
+        </is>
+      </c>
+      <c r="C1121" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gsiltq9xnlde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1122">
+      <c r="A1122" t="inlineStr">
+        <is>
+          <t>1i3n7zp</t>
+        </is>
+      </c>
+      <c r="B1122" t="inlineStr">
+        <is>
+          <t>Fashion and nails</t>
+        </is>
+      </c>
+      <c r="C1122" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3n7zp</t>
+        </is>
+      </c>
+    </row>
+    <row r="1123">
+      <c r="A1123" t="inlineStr">
+        <is>
+          <t>1i3n4un</t>
+        </is>
+      </c>
+      <c r="B1123" t="inlineStr">
+        <is>
+          <t>Did my nails last night 💙</t>
+        </is>
+      </c>
+      <c r="C1123" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3n4un</t>
+        </is>
+      </c>
+    </row>
+    <row r="1124">
+      <c r="A1124" t="inlineStr">
+        <is>
+          <t>1i3n45r</t>
+        </is>
+      </c>
+      <c r="B1124" t="inlineStr">
+        <is>
+          <t>Basic but my second ever acrylic manicure, I'm addicted 💅🏻</t>
+        </is>
+      </c>
+      <c r="C1124" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q9bh5lonklde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1125">
+      <c r="A1125" t="inlineStr">
+        <is>
+          <t>1i3mpo8</t>
+        </is>
+      </c>
+      <c r="B1125" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did my own acrylics for the 2nd time </t>
+        </is>
+      </c>
+      <c r="C1125" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8s5holgmhlde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1126">
+      <c r="A1126" t="inlineStr">
+        <is>
+          <t>1i3mo6n</t>
+        </is>
+      </c>
+      <c r="B1126" t="inlineStr">
+        <is>
+          <t>How do we feel about the color?</t>
+        </is>
+      </c>
+      <c r="C1126" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3c1bhquahlde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1127">
+      <c r="A1127" t="inlineStr">
+        <is>
+          <t>1i3mckz</t>
+        </is>
+      </c>
+      <c r="B1127" t="inlineStr">
+        <is>
+          <t>A different kind of Valentine’s set ❤️‍🔥</t>
+        </is>
+      </c>
+      <c r="C1127" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3mckz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1128">
+      <c r="A1128" t="inlineStr">
+        <is>
+          <t>1i3m0ek</t>
+        </is>
+      </c>
+      <c r="B1128" t="inlineStr">
+        <is>
+          <t>Why does the same nail break in the same exact place?</t>
+        </is>
+      </c>
+      <c r="C1128" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i3m0ek/why_does_the_same_nail_break_in_the_same_exact/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1129">
+      <c r="A1129" t="inlineStr">
+        <is>
+          <t>1i3m1rb</t>
+        </is>
+      </c>
+      <c r="B1129" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I woke up with a vision.. </t>
+        </is>
+      </c>
+      <c r="C1129" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cbw7j46nclde1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1130">
+      <c r="A1130" t="inlineStr">
+        <is>
+          <t>1i3lz1q</t>
+        </is>
+      </c>
+      <c r="B1130" t="inlineStr">
+        <is>
+          <t>Got my nails done for the firt time!!</t>
+        </is>
+      </c>
+      <c r="C1130" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3lz1q</t>
+        </is>
+      </c>
+    </row>
+    <row r="1131">
+      <c r="A1131" t="inlineStr">
+        <is>
+          <t>1i3luvf</t>
+        </is>
+      </c>
+      <c r="B1131" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Professional Amazon eFile? </t>
+        </is>
+      </c>
+      <c r="C1131" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i3luvf/professional_amazon_efile/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1132">
+      <c r="A1132" t="inlineStr">
+        <is>
+          <t>1i3lszs</t>
+        </is>
+      </c>
+      <c r="B1132" t="inlineStr">
+        <is>
+          <t>Just the most beautiful shade of wine red 🥰</t>
+        </is>
+      </c>
+      <c r="C1132" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3lszs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1133">
+      <c r="A1133" t="inlineStr">
+        <is>
+          <t>1i3lnil</t>
+        </is>
+      </c>
+      <c r="B1133" t="inlineStr">
+        <is>
+          <t>Staining Oddities</t>
+        </is>
+      </c>
+      <c r="C1133" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i3lnil/staining_oddities/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1134">
+      <c r="A1134" t="inlineStr">
+        <is>
+          <t>1i3l0is</t>
+        </is>
+      </c>
+      <c r="B1134" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Nude polish recommendations </t>
+        </is>
+      </c>
+      <c r="C1134" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3l0is</t>
+        </is>
+      </c>
+    </row>
+    <row r="1135">
+      <c r="A1135" t="inlineStr">
+        <is>
+          <t>1i3kxl0</t>
+        </is>
+      </c>
+      <c r="B1135" t="inlineStr">
+        <is>
+          <t>Chocolate Chrome 🤎</t>
+        </is>
+      </c>
+      <c r="C1135" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3kxl0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1136">
+      <c r="A1136" t="inlineStr">
+        <is>
+          <t>1i3kqkf</t>
+        </is>
+      </c>
+      <c r="B1136" t="inlineStr">
+        <is>
+          <t>January Manicure💎👑</t>
+        </is>
+      </c>
+      <c r="C1136" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/errtzi7w2lde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1137">
+      <c r="A1137" t="inlineStr">
+        <is>
+          <t>1i3kjje</t>
+        </is>
+      </c>
+      <c r="B1137" t="inlineStr">
+        <is>
+          <t>Gelx attached with acrylic</t>
+        </is>
+      </c>
+      <c r="C1137" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i3kjje/gelx_attached_with_acrylic/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1138">
+      <c r="A1138" t="inlineStr">
+        <is>
+          <t>1i3jwcy</t>
+        </is>
+      </c>
+      <c r="B1138" t="inlineStr">
+        <is>
+          <t>How to fix my nails?</t>
+        </is>
+      </c>
+      <c r="C1138" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3jwcy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1139">
+      <c r="A1139" t="inlineStr">
+        <is>
+          <t>1i3jjit</t>
+        </is>
+      </c>
+      <c r="B1139" t="inlineStr">
+        <is>
+          <t>I love how shiny these are 😍</t>
+        </is>
+      </c>
+      <c r="C1139" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3jjit</t>
+        </is>
+      </c>
+    </row>
+    <row r="1140">
+      <c r="A1140" t="inlineStr">
+        <is>
+          <t>1i3jitk</t>
+        </is>
+      </c>
+      <c r="B1140" t="inlineStr">
+        <is>
+          <t>I love my nails</t>
+        </is>
+      </c>
+      <c r="C1140" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fmza4qbstkde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1141">
+      <c r="A1141" t="inlineStr">
+        <is>
+          <t>1i3cj50</t>
+        </is>
+      </c>
+      <c r="B1141" t="inlineStr">
+        <is>
+          <t>Help with nail glue</t>
+        </is>
+      </c>
+      <c r="C1141" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i3cj50/help_with_nail_glue/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1142">
+      <c r="A1142" t="inlineStr">
+        <is>
+          <t>1i3g63y</t>
+        </is>
+      </c>
+      <c r="B1142" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Under nail pain </t>
+        </is>
+      </c>
+      <c r="C1142" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i3g63y/under_nail_pain/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1143">
+      <c r="A1143" t="inlineStr">
+        <is>
+          <t>1i3hy4r</t>
+        </is>
+      </c>
+      <c r="B1143" t="inlineStr">
+        <is>
+          <t>Weak nails, rubber base not helping</t>
+        </is>
+      </c>
+      <c r="C1143" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jf3q2ia9hkde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1144">
+      <c r="A1144" t="inlineStr">
+        <is>
+          <t>1i3az3b</t>
+        </is>
+      </c>
+      <c r="B1144" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Officially freaked out about developing gel allergy but how can I still get nice nails? </t>
+        </is>
+      </c>
+      <c r="C1144" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i3az3b/officially_freaked_out_about_developing_gel/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1145">
+      <c r="A1145" t="inlineStr">
+        <is>
+          <t>1i3irsz</t>
+        </is>
+      </c>
+      <c r="B1145" t="inlineStr">
+        <is>
+          <t xml:space="preserve">These picture frames though </t>
+        </is>
+      </c>
+      <c r="C1145" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/67mbtxwunkde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1146">
+      <c r="A1146" t="inlineStr">
+        <is>
+          <t>1i3iq1o</t>
+        </is>
+      </c>
+      <c r="B1146" t="inlineStr">
+        <is>
+          <t>My nails match my scrunchie</t>
+        </is>
+      </c>
+      <c r="C1146" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fg0ayjognkde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1147">
+      <c r="A1147" t="inlineStr">
+        <is>
+          <t>1i3i9fg</t>
+        </is>
+      </c>
+      <c r="B1147" t="inlineStr">
+        <is>
+          <t xml:space="preserve">A set I did last year I might redo again because I loved it so much 🤍🎀 </t>
+        </is>
+      </c>
+      <c r="C1147" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ayteez6tjkde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1148">
+      <c r="A1148" t="inlineStr">
+        <is>
+          <t>1i3i4ku</t>
+        </is>
+      </c>
+      <c r="B1148" t="inlineStr">
+        <is>
+          <t>My french tip practice from right to left</t>
+        </is>
+      </c>
+      <c r="C1148" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/krcoszorikde1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1149">
+      <c r="A1149" t="inlineStr">
+        <is>
+          <t>1i3hkzg</t>
+        </is>
+      </c>
+      <c r="B1149" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Engagement Nails </t>
+        </is>
+      </c>
+      <c r="C1149" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i3hkzg/engagement_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1150">
+      <c r="A1150" t="inlineStr">
+        <is>
+          <t>1i3hclm</t>
+        </is>
+      </c>
+      <c r="B1150" t="inlineStr">
+        <is>
+          <t>Almond or coffin?</t>
+        </is>
+      </c>
+      <c r="C1150" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3hclm</t>
+        </is>
+      </c>
+    </row>
+    <row r="1151">
+      <c r="A1151" t="inlineStr">
+        <is>
+          <t>1i3h9cb</t>
+        </is>
+      </c>
+      <c r="B1151" t="inlineStr">
+        <is>
+          <t>Gel alternative I can do myself (UK)</t>
+        </is>
+      </c>
+      <c r="C1151" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i3h9cb/gel_alternative_i_can_do_myself_uk/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1152">
+      <c r="A1152" t="inlineStr">
+        <is>
+          <t>1i3gxa6</t>
+        </is>
+      </c>
+      <c r="B1152" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love these from Halloween </t>
+        </is>
+      </c>
+      <c r="C1152" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/u5td3hjj8kde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1153">
+      <c r="A1153" t="inlineStr">
+        <is>
+          <t>1i42qfo</t>
+        </is>
+      </c>
+      <c r="B1153" t="inlineStr">
+        <is>
+          <t>Glossy or Matte?</t>
+        </is>
+      </c>
+      <c r="C1153" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i42qfo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1154">
+      <c r="A1154" t="inlineStr">
+        <is>
+          <t>1i42gnv</t>
+        </is>
+      </c>
+      <c r="B1154" t="inlineStr">
+        <is>
+          <t>Ocean Vibes</t>
+        </is>
+      </c>
+      <c r="C1154" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i42gnv</t>
+        </is>
+      </c>
+    </row>
+    <row r="1155">
+      <c r="A1155" t="inlineStr">
+        <is>
+          <t>1i42bfw</t>
+        </is>
+      </c>
+      <c r="B1155" t="inlineStr">
+        <is>
+          <t>Did my Friend’s Nails! Builder Gel on Natural Nails.</t>
+        </is>
+      </c>
+      <c r="C1155" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pecifhy4fpde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1156">
+      <c r="A1156" t="inlineStr">
+        <is>
+          <t>1i4270a</t>
+        </is>
+      </c>
+      <c r="B1156" t="inlineStr">
+        <is>
+          <t>Love this colour</t>
+        </is>
+      </c>
+      <c r="C1156" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4270a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1157">
+      <c r="A1157" t="inlineStr">
+        <is>
+          <t>1i40kov</t>
+        </is>
+      </c>
+      <c r="B1157" t="inlineStr">
+        <is>
+          <t>Is Builder Gel Cured under Press-Ons okay?</t>
+        </is>
+      </c>
+      <c r="C1157" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i40kov/is_builder_gel_cured_under_pressons_okay/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1158">
+      <c r="A1158" t="inlineStr">
+        <is>
+          <t>1i4022f</t>
+        </is>
+      </c>
+      <c r="B1158" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How do y’all organize your collection? </t>
+        </is>
+      </c>
+      <c r="C1158" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pnymoshdoode1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1159">
+      <c r="A1159" t="inlineStr">
+        <is>
+          <t>1i400o1</t>
+        </is>
+      </c>
+      <c r="B1159" t="inlineStr">
+        <is>
+          <t>Mooncat's Hardcore Basecoat</t>
+        </is>
+      </c>
+      <c r="C1159" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i400o1/mooncats_hardcore_basecoat/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1160">
+      <c r="A1160" t="inlineStr">
+        <is>
+          <t>1i3zose</t>
+        </is>
+      </c>
+      <c r="B1160" t="inlineStr">
+        <is>
+          <t>Swallow Your Tongue!</t>
+        </is>
+      </c>
+      <c r="C1160" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/eq40eqp9kode1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1161">
+      <c r="A1161" t="inlineStr">
+        <is>
+          <t>1i3zfi7</t>
+        </is>
+      </c>
+      <c r="B1161" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Polish wrinkles after shower? </t>
+        </is>
+      </c>
+      <c r="C1161" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/39vv2rvhhode1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1162">
+      <c r="A1162" t="inlineStr">
+        <is>
+          <t>1i3z2db</t>
+        </is>
+      </c>
+      <c r="B1162" t="inlineStr">
+        <is>
+          <t>Crispy Freezey January</t>
+        </is>
+      </c>
+      <c r="C1162" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3z2db</t>
+        </is>
+      </c>
+    </row>
+    <row r="1163">
+      <c r="A1163" t="inlineStr">
+        <is>
+          <t>1i3yo6d</t>
+        </is>
+      </c>
+      <c r="B1163" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Removing these today after 2 weeks ❤️ </t>
+        </is>
+      </c>
+      <c r="C1163" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/5qivv0sq9ode1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1164">
+      <c r="A1164" t="inlineStr">
+        <is>
+          <t>1i3yclk</t>
+        </is>
+      </c>
+      <c r="B1164" t="inlineStr">
+        <is>
+          <t>another day, another manicure 🩵</t>
+        </is>
+      </c>
+      <c r="C1164" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3yclk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1165">
+      <c r="A1165" t="inlineStr">
+        <is>
+          <t>1i3wsvz</t>
+        </is>
+      </c>
+      <c r="B1165" t="inlineStr">
+        <is>
+          <t>Mooncat Thermal Queen of the Damned</t>
+        </is>
+      </c>
+      <c r="C1165" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3wsvz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1166">
+      <c r="A1166" t="inlineStr">
+        <is>
+          <t>1i3wk2f</t>
+        </is>
+      </c>
+      <c r="B1166" t="inlineStr">
+        <is>
+          <t>HoH formula in other colors?</t>
+        </is>
+      </c>
+      <c r="C1166" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i3wk2f/hoh_formula_in_other_colors/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1167">
+      <c r="A1167" t="inlineStr">
+        <is>
+          <t>1i3we4n</t>
+        </is>
+      </c>
+      <c r="B1167" t="inlineStr">
+        <is>
+          <t>Are you all using press on nails?</t>
+        </is>
+      </c>
+      <c r="C1167" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i3we4n/are_you_all_using_press_on_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1168">
+      <c r="A1168" t="inlineStr">
+        <is>
+          <t>1i3wdj0</t>
+        </is>
+      </c>
+      <c r="B1168" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Very unique polish- Freddy vs Jason, Luna Lacquer </t>
+        </is>
+      </c>
+      <c r="C1168" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3wdj0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1169">
+      <c r="A1169" t="inlineStr">
+        <is>
+          <t>1i3wc19</t>
+        </is>
+      </c>
+      <c r="B1169" t="inlineStr">
+        <is>
+          <t>I'm in love with this nail polish 😩</t>
+        </is>
+      </c>
+      <c r="C1169" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3wc19</t>
+        </is>
+      </c>
+    </row>
+    <row r="1170">
+      <c r="A1170" t="inlineStr">
+        <is>
+          <t>1i3w8xn</t>
+        </is>
+      </c>
+      <c r="B1170" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I Scream Nails - Death by Rainbow. What am I doing wrong?! More in body text </t>
+        </is>
+      </c>
+      <c r="C1170" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3w8xn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1171">
+      <c r="A1171" t="inlineStr">
+        <is>
+          <t>1i3vq5g</t>
+        </is>
+      </c>
+      <c r="B1171" t="inlineStr">
+        <is>
+          <t>Redoing a nail that chipped and may have accidentally created a vibe</t>
+        </is>
+      </c>
+      <c r="C1171" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wsbnkl7whnde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1172">
+      <c r="A1172" t="inlineStr">
+        <is>
+          <t>1i3vkfz</t>
+        </is>
+      </c>
+      <c r="B1172" t="inlineStr">
+        <is>
+          <t>Essie Smooth-E. (What is this stuff?)</t>
+        </is>
+      </c>
+      <c r="C1172" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i3vkfz/essie_smoothe_what_is_this_stuff/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1173">
+      <c r="A1173" t="inlineStr">
+        <is>
+          <t>1i3vcjf</t>
+        </is>
+      </c>
+      <c r="B1173" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time using restore </t>
+        </is>
+      </c>
+      <c r="C1173" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i3vcjf/first_time_using_restore/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1174">
+      <c r="A1174" t="inlineStr">
+        <is>
+          <t>1i3u3ar</t>
+        </is>
+      </c>
+      <c r="B1174" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Any good nude magnetic lacquer? </t>
+        </is>
+      </c>
+      <c r="C1174" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i3u3ar/any_good_nude_magnetic_lacquer/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1175">
+      <c r="A1175" t="inlineStr">
+        <is>
+          <t>1i3twzt</t>
+        </is>
+      </c>
+      <c r="B1175" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How to begin! </t>
+        </is>
+      </c>
+      <c r="C1175" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i3twzt/how_to_begin/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1176">
+      <c r="A1176" t="inlineStr">
+        <is>
+          <t>1i3tf4r</t>
+        </is>
+      </c>
+      <c r="B1176" t="inlineStr">
+        <is>
+          <t>Polish lovers from US, please help</t>
+        </is>
+      </c>
+      <c r="C1176" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i3tf4r/polish_lovers_from_us_please_help/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1177">
+      <c r="A1177" t="inlineStr">
+        <is>
+          <t>1i3taur</t>
+        </is>
+      </c>
+      <c r="B1177" t="inlineStr">
+        <is>
+          <t>I didn't review my cart carefully while BF shopping and ended up with duplicates</t>
+        </is>
+      </c>
+      <c r="C1177" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8mgoyfx7xmde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1178">
+      <c r="A1178" t="inlineStr">
+        <is>
+          <t>1i3t9b1</t>
+        </is>
+      </c>
+      <c r="B1178" t="inlineStr">
+        <is>
+          <t>ILNP Starlight</t>
+        </is>
+      </c>
+      <c r="C1178" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oibe5u4vwmde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1179">
+      <c r="A1179" t="inlineStr">
+        <is>
+          <t>1i3t25e</t>
+        </is>
+      </c>
+      <c r="B1179" t="inlineStr">
+        <is>
+          <t>Looking for a nail polish that looks like this chocolate wraps!  👇</t>
+        </is>
+      </c>
+      <c r="C1179" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9jn13gc7vmde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1180">
+      <c r="A1180" t="inlineStr">
+        <is>
+          <t>1i3sz8y</t>
+        </is>
+      </c>
+      <c r="B1180" t="inlineStr">
+        <is>
+          <t>Oooh, we have a glower.</t>
+        </is>
+      </c>
+      <c r="C1180" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3sz8y</t>
+        </is>
+      </c>
+    </row>
+    <row r="1181">
+      <c r="A1181" t="inlineStr">
+        <is>
+          <t>1i3shw7</t>
+        </is>
+      </c>
+      <c r="B1181" t="inlineStr">
+        <is>
+          <t>i was worried this wouldn’t be my color and it 100% isn’t 😅</t>
+        </is>
+      </c>
+      <c r="C1181" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3shw7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1182">
+      <c r="A1182" t="inlineStr">
+        <is>
+          <t>1i3rids</t>
+        </is>
+      </c>
+      <c r="B1182" t="inlineStr">
+        <is>
+          <t>Galaxy nails 🌌</t>
+        </is>
+      </c>
+      <c r="C1182" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3rids</t>
+        </is>
+      </c>
+    </row>
+    <row r="1183">
+      <c r="A1183" t="inlineStr">
+        <is>
+          <t>1i3rewr</t>
+        </is>
+      </c>
+      <c r="B1183" t="inlineStr">
+        <is>
+          <t>What brand(s) are you drawn to most in your collection? What do you neglect?</t>
+        </is>
+      </c>
+      <c r="C1183" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i3rewr/what_brands_are_you_drawn_to_most_in_your/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1184">
+      <c r="A1184" t="inlineStr">
+        <is>
+          <t>1i3raz9</t>
+        </is>
+      </c>
+      <c r="B1184" t="inlineStr">
+        <is>
+          <t>What's an older polish that still makes you say "wow"?</t>
+        </is>
+      </c>
+      <c r="C1184" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i3raz9/whats_an_older_polish_that_still_makes_you_say_wow/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1185">
+      <c r="A1185" t="inlineStr">
+        <is>
+          <t>1i3r386</t>
+        </is>
+      </c>
+      <c r="B1185" t="inlineStr">
+        <is>
+          <t xml:space="preserve">KBShimmer Along For The Ride and Northern Frights </t>
+        </is>
+      </c>
+      <c r="C1185" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3r386</t>
+        </is>
+      </c>
+    </row>
+    <row r="1186">
+      <c r="A1186" t="inlineStr">
+        <is>
+          <t>1i3r348</t>
+        </is>
+      </c>
+      <c r="B1186" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ozmopolitan </t>
+        </is>
+      </c>
+      <c r="C1186" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3r348</t>
+        </is>
+      </c>
+    </row>
+    <row r="1187">
+      <c r="A1187" t="inlineStr">
+        <is>
+          <t>1i3qhzi</t>
+        </is>
+      </c>
+      <c r="B1187" t="inlineStr">
+        <is>
+          <t>True Love’s First Kiss by Cirque Colors 🐸👑💋</t>
+        </is>
+      </c>
+      <c r="C1187" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3qhzi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1188">
+      <c r="A1188" t="inlineStr">
+        <is>
+          <t>1i3q7vo</t>
+        </is>
+      </c>
+      <c r="B1188" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Fiduciary Responsibility is a Stunner! </t>
+        </is>
+      </c>
+      <c r="C1188" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3q7vo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1189">
+      <c r="A1189" t="inlineStr">
+        <is>
+          <t>1i3q4m9</t>
+        </is>
+      </c>
+      <c r="B1189" t="inlineStr">
+        <is>
+          <t>Super fine reflective glitter?</t>
+        </is>
+      </c>
+      <c r="C1189" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i3q4m9/super_fine_reflective_glitter/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1190">
+      <c r="A1190" t="inlineStr">
+        <is>
+          <t>1i3po2x</t>
+        </is>
+      </c>
+      <c r="B1190" t="inlineStr">
+        <is>
+          <t>Pi Colours Red Glow just another red black multichrome?</t>
+        </is>
+      </c>
+      <c r="C1190" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i3po2x/pi_colours_red_glow_just_another_red_black/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1191">
+      <c r="A1191" t="inlineStr">
+        <is>
+          <t>1i3pceq</t>
+        </is>
+      </c>
+      <c r="B1191" t="inlineStr">
+        <is>
+          <t>Orly - Sale on Bundles (6 polish sets for $25)</t>
+        </is>
+      </c>
+      <c r="C1191" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i3pceq/orly_sale_on_bundles_6_polish_sets_for_25/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1192">
+      <c r="A1192" t="inlineStr">
+        <is>
+          <t>1i3pc30</t>
+        </is>
+      </c>
+      <c r="B1192" t="inlineStr">
+        <is>
+          <t>Replacement Handles for Mooncat Polishes?</t>
+        </is>
+      </c>
+      <c r="C1192" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i3pc30/replacement_handles_for_mooncat_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1193">
+      <c r="A1193" t="inlineStr">
+        <is>
+          <t>1i3ozc7</t>
+        </is>
+      </c>
+      <c r="B1193" t="inlineStr">
+        <is>
+          <t>Fun nail stores near Phoenix, AZ?</t>
+        </is>
+      </c>
+      <c r="C1193" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i3ozc7/fun_nail_stores_near_phoenix_az/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1194">
+      <c r="A1194" t="inlineStr">
+        <is>
+          <t>1i3orw0</t>
+        </is>
+      </c>
+      <c r="B1194" t="inlineStr">
+        <is>
+          <t xml:space="preserve">This is THE coolest polish I think I’ve ever seen. Any similar polishes that you all can recommend? Details in body text. </t>
+        </is>
+      </c>
+      <c r="C1194" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/75qqk9vcxlde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1195">
+      <c r="A1195" t="inlineStr">
+        <is>
+          <t>1i3o1c2</t>
+        </is>
+      </c>
+      <c r="B1195" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Basecoat Battle Round One: </t>
+        </is>
+      </c>
+      <c r="C1195" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/r7bjfi1nrlde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1196">
+      <c r="A1196" t="inlineStr">
+        <is>
+          <t>1i3ny4a</t>
+        </is>
+      </c>
+      <c r="B1196" t="inlineStr">
+        <is>
+          <t>So, Swatches...</t>
+        </is>
+      </c>
+      <c r="C1196" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i3ny4a/so_swatches/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1197">
+      <c r="A1197" t="inlineStr">
+        <is>
+          <t>1i3nqjx</t>
+        </is>
+      </c>
+      <c r="B1197" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Ancient Being, Elbe - HHC November </t>
+        </is>
+      </c>
+      <c r="C1197" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3nqjx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1198">
+      <c r="A1198" t="inlineStr">
+        <is>
+          <t>1i3n7rx</t>
+        </is>
+      </c>
+      <c r="B1198" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Two weeks of wear without base coat! </t>
+        </is>
+      </c>
+      <c r="C1198" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/i78bgvffllde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1199">
+      <c r="A1199" t="inlineStr">
+        <is>
+          <t>1i3n23r</t>
+        </is>
+      </c>
+      <c r="B1199" t="inlineStr">
+        <is>
+          <t>Butterfly sparkles ✨🦋</t>
+        </is>
+      </c>
+      <c r="C1199" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3m8h1m28klde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1200">
+      <c r="A1200" t="inlineStr">
+        <is>
+          <t>1i3mlad</t>
+        </is>
+      </c>
+      <c r="B1200" t="inlineStr">
+        <is>
+          <t>Ready for some Trek with Jen &amp; Berries "There are Four Lights" from PPU</t>
+        </is>
+      </c>
+      <c r="C1200" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3mlad</t>
+        </is>
+      </c>
+    </row>
+    <row r="1201">
+      <c r="A1201" t="inlineStr">
+        <is>
+          <t>1i3mi1n</t>
+        </is>
+      </c>
+      <c r="B1201" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Can’t find this glitter online for my life! Pinterest comments aren’t helpful. </t>
+        </is>
+      </c>
+      <c r="C1201" t="inlineStr">
+        <is>
+          <t>https://pin.it/338iCeyoc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1202">
+      <c r="A1202" t="inlineStr">
+        <is>
+          <t>1i3mfxk</t>
+        </is>
+      </c>
+      <c r="B1202" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Leveling up your technique </t>
+        </is>
+      </c>
+      <c r="C1202" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i3mfxk/leveling_up_your_technique/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1203">
+      <c r="A1203" t="inlineStr">
+        <is>
+          <t>1i3mdki</t>
+        </is>
+      </c>
+      <c r="B1203" t="inlineStr">
+        <is>
+          <t>I feel like an ice princess!</t>
+        </is>
+      </c>
+      <c r="C1203" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3mdki</t>
+        </is>
+      </c>
+    </row>
+    <row r="1204">
+      <c r="A1204" t="inlineStr">
+        <is>
+          <t>1i3lzu6</t>
+        </is>
+      </c>
+      <c r="B1204" t="inlineStr">
+        <is>
+          <t>Staining Oddities</t>
+        </is>
+      </c>
+      <c r="C1204" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i3lzu6/staining_oddities/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1205">
+      <c r="A1205" t="inlineStr">
+        <is>
+          <t>1i3lmrc</t>
+        </is>
+      </c>
+      <c r="B1205" t="inlineStr">
+        <is>
+          <t>Zoya Dream</t>
+        </is>
+      </c>
+      <c r="C1205" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3lmrc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1206">
+      <c r="A1206" t="inlineStr">
+        <is>
+          <t>1i3lj7j</t>
+        </is>
+      </c>
+      <c r="B1206" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did my nails last night….. hate them </t>
+        </is>
+      </c>
+      <c r="C1206" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3lj7j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1207">
+      <c r="A1207" t="inlineStr">
+        <is>
+          <t>1i3la19</t>
+        </is>
+      </c>
+      <c r="B1207" t="inlineStr">
+        <is>
+          <t>If you like flower child…</t>
+        </is>
+      </c>
+      <c r="C1207" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1hzpqqj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1208">
+      <c r="A1208" t="inlineStr">
+        <is>
+          <t>1i3l8nz</t>
+        </is>
+      </c>
+      <c r="B1208" t="inlineStr">
+        <is>
+          <t>Case of the winter blues called for some rainbow chaos</t>
+        </is>
+      </c>
+      <c r="C1208" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3l8nz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1209">
+      <c r="A1209" t="inlineStr">
+        <is>
+          <t>1i3l8ar</t>
+        </is>
+      </c>
+      <c r="B1209" t="inlineStr">
+        <is>
+          <t>Silvergrass is the ethereal fairy polish of my dreams ✨🧚🏻‍♂️🌷💖🌙✨</t>
+        </is>
+      </c>
+      <c r="C1209" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3l8ar</t>
+        </is>
+      </c>
+    </row>
+    <row r="1210">
+      <c r="A1210" t="inlineStr">
+        <is>
+          <t>1i3l78t</t>
+        </is>
+      </c>
+      <c r="B1210" t="inlineStr">
+        <is>
+          <t>Not sure if I like but it’s grew on me.</t>
+        </is>
+      </c>
+      <c r="C1210" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/o1uh8ama6lde1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1211">
+      <c r="A1211" t="inlineStr">
+        <is>
+          <t>1i3kluy</t>
+        </is>
+      </c>
+      <c r="B1211" t="inlineStr">
+        <is>
+          <t>Thank you from the bottom of my sparkly heart</t>
+        </is>
+      </c>
+      <c r="C1211" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/pzhl5efx1lde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1212">
+      <c r="A1212" t="inlineStr">
+        <is>
+          <t>1i3kcpc</t>
+        </is>
+      </c>
+      <c r="B1212" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Unicorn + Day Glow = Bright Perfection </t>
+        </is>
+      </c>
+      <c r="C1212" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3kcpc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1213">
+      <c r="A1213" t="inlineStr">
+        <is>
+          <t>1i3k5ko</t>
+        </is>
+      </c>
+      <c r="B1213" t="inlineStr">
+        <is>
+          <t>My first ILNP 💜</t>
+        </is>
+      </c>
+      <c r="C1213" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wtpg26dkykde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1214">
+      <c r="A1214" t="inlineStr">
+        <is>
+          <t>1i3k55r</t>
+        </is>
+      </c>
+      <c r="B1214" t="inlineStr">
+        <is>
+          <t>Looking for the perfect pale pink…</t>
+        </is>
+      </c>
+      <c r="C1214" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i3k55r/looking_for_the_perfect_pale_pink/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1215">
+      <c r="A1215" t="inlineStr">
+        <is>
+          <t>1i3jmey</t>
+        </is>
+      </c>
+      <c r="B1215" t="inlineStr">
+        <is>
+          <t>Zoya skittles</t>
+        </is>
+      </c>
+      <c r="C1215" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nf6fav1jukde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1216">
+      <c r="A1216" t="inlineStr">
+        <is>
+          <t>1i3iyqq</t>
+        </is>
+      </c>
+      <c r="B1216" t="inlineStr">
+        <is>
+          <t>ILNP Funhouse</t>
+        </is>
+      </c>
+      <c r="C1216" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1nn034pepkde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1217">
+      <c r="A1217" t="inlineStr">
+        <is>
+          <t>1i3iwmc</t>
+        </is>
+      </c>
+      <c r="B1217" t="inlineStr">
+        <is>
+          <t>Tectonic Shift/Mooncat 😍</t>
+        </is>
+      </c>
+      <c r="C1217" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3iwmc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1218">
+      <c r="A1218" t="inlineStr">
+        <is>
+          <t>1i3h82s</t>
+        </is>
+      </c>
+      <c r="B1218" t="inlineStr">
+        <is>
+          <t xml:space="preserve">W7 One coat chrome </t>
+        </is>
+      </c>
+      <c r="C1218" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3h82s</t>
+        </is>
+      </c>
+    </row>
+    <row r="1219">
+      <c r="A1219" t="inlineStr">
+        <is>
+          <t>1i3h7oq</t>
+        </is>
+      </c>
+      <c r="B1219" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Any recs for bright, yellow-toned greens like the ones pictured? </t>
+        </is>
+      </c>
+      <c r="C1219" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3h7oq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1220">
+      <c r="A1220" t="inlineStr">
+        <is>
+          <t>1i3gplp</t>
+        </is>
+      </c>
+      <c r="B1220" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Reflections </t>
+        </is>
+      </c>
+      <c r="C1220" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/3opch5kh6kde1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1221">
+      <c r="A1221" t="inlineStr">
+        <is>
+          <t>1i3gge8</t>
+        </is>
+      </c>
+      <c r="B1221" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Belugaria accent ✨ </t>
+        </is>
+      </c>
+      <c r="C1221" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jenfi6x74kde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1222">
+      <c r="A1222" t="inlineStr">
+        <is>
+          <t>1i3f9pw</t>
+        </is>
+      </c>
+      <c r="B1222" t="inlineStr">
+        <is>
+          <t>Ethereal Lacquer Obscure as a topper?</t>
+        </is>
+      </c>
+      <c r="C1222" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i3f9pw/ethereal_lacquer_obscure_as_a_topper/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1223">
+      <c r="A1223" t="inlineStr">
+        <is>
+          <t>1i3f8mo</t>
+        </is>
+      </c>
+      <c r="B1223" t="inlineStr">
+        <is>
+          <t xml:space="preserve">DAM Polish- Chicago River </t>
+        </is>
+      </c>
+      <c r="C1223" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9dmnne97sjde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1224">
+      <c r="A1224" t="inlineStr">
+        <is>
+          <t>1i3f0bs</t>
+        </is>
+      </c>
+      <c r="B1224" t="inlineStr">
+        <is>
+          <t>You Do Blue</t>
+        </is>
+      </c>
+      <c r="C1224" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3f0bs</t>
+        </is>
+      </c>
+    </row>
+    <row r="1225">
+      <c r="A1225" t="inlineStr">
+        <is>
+          <t>1i3ectd</t>
+        </is>
+      </c>
+      <c r="B1225" t="inlineStr">
+        <is>
+          <t>January refresh</t>
+        </is>
+      </c>
+      <c r="C1225" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/n1u46b8aijde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1226">
+      <c r="A1226" t="inlineStr">
+        <is>
+          <t>1i3eab6</t>
+        </is>
+      </c>
+      <c r="B1226" t="inlineStr">
+        <is>
+          <t>such a pretty brown from The Gel Bottle Inc</t>
+        </is>
+      </c>
+      <c r="C1226" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tyrx7cihhjde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1227">
+      <c r="A1227" t="inlineStr">
+        <is>
+          <t>1i3drkc</t>
+        </is>
+      </c>
+      <c r="B1227" t="inlineStr">
+        <is>
+          <t>shattered glass</t>
+        </is>
+      </c>
+      <c r="C1227" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8cyom235bjde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1228">
+      <c r="A1228" t="inlineStr">
+        <is>
+          <t>1i346ux</t>
+        </is>
+      </c>
+      <c r="B1228" t="inlineStr">
+        <is>
+          <t>Goth/grunge indie brand recs?</t>
+        </is>
+      </c>
+      <c r="C1228" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i346ux/gothgrunge_indie_brand_recs/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1229">
+      <c r="A1229" t="inlineStr">
+        <is>
+          <t>1i3bqkw</t>
+        </is>
+      </c>
+      <c r="B1229" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Sweater nails so I can pretend my nails feel warm and cozy </t>
+        </is>
+      </c>
+      <c r="C1229" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/birdvu7fjide1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1230">
+      <c r="A1230" t="inlineStr">
+        <is>
+          <t>1i42rs7</t>
+        </is>
+      </c>
+      <c r="B1230" t="inlineStr">
+        <is>
+          <t>Blooming jail</t>
+        </is>
+      </c>
+      <c r="C1230" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/imvzfej6lpde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1231">
+      <c r="A1231" t="inlineStr">
+        <is>
+          <t>1i42hz9</t>
+        </is>
+      </c>
+      <c r="B1231" t="inlineStr">
+        <is>
+          <t>Ocean Vibes</t>
+        </is>
+      </c>
+      <c r="C1231" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i42hz9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1232">
+      <c r="A1232" t="inlineStr">
+        <is>
+          <t>1i42dhu</t>
+        </is>
+      </c>
+      <c r="B1232" t="inlineStr">
+        <is>
+          <t>first gel x set ever!</t>
+        </is>
+      </c>
+      <c r="C1232" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zkrj4q1vfpde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1233">
+      <c r="A1233" t="inlineStr">
+        <is>
+          <t>1i41pj2</t>
+        </is>
+      </c>
+      <c r="B1233" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First tries </t>
+        </is>
+      </c>
+      <c r="C1233" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wg7jng1h7pde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1234">
+      <c r="A1234" t="inlineStr">
+        <is>
+          <t>1i40i9s</t>
+        </is>
+      </c>
+      <c r="B1234" t="inlineStr">
+        <is>
+          <t>What kind of glue works best for nail charms?</t>
+        </is>
+      </c>
+      <c r="C1234" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tc5tb1e7tode1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1235">
+      <c r="A1235" t="inlineStr">
+        <is>
+          <t>1i3zyf5</t>
+        </is>
+      </c>
+      <c r="B1235" t="inlineStr">
+        <is>
+          <t xml:space="preserve">getting things out of budget </t>
+        </is>
+      </c>
+      <c r="C1235" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1i3zyf5/getting_things_out_of_budget/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1236">
+      <c r="A1236" t="inlineStr">
+        <is>
+          <t>1i3yu1i</t>
+        </is>
+      </c>
+      <c r="B1236" t="inlineStr">
+        <is>
+          <t>Scooby doo</t>
+        </is>
+      </c>
+      <c r="C1236" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gpr0irhdbode1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1237">
+      <c r="A1237" t="inlineStr">
+        <is>
+          <t>1i3ykxk</t>
+        </is>
+      </c>
+      <c r="B1237" t="inlineStr">
+        <is>
+          <t>Ready for the FREEZE ❄️🥶</t>
+        </is>
+      </c>
+      <c r="C1237" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3ykxk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1238">
+      <c r="A1238" t="inlineStr">
+        <is>
+          <t>1i3xtlx</t>
+        </is>
+      </c>
+      <c r="B1238" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First set! </t>
+        </is>
+      </c>
+      <c r="C1238" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xxo3cngc1ode1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1239">
+      <c r="A1239" t="inlineStr">
+        <is>
+          <t>1i3xbng</t>
+        </is>
+      </c>
+      <c r="B1239" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Anyone familiar with this? </t>
+        </is>
+      </c>
+      <c r="C1239" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wg42lr2kwnde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1240">
+      <c r="A1240" t="inlineStr">
+        <is>
+          <t>1i3wrzx</t>
+        </is>
+      </c>
+      <c r="B1240" t="inlineStr">
+        <is>
+          <t>My second EVER nail set- Mom already negative towards it..</t>
+        </is>
+      </c>
+      <c r="C1240" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3wrzx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1241">
+      <c r="A1241" t="inlineStr">
+        <is>
+          <t>1i3w294</t>
+        </is>
+      </c>
+      <c r="B1241" t="inlineStr">
+        <is>
+          <t>good top coat recommendations</t>
+        </is>
+      </c>
+      <c r="C1241" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1i3w294/good_top_coat_recommendations/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1242">
+      <c r="A1242" t="inlineStr">
+        <is>
+          <t>1i3uvn2</t>
+        </is>
+      </c>
+      <c r="B1242" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I have a rather weird gel polish request. </t>
+        </is>
+      </c>
+      <c r="C1242" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1i3uvn2/i_have_a_rather_weird_gel_polish_request/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1243">
+      <c r="A1243" t="inlineStr">
+        <is>
+          <t>1i3tnoc</t>
+        </is>
+      </c>
+      <c r="B1243" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love notes 🩷📝 Valentine’s Day nail set done by my queen nails_emmywynn on IG! </t>
+        </is>
+      </c>
+      <c r="C1243" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/kfbfcm660nde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1244">
+      <c r="A1244" t="inlineStr">
+        <is>
+          <t>1i3thq8</t>
+        </is>
+      </c>
+      <c r="B1244" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I started learning nail art a few months ago and did these on myself with gold foil </t>
+        </is>
+      </c>
+      <c r="C1244" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3thq8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1245">
+      <c r="A1245" t="inlineStr">
+        <is>
+          <t>1i3t6of</t>
+        </is>
+      </c>
+      <c r="B1245" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I love different </t>
+        </is>
+      </c>
+      <c r="C1245" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3t6of</t>
+        </is>
+      </c>
+    </row>
+    <row r="1246">
+      <c r="A1246" t="inlineStr">
+        <is>
+          <t>1i3rsgr</t>
+        </is>
+      </c>
+      <c r="B1246" t="inlineStr">
+        <is>
+          <t>anti vday conversation hearts 🗡️</t>
+        </is>
+      </c>
+      <c r="C1246" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3rsgr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1247">
+      <c r="A1247" t="inlineStr">
+        <is>
+          <t>1i3nmpv</t>
+        </is>
+      </c>
+      <c r="B1247" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What chrome powder do you guys use? </t>
+        </is>
+      </c>
+      <c r="C1247" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/NailArt/comments/1i3nmpv/what_chrome_powder_do_you_guys_use/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1248">
+      <c r="A1248" t="inlineStr">
+        <is>
+          <t>1i3nk3r</t>
+        </is>
+      </c>
+      <c r="B1248" t="inlineStr">
+        <is>
+          <t>First timer!</t>
+        </is>
+      </c>
+      <c r="C1248" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3nk3r</t>
+        </is>
+      </c>
+    </row>
+    <row r="1249">
+      <c r="A1249" t="inlineStr">
+        <is>
+          <t>1i3n4oo</t>
+        </is>
+      </c>
+      <c r="B1249" t="inlineStr">
+        <is>
+          <t>Fashion and nails 2</t>
+        </is>
+      </c>
+      <c r="C1249" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3n4oo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1250">
+      <c r="A1250" t="inlineStr">
+        <is>
+          <t>1i3n3qy</t>
+        </is>
+      </c>
+      <c r="B1250" t="inlineStr">
+        <is>
+          <t>Pink fire 💖🔥</t>
+        </is>
+      </c>
+      <c r="C1250" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/f8py5j4kklde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1251">
+      <c r="A1251" t="inlineStr">
+        <is>
+          <t>1i3kzrn</t>
+        </is>
+      </c>
+      <c r="B1251" t="inlineStr">
+        <is>
+          <t>How do we feel? I can’t make up my mind if these are cute, or kinda icky 😅😬</t>
+        </is>
+      </c>
+      <c r="C1251" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zbjyzyht4lde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1252">
+      <c r="A1252" t="inlineStr">
+        <is>
+          <t>1i3i8dc</t>
+        </is>
+      </c>
+      <c r="B1252" t="inlineStr">
+        <is>
+          <t xml:space="preserve">i love this design </t>
+        </is>
+      </c>
+      <c r="C1252" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i3i8dc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1253">
+      <c r="A1253" t="inlineStr">
+        <is>
+          <t>1i3bpfn</t>
+        </is>
+      </c>
+      <c r="B1253" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I decided to try something new. Worth it? </t>
+        </is>
+      </c>
+      <c r="C1253" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/bkdy9hewiide1.jpeg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Get daily reddit data: Sun Jan 19 08:09:07 UTC 2025
</commit_message>
<xml_diff>
--- a/data/collected_data/2025_01_19.xlsx
+++ b/data/collected_data/2025_01_19.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1253"/>
+  <dimension ref="A1:C1440"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -21736,6 +21736,3185 @@
         </is>
       </c>
     </row>
+    <row r="1254">
+      <c r="A1254" t="inlineStr">
+        <is>
+          <t>1i4shq1</t>
+        </is>
+      </c>
+      <c r="B1254" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Press on nails feedback </t>
+        </is>
+      </c>
+      <c r="C1254" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4shq1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1255">
+      <c r="A1255" t="inlineStr">
+        <is>
+          <t>1i4sadz</t>
+        </is>
+      </c>
+      <c r="B1255" t="inlineStr">
+        <is>
+          <t>2024 was a year of great sets.</t>
+        </is>
+      </c>
+      <c r="C1255" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q0lasxtp9wde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1256">
+      <c r="A1256" t="inlineStr">
+        <is>
+          <t>1i4s6ij</t>
+        </is>
+      </c>
+      <c r="B1256" t="inlineStr">
+        <is>
+          <t>Can I mix matte and glossy gel for a satin effect?</t>
+        </is>
+      </c>
+      <c r="C1256" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i4s6ij/can_i_mix_matte_and_glossy_gel_for_a_satin_effect/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1257">
+      <c r="A1257" t="inlineStr">
+        <is>
+          <t>1i4s09j</t>
+        </is>
+      </c>
+      <c r="B1257" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New set </t>
+        </is>
+      </c>
+      <c r="C1257" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4s09j</t>
+        </is>
+      </c>
+    </row>
+    <row r="1258">
+      <c r="A1258" t="inlineStr">
+        <is>
+          <t>1i4roh7</t>
+        </is>
+      </c>
+      <c r="B1258" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Base coat for gel nails? </t>
+        </is>
+      </c>
+      <c r="C1258" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i4roh7/base_coat_for_gel_nails/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1259">
+      <c r="A1259" t="inlineStr">
+        <is>
+          <t>1i4rmcy</t>
+        </is>
+      </c>
+      <c r="B1259" t="inlineStr">
+        <is>
+          <t>4/52 wks of Nails</t>
+        </is>
+      </c>
+      <c r="C1259" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gm61wwu62wde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1260">
+      <c r="A1260" t="inlineStr">
+        <is>
+          <t>1i4rk8m</t>
+        </is>
+      </c>
+      <c r="B1260" t="inlineStr">
+        <is>
+          <t xml:space="preserve">magnetic polish is magical </t>
+        </is>
+      </c>
+      <c r="C1260" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4rk8m</t>
+        </is>
+      </c>
+    </row>
+    <row r="1261">
+      <c r="A1261" t="inlineStr">
+        <is>
+          <t>1i4rg7h</t>
+        </is>
+      </c>
+      <c r="B1261" t="inlineStr">
+        <is>
+          <t>Is it normal for my thumb nail bed to look like this?</t>
+        </is>
+      </c>
+      <c r="C1261" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jp93frsa0wde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1262">
+      <c r="A1262" t="inlineStr">
+        <is>
+          <t>1i4qydf</t>
+        </is>
+      </c>
+      <c r="B1262" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Zoya customer service </t>
+        </is>
+      </c>
+      <c r="C1262" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/3k3m28x3vvde1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1263">
+      <c r="A1263" t="inlineStr">
+        <is>
+          <t>1i4r3f7</t>
+        </is>
+      </c>
+      <c r="B1263" t="inlineStr">
+        <is>
+          <t>Lots of cute nails I’ve been doing lately</t>
+        </is>
+      </c>
+      <c r="C1263" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4r3f7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1264">
+      <c r="A1264" t="inlineStr">
+        <is>
+          <t>1i4qlym</t>
+        </is>
+      </c>
+      <c r="B1264" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Day 20 of these press ons </t>
+        </is>
+      </c>
+      <c r="C1264" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4qlym</t>
+        </is>
+      </c>
+    </row>
+    <row r="1265">
+      <c r="A1265" t="inlineStr">
+        <is>
+          <t>1i4pmzd</t>
+        </is>
+      </c>
+      <c r="B1265" t="inlineStr">
+        <is>
+          <t>Pre-Valentine's Day</t>
+        </is>
+      </c>
+      <c r="C1265" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/sy4paucvivde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1266">
+      <c r="A1266" t="inlineStr">
+        <is>
+          <t>1i4owaa</t>
+        </is>
+      </c>
+      <c r="B1266" t="inlineStr">
+        <is>
+          <t>Decided to go funky..</t>
+        </is>
+      </c>
+      <c r="C1266" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/72yk6rq1cvde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1267">
+      <c r="A1267" t="inlineStr">
+        <is>
+          <t>1i4p74n</t>
+        </is>
+      </c>
+      <c r="B1267" t="inlineStr">
+        <is>
+          <t>Coquette nails!  💞</t>
+        </is>
+      </c>
+      <c r="C1267" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rnwka1l2fvde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1268">
+      <c r="A1268" t="inlineStr">
+        <is>
+          <t>1i4oy9f</t>
+        </is>
+      </c>
+      <c r="B1268" t="inlineStr">
+        <is>
+          <t>HOW are yall doing chrome?!!</t>
+        </is>
+      </c>
+      <c r="C1268" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4oy9f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1269">
+      <c r="A1269" t="inlineStr">
+        <is>
+          <t>1i4oxgi</t>
+        </is>
+      </c>
+      <c r="B1269" t="inlineStr">
+        <is>
+          <t>First time working with builder gel 💕</t>
+        </is>
+      </c>
+      <c r="C1269" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aastuf7ecvde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1270">
+      <c r="A1270" t="inlineStr">
+        <is>
+          <t>1i4omr7</t>
+        </is>
+      </c>
+      <c r="B1270" t="inlineStr">
+        <is>
+          <t>Winter Cateyes</t>
+        </is>
+      </c>
+      <c r="C1270" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4omr7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1271">
+      <c r="A1271" t="inlineStr">
+        <is>
+          <t>1i4ofhq</t>
+        </is>
+      </c>
+      <c r="B1271" t="inlineStr">
+        <is>
+          <t>Nightmare before Christmas themed !! By Ruby at @ confession booth in Manchester England 🖤</t>
+        </is>
+      </c>
+      <c r="C1271" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4ofhq</t>
+        </is>
+      </c>
+    </row>
+    <row r="1272">
+      <c r="A1272" t="inlineStr">
+        <is>
+          <t>1i4ofgn</t>
+        </is>
+      </c>
+      <c r="B1272" t="inlineStr">
+        <is>
+          <t>Valentines nails</t>
+        </is>
+      </c>
+      <c r="C1272" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4ofgn</t>
+        </is>
+      </c>
+    </row>
+    <row r="1273">
+      <c r="A1273" t="inlineStr">
+        <is>
+          <t>1i4od5b</t>
+        </is>
+      </c>
+      <c r="B1273" t="inlineStr">
+        <is>
+          <t>valentines day</t>
+        </is>
+      </c>
+      <c r="C1273" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4od5b</t>
+        </is>
+      </c>
+    </row>
+    <row r="1274">
+      <c r="A1274" t="inlineStr">
+        <is>
+          <t>1i4o42n</t>
+        </is>
+      </c>
+      <c r="B1274" t="inlineStr">
+        <is>
+          <t>HotPink Holographic 🙌🏻</t>
+        </is>
+      </c>
+      <c r="C1274" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/t2zihote4vde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1275">
+      <c r="A1275" t="inlineStr">
+        <is>
+          <t>1i4o3k5</t>
+        </is>
+      </c>
+      <c r="B1275" t="inlineStr">
+        <is>
+          <t xml:space="preserve">thougths? </t>
+        </is>
+      </c>
+      <c r="C1275" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/k55gz5294vde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1276">
+      <c r="A1276" t="inlineStr">
+        <is>
+          <t>1i4muoc</t>
+        </is>
+      </c>
+      <c r="B1276" t="inlineStr">
+        <is>
+          <t>what nail/hand shape do i have based on this chart? (creator of chart on insta @misssunshine_nails)</t>
+        </is>
+      </c>
+      <c r="C1276" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4muoc</t>
+        </is>
+      </c>
+    </row>
+    <row r="1277">
+      <c r="A1277" t="inlineStr">
+        <is>
+          <t>1i4ns24</t>
+        </is>
+      </c>
+      <c r="B1277" t="inlineStr">
+        <is>
+          <t>Valentine’s Day nails! ❤️🎀</t>
+        </is>
+      </c>
+      <c r="C1277" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4ns24</t>
+        </is>
+      </c>
+    </row>
+    <row r="1278">
+      <c r="A1278" t="inlineStr">
+        <is>
+          <t>1i4ngd8</t>
+        </is>
+      </c>
+      <c r="B1278" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Did such snake by hand, what do you think? 🐍 </t>
+        </is>
+      </c>
+      <c r="C1278" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/dvnh8m55yude1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1279">
+      <c r="A1279" t="inlineStr">
+        <is>
+          <t>1i4n5qh</t>
+        </is>
+      </c>
+      <c r="B1279" t="inlineStr">
+        <is>
+          <t>I need help asap</t>
+        </is>
+      </c>
+      <c r="C1279" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4n5qh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1280">
+      <c r="A1280" t="inlineStr">
+        <is>
+          <t>1i4n51b</t>
+        </is>
+      </c>
+      <c r="B1280" t="inlineStr">
+        <is>
+          <t>Changing Nail Tech at Same Salon</t>
+        </is>
+      </c>
+      <c r="C1280" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i4n51b/changing_nail_tech_at_same_salon/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1281">
+      <c r="A1281" t="inlineStr">
+        <is>
+          <t>1i4mpkz</t>
+        </is>
+      </c>
+      <c r="B1281" t="inlineStr">
+        <is>
+          <t>Guess the theme</t>
+        </is>
+      </c>
+      <c r="C1281" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4mpkz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1282">
+      <c r="A1282" t="inlineStr">
+        <is>
+          <t>1i4mhag</t>
+        </is>
+      </c>
+      <c r="B1282" t="inlineStr">
+        <is>
+          <t>First attempt at an at-home gel mani</t>
+        </is>
+      </c>
+      <c r="C1282" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zi98hwu4pude1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1283">
+      <c r="A1283" t="inlineStr">
+        <is>
+          <t>1i4mevn</t>
+        </is>
+      </c>
+      <c r="B1283" t="inlineStr">
+        <is>
+          <t>New Nails. Somewhat Subtle Valentines edition</t>
+        </is>
+      </c>
+      <c r="C1283" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/6rn8vvqioude1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1284">
+      <c r="A1284" t="inlineStr">
+        <is>
+          <t>1i4lnog</t>
+        </is>
+      </c>
+      <c r="B1284" t="inlineStr">
+        <is>
+          <t>Opinion Wanted</t>
+        </is>
+      </c>
+      <c r="C1284" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4lnog</t>
+        </is>
+      </c>
+    </row>
+    <row r="1285">
+      <c r="A1285" t="inlineStr">
+        <is>
+          <t>1i4m6n8</t>
+        </is>
+      </c>
+      <c r="B1285" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Advice for thin nails with short nail beds </t>
+        </is>
+      </c>
+      <c r="C1285" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i4m6n8/advice_for_thin_nails_with_short_nail_beds/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1286">
+      <c r="A1286" t="inlineStr">
+        <is>
+          <t>1i4m65s</t>
+        </is>
+      </c>
+      <c r="B1286" t="inlineStr">
+        <is>
+          <t>I loved this result! I consider it to be a delicate and at the same time elegant option. And you? What do you think?</t>
+        </is>
+      </c>
+      <c r="C1286" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/lxwgb5vdmude1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1287">
+      <c r="A1287" t="inlineStr">
+        <is>
+          <t>1i4lz02</t>
+        </is>
+      </c>
+      <c r="B1287" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tried chrome for the first time and I’m obsessed </t>
+        </is>
+      </c>
+      <c r="C1287" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/gexk102mkude1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1288">
+      <c r="A1288" t="inlineStr">
+        <is>
+          <t>1i4lqcz</t>
+        </is>
+      </c>
+      <c r="B1288" t="inlineStr">
+        <is>
+          <t>Lunar New Year Nails</t>
+        </is>
+      </c>
+      <c r="C1288" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ielxm9gfiude1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1289">
+      <c r="A1289" t="inlineStr">
+        <is>
+          <t>1i4llva</t>
+        </is>
+      </c>
+      <c r="B1289" t="inlineStr">
+        <is>
+          <t>A manicure so good, it speaks French💋</t>
+        </is>
+      </c>
+      <c r="C1289" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2y71gqjchude1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1290">
+      <c r="A1290" t="inlineStr">
+        <is>
+          <t>1i4ldrm</t>
+        </is>
+      </c>
+      <c r="B1290" t="inlineStr">
+        <is>
+          <t>By FAR my favorite mani!!</t>
+        </is>
+      </c>
+      <c r="C1290" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/h29hs3jbfude1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1291">
+      <c r="A1291" t="inlineStr">
+        <is>
+          <t>1i4lc98</t>
+        </is>
+      </c>
+      <c r="B1291" t="inlineStr">
+        <is>
+          <t>New nails what do yall think (added better pics since someone said they couldn’t see them clearly)</t>
+        </is>
+      </c>
+      <c r="C1291" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4lc98</t>
+        </is>
+      </c>
+    </row>
+    <row r="1292">
+      <c r="A1292" t="inlineStr">
+        <is>
+          <t>1i4l0f4</t>
+        </is>
+      </c>
+      <c r="B1292" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Purple French tip with chrome 💜 </t>
+        </is>
+      </c>
+      <c r="C1292" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4l0f4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1293">
+      <c r="A1293" t="inlineStr">
+        <is>
+          <t>1i4kx09</t>
+        </is>
+      </c>
+      <c r="B1293" t="inlineStr">
+        <is>
+          <t>Pink always make me feel like I’m that girl 🥰🩷</t>
+        </is>
+      </c>
+      <c r="C1293" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4kx09</t>
+        </is>
+      </c>
+    </row>
+    <row r="1294">
+      <c r="A1294" t="inlineStr">
+        <is>
+          <t>1i4kepr</t>
+        </is>
+      </c>
+      <c r="B1294" t="inlineStr">
+        <is>
+          <t>New nails what yall think?</t>
+        </is>
+      </c>
+      <c r="C1294" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4kepr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1295">
+      <c r="A1295" t="inlineStr">
+        <is>
+          <t>1i4kbie</t>
+        </is>
+      </c>
+      <c r="B1295" t="inlineStr">
+        <is>
+          <t>first time trying nail stickers ✨️</t>
+        </is>
+      </c>
+      <c r="C1295" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qez5rta06ude1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1296">
+      <c r="A1296" t="inlineStr">
+        <is>
+          <t>1i4jvcb</t>
+        </is>
+      </c>
+      <c r="B1296" t="inlineStr">
+        <is>
+          <t>Set No.2 for January🙂‍↔️</t>
+        </is>
+      </c>
+      <c r="C1296" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4jvcb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1297">
+      <c r="A1297" t="inlineStr">
+        <is>
+          <t>1i4jumi</t>
+        </is>
+      </c>
+      <c r="B1297" t="inlineStr">
+        <is>
+          <t>Which nail polish color suits my hand?</t>
+        </is>
+      </c>
+      <c r="C1297" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4jumi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1298">
+      <c r="A1298" t="inlineStr">
+        <is>
+          <t>1i4jgc0</t>
+        </is>
+      </c>
+      <c r="B1298" t="inlineStr">
+        <is>
+          <t>are these worth $140?</t>
+        </is>
+      </c>
+      <c r="C1298" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4jgc0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1299">
+      <c r="A1299" t="inlineStr">
+        <is>
+          <t>1i4jeum</t>
+        </is>
+      </c>
+      <c r="B1299" t="inlineStr">
+        <is>
+          <t>Belle 📚🌹✨</t>
+        </is>
+      </c>
+      <c r="C1299" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/1udu8o17ytde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1300">
+      <c r="A1300" t="inlineStr">
+        <is>
+          <t>1i4j8ft</t>
+        </is>
+      </c>
+      <c r="B1300" t="inlineStr">
+        <is>
+          <t>i’m obsessed</t>
+        </is>
+      </c>
+      <c r="C1300" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4j8ft</t>
+        </is>
+      </c>
+    </row>
+    <row r="1301">
+      <c r="A1301" t="inlineStr">
+        <is>
+          <t>1i4gqgf</t>
+        </is>
+      </c>
+      <c r="B1301" t="inlineStr">
+        <is>
+          <t>how do I take care of them?</t>
+        </is>
+      </c>
+      <c r="C1301" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i4gqgf/how_do_i_take_care_of_them/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1302">
+      <c r="A1302" t="inlineStr">
+        <is>
+          <t>1i4hay9</t>
+        </is>
+      </c>
+      <c r="B1302" t="inlineStr">
+        <is>
+          <t>How do i use nailtiques formula 2 with gel nail polish?</t>
+        </is>
+      </c>
+      <c r="C1302" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i4hay9/how_do_i_use_nailtiques_formula_2_with_gel_nail/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1303">
+      <c r="A1303" t="inlineStr">
+        <is>
+          <t>1i4gyaw</t>
+        </is>
+      </c>
+      <c r="B1303" t="inlineStr">
+        <is>
+          <t>SNS equivalent in OPI or Essie</t>
+        </is>
+      </c>
+      <c r="C1303" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fxdn4302etde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1304">
+      <c r="A1304" t="inlineStr">
+        <is>
+          <t>1i4j43j</t>
+        </is>
+      </c>
+      <c r="B1304" t="inlineStr">
+        <is>
+          <t>My new nails 🤍</t>
+        </is>
+      </c>
+      <c r="C1304" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/2idwvo6ovtde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1305">
+      <c r="A1305" t="inlineStr">
+        <is>
+          <t>1i4imka</t>
+        </is>
+      </c>
+      <c r="B1305" t="inlineStr">
+        <is>
+          <t>new set🌹</t>
+        </is>
+      </c>
+      <c r="C1305" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4imka</t>
+        </is>
+      </c>
+    </row>
+    <row r="1306">
+      <c r="A1306" t="inlineStr">
+        <is>
+          <t>1i4iina</t>
+        </is>
+      </c>
+      <c r="B1306" t="inlineStr">
+        <is>
+          <t>First time using gel x</t>
+        </is>
+      </c>
+      <c r="C1306" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4iina</t>
+        </is>
+      </c>
+    </row>
+    <row r="1307">
+      <c r="A1307" t="inlineStr">
+        <is>
+          <t>1i4igb7</t>
+        </is>
+      </c>
+      <c r="B1307" t="inlineStr">
+        <is>
+          <t>LNY nails 🐍🧧</t>
+        </is>
+      </c>
+      <c r="C1307" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4igb7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1308">
+      <c r="A1308" t="inlineStr">
+        <is>
+          <t>1i4ifat</t>
+        </is>
+      </c>
+      <c r="B1308" t="inlineStr">
+        <is>
+          <t>Just got a new full</t>
+        </is>
+      </c>
+      <c r="C1308" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4ifat</t>
+        </is>
+      </c>
+    </row>
+    <row r="1309">
+      <c r="A1309" t="inlineStr">
+        <is>
+          <t>1i4i453</t>
+        </is>
+      </c>
+      <c r="B1309" t="inlineStr">
+        <is>
+          <t>Suddenly lost my corn snake so I made this set to honor him. I love you Charlie ❤️</t>
+        </is>
+      </c>
+      <c r="C1309" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4i453</t>
+        </is>
+      </c>
+    </row>
+    <row r="1310">
+      <c r="A1310" t="inlineStr">
+        <is>
+          <t>1i4hx0i</t>
+        </is>
+      </c>
+      <c r="B1310" t="inlineStr">
+        <is>
+          <t xml:space="preserve">2009 Zoya - Kalmia </t>
+        </is>
+      </c>
+      <c r="C1310" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4hx0i</t>
+        </is>
+      </c>
+    </row>
+    <row r="1311">
+      <c r="A1311" t="inlineStr">
+        <is>
+          <t>1i4hrr8</t>
+        </is>
+      </c>
+      <c r="B1311" t="inlineStr">
+        <is>
+          <t>Do these look thick for my short nails? Builder gel with gel polish</t>
+        </is>
+      </c>
+      <c r="C1311" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jdkyq70oktde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1312">
+      <c r="A1312" t="inlineStr">
+        <is>
+          <t>1i4hp0w</t>
+        </is>
+      </c>
+      <c r="B1312" t="inlineStr">
+        <is>
+          <t>thermal nails except it's chilly out lol</t>
+        </is>
+      </c>
+      <c r="C1312" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4hp0w</t>
+        </is>
+      </c>
+    </row>
+    <row r="1313">
+      <c r="A1313" t="inlineStr">
+        <is>
+          <t>1i4hdfl</t>
+        </is>
+      </c>
+      <c r="B1313" t="inlineStr">
+        <is>
+          <t>Third attempt with hard gel</t>
+        </is>
+      </c>
+      <c r="C1313" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4hdfl</t>
+        </is>
+      </c>
+    </row>
+    <row r="1314">
+      <c r="A1314" t="inlineStr">
+        <is>
+          <t>1i4h9l9</t>
+        </is>
+      </c>
+      <c r="B1314" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Birthday nails </t>
+        </is>
+      </c>
+      <c r="C1314" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4h9l9</t>
+        </is>
+      </c>
+    </row>
+    <row r="1315">
+      <c r="A1315" t="inlineStr">
+        <is>
+          <t>1i4gzag</t>
+        </is>
+      </c>
+      <c r="B1315" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Asked my sister to take pictures of my nails </t>
+        </is>
+      </c>
+      <c r="C1315" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4gzag</t>
+        </is>
+      </c>
+    </row>
+    <row r="1316">
+      <c r="A1316" t="inlineStr">
+        <is>
+          <t>1i4ge45</t>
+        </is>
+      </c>
+      <c r="B1316" t="inlineStr">
+        <is>
+          <t>Clean girl glam</t>
+        </is>
+      </c>
+      <c r="C1316" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4ge45</t>
+        </is>
+      </c>
+    </row>
+    <row r="1317">
+      <c r="A1317" t="inlineStr">
+        <is>
+          <t>1i4ejh6</t>
+        </is>
+      </c>
+      <c r="B1317" t="inlineStr">
+        <is>
+          <t>i found bruise-like spots on 3 of my nails after scraping off my nail polish in the shower.</t>
+        </is>
+      </c>
+      <c r="C1317" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/9vwiangmusde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1318">
+      <c r="A1318" t="inlineStr">
+        <is>
+          <t>1i4e1uj</t>
+        </is>
+      </c>
+      <c r="B1318" t="inlineStr">
+        <is>
+          <t>Are my nails too long?</t>
+        </is>
+      </c>
+      <c r="C1318" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/49gb72qnqsde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1319">
+      <c r="A1319" t="inlineStr">
+        <is>
+          <t>1i4chi3</t>
+        </is>
+      </c>
+      <c r="B1319" t="inlineStr">
+        <is>
+          <t>Are these nails good or no?</t>
+        </is>
+      </c>
+      <c r="C1319" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4chi3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1320">
+      <c r="A1320" t="inlineStr">
+        <is>
+          <t>1i4azwt</t>
+        </is>
+      </c>
+      <c r="B1320" t="inlineStr">
+        <is>
+          <t>Was I overreacting?</t>
+        </is>
+      </c>
+      <c r="C1320" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4azwt</t>
+        </is>
+      </c>
+    </row>
+    <row r="1321">
+      <c r="A1321" t="inlineStr">
+        <is>
+          <t>1i4elvg</t>
+        </is>
+      </c>
+      <c r="B1321" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Breaking the habit of neutral colors </t>
+        </is>
+      </c>
+      <c r="C1321" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i4elvg/breaking_the_habit_of_neutral_colors/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1322">
+      <c r="A1322" t="inlineStr">
+        <is>
+          <t>1i4fxpc</t>
+        </is>
+      </c>
+      <c r="B1322" t="inlineStr">
+        <is>
+          <t>New shape for me</t>
+        </is>
+      </c>
+      <c r="C1322" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rsv82zer5tde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1323">
+      <c r="A1323" t="inlineStr">
+        <is>
+          <t>1i4frrm</t>
+        </is>
+      </c>
+      <c r="B1323" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cat eye for my manicure to me. </t>
+        </is>
+      </c>
+      <c r="C1323" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xdvco5ie4tde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1324">
+      <c r="A1324" t="inlineStr">
+        <is>
+          <t>1i4fqd2</t>
+        </is>
+      </c>
+      <c r="B1324" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time trying to separate polishes! </t>
+        </is>
+      </c>
+      <c r="C1324" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/652hiee34tde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1325">
+      <c r="A1325" t="inlineStr">
+        <is>
+          <t>1i4f0to</t>
+        </is>
+      </c>
+      <c r="B1325" t="inlineStr">
+        <is>
+          <t>Vday nails 🥰</t>
+        </is>
+      </c>
+      <c r="C1325" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4f0to</t>
+        </is>
+      </c>
+    </row>
+    <row r="1326">
+      <c r="A1326" t="inlineStr">
+        <is>
+          <t>1i4ec9y</t>
+        </is>
+      </c>
+      <c r="B1326" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Obsessed </t>
+        </is>
+      </c>
+      <c r="C1326" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/rcypqmyyssde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1327">
+      <c r="A1327" t="inlineStr">
+        <is>
+          <t>1i4e8nk</t>
+        </is>
+      </c>
+      <c r="B1327" t="inlineStr">
+        <is>
+          <t>gel french tips over my natural nails 🤍</t>
+        </is>
+      </c>
+      <c r="C1327" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4e8nk</t>
+        </is>
+      </c>
+    </row>
+    <row r="1328">
+      <c r="A1328" t="inlineStr">
+        <is>
+          <t>1i4e7hg</t>
+        </is>
+      </c>
+      <c r="B1328" t="inlineStr">
+        <is>
+          <t>does this shape suit me?</t>
+        </is>
+      </c>
+      <c r="C1328" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4e7hg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1329">
+      <c r="A1329" t="inlineStr">
+        <is>
+          <t>1i4e33l</t>
+        </is>
+      </c>
+      <c r="B1329" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Love my cute nails! </t>
+        </is>
+      </c>
+      <c r="C1329" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/na2yek2yqsde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1330">
+      <c r="A1330" t="inlineStr">
+        <is>
+          <t>1i4e061</t>
+        </is>
+      </c>
+      <c r="B1330" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Painted my nails rose gold and opal to match my engagement ring. Obsessed is an understatement. </t>
+        </is>
+      </c>
+      <c r="C1330" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/22yw1gjaqsde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1331">
+      <c r="A1331" t="inlineStr">
+        <is>
+          <t>1i4e048</t>
+        </is>
+      </c>
+      <c r="B1331" t="inlineStr">
+        <is>
+          <t>Did my own birthday nails today✨☘️</t>
+        </is>
+      </c>
+      <c r="C1331" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4e048</t>
+        </is>
+      </c>
+    </row>
+    <row r="1332">
+      <c r="A1332" t="inlineStr">
+        <is>
+          <t>1i4dxvr</t>
+        </is>
+      </c>
+      <c r="B1332" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Square or Almond? </t>
+        </is>
+      </c>
+      <c r="C1332" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4dxvr</t>
+        </is>
+      </c>
+    </row>
+    <row r="1333">
+      <c r="A1333" t="inlineStr">
+        <is>
+          <t>1i4ds2o</t>
+        </is>
+      </c>
+      <c r="B1333" t="inlineStr">
+        <is>
+          <t>First Valentines Day set💕</t>
+        </is>
+      </c>
+      <c r="C1333" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/o2kml3uiosde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1334">
+      <c r="A1334" t="inlineStr">
+        <is>
+          <t>1i4drl3</t>
+        </is>
+      </c>
+      <c r="B1334" t="inlineStr">
+        <is>
+          <t>Oh it’s shiftyyyyyyyyy</t>
+        </is>
+      </c>
+      <c r="C1334" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/7h1d15afosde1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1335">
+      <c r="A1335" t="inlineStr">
+        <is>
+          <t>1i4dox4</t>
+        </is>
+      </c>
+      <c r="B1335" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Really loving the Gold look </t>
+        </is>
+      </c>
+      <c r="C1335" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/s84fnt1unsde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1336">
+      <c r="A1336" t="inlineStr">
+        <is>
+          <t>1i4dcfa</t>
+        </is>
+      </c>
+      <c r="B1336" t="inlineStr">
+        <is>
+          <t>I loved the tone, it looks very pretty</t>
+        </is>
+      </c>
+      <c r="C1336" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/q6z8cv93lsde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1337">
+      <c r="A1337" t="inlineStr">
+        <is>
+          <t>1i4ct8l</t>
+        </is>
+      </c>
+      <c r="B1337" t="inlineStr">
+        <is>
+          <t>Not sure how I feel about purple</t>
+        </is>
+      </c>
+      <c r="C1337" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0eeycncxgsde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1338">
+      <c r="A1338" t="inlineStr">
+        <is>
+          <t>1i4cmj3</t>
+        </is>
+      </c>
+      <c r="B1338" t="inlineStr">
+        <is>
+          <t>Fine china nails!!</t>
+        </is>
+      </c>
+      <c r="C1338" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4cmj3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1339">
+      <c r="A1339" t="inlineStr">
+        <is>
+          <t>1i4cm37</t>
+        </is>
+      </c>
+      <c r="B1339" t="inlineStr">
+        <is>
+          <t>When you find an artist that brings your vision to life. Year of the snake 🐍</t>
+        </is>
+      </c>
+      <c r="C1339" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ucyl3jhdfsde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1340">
+      <c r="A1340" t="inlineStr">
+        <is>
+          <t>1i4btoc</t>
+        </is>
+      </c>
+      <c r="B1340" t="inlineStr">
+        <is>
+          <t xml:space="preserve">$10 cvs press ons </t>
+        </is>
+      </c>
+      <c r="C1340" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ikq3lh779sde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1341">
+      <c r="A1341" t="inlineStr">
+        <is>
+          <t>1i4aycx</t>
+        </is>
+      </c>
+      <c r="B1341" t="inlineStr">
+        <is>
+          <t>Beetles Gel Polish Suggestions</t>
+        </is>
+      </c>
+      <c r="C1341" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i4aycx/beetles_gel_polish_suggestions/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1342">
+      <c r="A1342" t="inlineStr">
+        <is>
+          <t>1i4awao</t>
+        </is>
+      </c>
+      <c r="B1342" t="inlineStr">
+        <is>
+          <t>Having trouble getting my nails to fully dry. What am I doing wrong?</t>
+        </is>
+      </c>
+      <c r="C1342" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i4awao/having_trouble_getting_my_nails_to_fully_dry_what/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1343">
+      <c r="A1343" t="inlineStr">
+        <is>
+          <t>1i4atco</t>
+        </is>
+      </c>
+      <c r="B1343" t="inlineStr">
+        <is>
+          <t>New set</t>
+        </is>
+      </c>
+      <c r="C1343" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y84vx4x11sde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1344">
+      <c r="A1344" t="inlineStr">
+        <is>
+          <t>1i4at4d</t>
+        </is>
+      </c>
+      <c r="B1344" t="inlineStr">
+        <is>
+          <t xml:space="preserve">New claws who dis </t>
+        </is>
+      </c>
+      <c r="C1344" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/y64pxcyy0sde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1345">
+      <c r="A1345" t="inlineStr">
+        <is>
+          <t>1i4ahcy</t>
+        </is>
+      </c>
+      <c r="B1345" t="inlineStr">
+        <is>
+          <t>How bad is this? This is when my local shop removed gelx.</t>
+        </is>
+      </c>
+      <c r="C1345" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4ahcy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1346">
+      <c r="A1346" t="inlineStr">
+        <is>
+          <t>1i4agul</t>
+        </is>
+      </c>
+      <c r="B1346" t="inlineStr">
+        <is>
+          <t>Tiny hands</t>
+        </is>
+      </c>
+      <c r="C1346" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i4agul/tiny_hands/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1347">
+      <c r="A1347" t="inlineStr">
+        <is>
+          <t>1i45l03</t>
+        </is>
+      </c>
+      <c r="B1347" t="inlineStr">
+        <is>
+          <t>Nail separated from nail bed</t>
+        </is>
+      </c>
+      <c r="C1347" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/db2wxs0xlqde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1348">
+      <c r="A1348" t="inlineStr">
+        <is>
+          <t>1i4a0r7</t>
+        </is>
+      </c>
+      <c r="B1348" t="inlineStr">
+        <is>
+          <t>Paw nails</t>
+        </is>
+      </c>
+      <c r="C1348" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/fxnphdbkurde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1349">
+      <c r="A1349" t="inlineStr">
+        <is>
+          <t>1i49ses</t>
+        </is>
+      </c>
+      <c r="B1349" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Just love my nails </t>
+        </is>
+      </c>
+      <c r="C1349" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x72rh1olsrde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1350">
+      <c r="A1350" t="inlineStr">
+        <is>
+          <t>1i49nul</t>
+        </is>
+      </c>
+      <c r="B1350" t="inlineStr">
+        <is>
+          <t>Holding on to frosty season</t>
+        </is>
+      </c>
+      <c r="C1350" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i49nul</t>
+        </is>
+      </c>
+    </row>
+    <row r="1351">
+      <c r="A1351" t="inlineStr">
+        <is>
+          <t>1i49epk</t>
+        </is>
+      </c>
+      <c r="B1351" t="inlineStr">
+        <is>
+          <t xml:space="preserve">prepping hard gel to not lift </t>
+        </is>
+      </c>
+      <c r="C1351" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/aapio1caprde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1352">
+      <c r="A1352" t="inlineStr">
+        <is>
+          <t>1i49701</t>
+        </is>
+      </c>
+      <c r="B1352" t="inlineStr">
+        <is>
+          <t>New nail tech</t>
+        </is>
+      </c>
+      <c r="C1352" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i49701</t>
+        </is>
+      </c>
+    </row>
+    <row r="1353">
+      <c r="A1353" t="inlineStr">
+        <is>
+          <t>1i494cn</t>
+        </is>
+      </c>
+      <c r="B1353" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I Adore This Color </t>
+        </is>
+      </c>
+      <c r="C1353" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/Nails/comments/1i494cn/i_adore_this_color/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1354">
+      <c r="A1354" t="inlineStr">
+        <is>
+          <t>1i4tjsi</t>
+        </is>
+      </c>
+      <c r="B1354" t="inlineStr">
+        <is>
+          <t xml:space="preserve">cirque haul (purchased prior to learning about many peoples gripes with them) </t>
+        </is>
+      </c>
+      <c r="C1354" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4tjsi</t>
+        </is>
+      </c>
+    </row>
+    <row r="1355">
+      <c r="A1355" t="inlineStr">
+        <is>
+          <t>1i4th7a</t>
+        </is>
+      </c>
+      <c r="B1355" t="inlineStr">
+        <is>
+          <t>Deep purple (rain)</t>
+        </is>
+      </c>
+      <c r="C1355" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4th7a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1356">
+      <c r="A1356" t="inlineStr">
+        <is>
+          <t>1i4tg9a</t>
+        </is>
+      </c>
+      <c r="B1356" t="inlineStr">
+        <is>
+          <t>Best protective base coat for someone who picks at her mani?</t>
+        </is>
+      </c>
+      <c r="C1356" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/0dpesdnznwde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1357">
+      <c r="A1357" t="inlineStr">
+        <is>
+          <t>1i4rjh8</t>
+        </is>
+      </c>
+      <c r="B1357" t="inlineStr">
+        <is>
+          <t>Cirque Rosewater Jelly 💖</t>
+        </is>
+      </c>
+      <c r="C1357" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4rjh8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1358">
+      <c r="A1358" t="inlineStr">
+        <is>
+          <t>1i4r9os</t>
+        </is>
+      </c>
+      <c r="B1358" t="inlineStr">
+        <is>
+          <t>Linear Holo + Shifty Shimmer = 🌈🔥</t>
+        </is>
+      </c>
+      <c r="C1358" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/5tb6z5r9yvde1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1359">
+      <c r="A1359" t="inlineStr">
+        <is>
+          <t>1i4r6b0</t>
+        </is>
+      </c>
+      <c r="B1359" t="inlineStr">
+        <is>
+          <t>Most unique ILNP polishes?</t>
+        </is>
+      </c>
+      <c r="C1359" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i4r6b0/most_unique_ilnp_polishes/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1360">
+      <c r="A1360" t="inlineStr">
+        <is>
+          <t>1i4qx7e</t>
+        </is>
+      </c>
+      <c r="B1360" t="inlineStr">
+        <is>
+          <t>Holotaco mani today ❤️</t>
+        </is>
+      </c>
+      <c r="C1360" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4qx7e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1361">
+      <c r="A1361" t="inlineStr">
+        <is>
+          <t>1i4qbzj</t>
+        </is>
+      </c>
+      <c r="B1361" t="inlineStr">
+        <is>
+          <t>Been searching for a Gold/yellow, and or orange shimmer topper</t>
+        </is>
+      </c>
+      <c r="C1361" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i4qbzj/been_searching_for_a_goldyellow_and_or_orange/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1362">
+      <c r="A1362" t="inlineStr">
+        <is>
+          <t>1i4q9i5</t>
+        </is>
+      </c>
+      <c r="B1362" t="inlineStr">
+        <is>
+          <t>Are Cracked and Kathleen brushes the same?</t>
+        </is>
+      </c>
+      <c r="C1362" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i4q9i5/are_cracked_and_kathleen_brushes_the_same/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1363">
+      <c r="A1363" t="inlineStr">
+        <is>
+          <t>1i4q2be</t>
+        </is>
+      </c>
+      <c r="B1363" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Excellent Buy Nothing Score! </t>
+        </is>
+      </c>
+      <c r="C1363" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/py8vghbpmvde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1364">
+      <c r="A1364" t="inlineStr">
+        <is>
+          <t>1i4pw79</t>
+        </is>
+      </c>
+      <c r="B1364" t="inlineStr">
+        <is>
+          <t>Wildflower fairy dust</t>
+        </is>
+      </c>
+      <c r="C1364" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/zkstfml4lvde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1365">
+      <c r="A1365" t="inlineStr">
+        <is>
+          <t>1i4plwz</t>
+        </is>
+      </c>
+      <c r="B1365" t="inlineStr">
+        <is>
+          <t>Shimmery teal!</t>
+        </is>
+      </c>
+      <c r="C1365" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vf08lpglivde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1366">
+      <c r="A1366" t="inlineStr">
+        <is>
+          <t>1i4onc3</t>
+        </is>
+      </c>
+      <c r="B1366" t="inlineStr">
+        <is>
+          <t>Winter Cateyes</t>
+        </is>
+      </c>
+      <c r="C1366" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4onc3</t>
+        </is>
+      </c>
+    </row>
+    <row r="1367">
+      <c r="A1367" t="inlineStr">
+        <is>
+          <t>1i4novd</t>
+        </is>
+      </c>
+      <c r="B1367" t="inlineStr">
+        <is>
+          <t>I was able to grab the ILNP horseshoe magnet for my birthday!</t>
+        </is>
+      </c>
+      <c r="C1367" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wcqwbvob0vde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1368">
+      <c r="A1368" t="inlineStr">
+        <is>
+          <t>1i4n231</t>
+        </is>
+      </c>
+      <c r="B1368" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Kerasal is watery </t>
+        </is>
+      </c>
+      <c r="C1368" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i4n231/kerasal_is_watery/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1369">
+      <c r="A1369" t="inlineStr">
+        <is>
+          <t>1i4mz97</t>
+        </is>
+      </c>
+      <c r="B1369" t="inlineStr">
+        <is>
+          <t xml:space="preserve">The Irish unknown </t>
+        </is>
+      </c>
+      <c r="C1369" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i4mz97/the_irish_unknown/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1370">
+      <c r="A1370" t="inlineStr">
+        <is>
+          <t>1i4mm11</t>
+        </is>
+      </c>
+      <c r="B1370" t="inlineStr">
+        <is>
+          <t>Gel allergy tips?</t>
+        </is>
+      </c>
+      <c r="C1370" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i4mm11/gel_allergy_tips/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1371">
+      <c r="A1371" t="inlineStr">
+        <is>
+          <t>1i4lu6p</t>
+        </is>
+      </c>
+      <c r="B1371" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Lighted magnification glasses have improved my nail game so much. </t>
+        </is>
+      </c>
+      <c r="C1371" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/hzrw3tffjude1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1372">
+      <c r="A1372" t="inlineStr">
+        <is>
+          <t>1i4lr92</t>
+        </is>
+      </c>
+      <c r="B1372" t="inlineStr">
+        <is>
+          <t>Become The Art Yourself</t>
+        </is>
+      </c>
+      <c r="C1372" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4lr92</t>
+        </is>
+      </c>
+    </row>
+    <row r="1373">
+      <c r="A1373" t="inlineStr">
+        <is>
+          <t>1i4lnaz</t>
+        </is>
+      </c>
+      <c r="B1373" t="inlineStr">
+        <is>
+          <t>You all were so right about Sassy Sauce 🤍</t>
+        </is>
+      </c>
+      <c r="C1373" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4lnaz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1374">
+      <c r="A1374" t="inlineStr">
+        <is>
+          <t>1i4lkke</t>
+        </is>
+      </c>
+      <c r="B1374" t="inlineStr">
+        <is>
+          <t>My Zoya sale haul arrived!!</t>
+        </is>
+      </c>
+      <c r="C1374" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/xgu8kfy0hude1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1375">
+      <c r="A1375" t="inlineStr">
+        <is>
+          <t>1i4lh0o</t>
+        </is>
+      </c>
+      <c r="B1375" t="inlineStr">
+        <is>
+          <t>A million years later....</t>
+        </is>
+      </c>
+      <c r="C1375" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4lh0o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1376">
+      <c r="A1376" t="inlineStr">
+        <is>
+          <t>1i4ku9n</t>
+        </is>
+      </c>
+      <c r="B1376" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Feeling very Deep Space </t>
+        </is>
+      </c>
+      <c r="C1376" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4ku9n</t>
+        </is>
+      </c>
+    </row>
+    <row r="1377">
+      <c r="A1377" t="inlineStr">
+        <is>
+          <t>1i4kmw8</t>
+        </is>
+      </c>
+      <c r="B1377" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Essie skittles for holo goodness </t>
+        </is>
+      </c>
+      <c r="C1377" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4kmw8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1378">
+      <c r="A1378" t="inlineStr">
+        <is>
+          <t>1i4km54</t>
+        </is>
+      </c>
+      <c r="B1378" t="inlineStr">
+        <is>
+          <t>Claw display!</t>
+        </is>
+      </c>
+      <c r="C1378" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/h3ifv06m8ude1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1379">
+      <c r="A1379" t="inlineStr">
+        <is>
+          <t>1i4kkfd</t>
+        </is>
+      </c>
+      <c r="B1379" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mooncat Sagebrush  </t>
+        </is>
+      </c>
+      <c r="C1379" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4kkfd</t>
+        </is>
+      </c>
+    </row>
+    <row r="1380">
+      <c r="A1380" t="inlineStr">
+        <is>
+          <t>1i4keuq</t>
+        </is>
+      </c>
+      <c r="B1380" t="inlineStr">
+        <is>
+          <t>Anyone else doing Valentine's Day all month?</t>
+        </is>
+      </c>
+      <c r="C1380" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/vbz9wvsu6ude1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1381">
+      <c r="A1381" t="inlineStr">
+        <is>
+          <t>1i4k9vf</t>
+        </is>
+      </c>
+      <c r="B1381" t="inlineStr">
+        <is>
+          <t xml:space="preserve">My new favorite winter mani </t>
+        </is>
+      </c>
+      <c r="C1381" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4k9vf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1382">
+      <c r="A1382" t="inlineStr">
+        <is>
+          <t>1i4k4yg</t>
+        </is>
+      </c>
+      <c r="B1382" t="inlineStr">
+        <is>
+          <t>Shimmer Skittle</t>
+        </is>
+      </c>
+      <c r="C1382" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4k4yg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1383">
+      <c r="A1383" t="inlineStr">
+        <is>
+          <t>1i4k1b6</t>
+        </is>
+      </c>
+      <c r="B1383" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First fresh set of the new year! Tortoise shell, but a little on the darker side. 🐢 Gel-X. </t>
+        </is>
+      </c>
+      <c r="C1383" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/qevqpu4k3ude1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1384">
+      <c r="A1384" t="inlineStr">
+        <is>
+          <t>1i4k0s3</t>
+        </is>
+      </c>
+      <c r="B1384" t="inlineStr">
+        <is>
+          <t>Me rewatching the sparkles over and over 🤤</t>
+        </is>
+      </c>
+      <c r="C1384" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/265li76e3ude1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1385">
+      <c r="A1385" t="inlineStr">
+        <is>
+          <t>1i4jz4e</t>
+        </is>
+      </c>
+      <c r="B1385" t="inlineStr">
+        <is>
+          <t xml:space="preserve">How can I avoid the top coat rubbing off the color underneath? I let my last coat of color dry for 4 hours before I did the top coat and it still happened. The color was so even before! </t>
+        </is>
+      </c>
+      <c r="C1385" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4jz4e</t>
+        </is>
+      </c>
+    </row>
+    <row r="1386">
+      <c r="A1386" t="inlineStr">
+        <is>
+          <t>1i4jybq</t>
+        </is>
+      </c>
+      <c r="B1386" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Where do you paint your nails? </t>
+        </is>
+      </c>
+      <c r="C1386" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ep26qyms2ude1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1387">
+      <c r="A1387" t="inlineStr">
+        <is>
+          <t>1i4jwud</t>
+        </is>
+      </c>
+      <c r="B1387" t="inlineStr">
+        <is>
+          <t>Hanging Foldable Nail Polish Holder with 54 Mesh Pockets?</t>
+        </is>
+      </c>
+      <c r="C1387" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i4jwud/hanging_foldable_nail_polish_holder_with_54_mesh/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1388">
+      <c r="A1388" t="inlineStr">
+        <is>
+          <t>1i4jt2i</t>
+        </is>
+      </c>
+      <c r="B1388" t="inlineStr">
+        <is>
+          <t>I’m gonna need these in every shade lol</t>
+        </is>
+      </c>
+      <c r="C1388" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/jtwhofqk1ude1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1389">
+      <c r="A1389" t="inlineStr">
+        <is>
+          <t>1i4j6lv</t>
+        </is>
+      </c>
+      <c r="B1389" t="inlineStr">
+        <is>
+          <t>Witches of Oz inspired</t>
+        </is>
+      </c>
+      <c r="C1389" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/m8xx8uoawtde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1390">
+      <c r="A1390" t="inlineStr">
+        <is>
+          <t>1i4ixia</t>
+        </is>
+      </c>
+      <c r="B1390" t="inlineStr">
+        <is>
+          <t xml:space="preserve">more Flowerchild love and a genuine thank you! 💕 </t>
+        </is>
+      </c>
+      <c r="C1390" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/oiawys26utde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1391">
+      <c r="A1391" t="inlineStr">
+        <is>
+          <t>1i4itij</t>
+        </is>
+      </c>
+      <c r="B1391" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tectonic Shift + Bugs! </t>
+        </is>
+      </c>
+      <c r="C1391" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/dunekrx8ttde1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1392">
+      <c r="A1392" t="inlineStr">
+        <is>
+          <t>1i4iol7</t>
+        </is>
+      </c>
+      <c r="B1392" t="inlineStr">
+        <is>
+          <t>Kozmic colors quick setter - what is this?</t>
+        </is>
+      </c>
+      <c r="C1392" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4iol7</t>
+        </is>
+      </c>
+    </row>
+    <row r="1393">
+      <c r="A1393" t="inlineStr">
+        <is>
+          <t>1i4ieav</t>
+        </is>
+      </c>
+      <c r="B1393" t="inlineStr">
+        <is>
+          <t>Similar to Riding Sleeping Bags Down the Stairs but in red / burgundy?</t>
+        </is>
+      </c>
+      <c r="C1393" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/e9bd1y3rptde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1394">
+      <c r="A1394" t="inlineStr">
+        <is>
+          <t>1i4i5ze</t>
+        </is>
+      </c>
+      <c r="B1394" t="inlineStr">
+        <is>
+          <t>Peel Off Base Coat for regular nail polish</t>
+        </is>
+      </c>
+      <c r="C1394" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i4i5ze/peel_off_base_coat_for_regular_nail_polish/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1395">
+      <c r="A1395" t="inlineStr">
+        <is>
+          <t>1i4i12c</t>
+        </is>
+      </c>
+      <c r="B1395" t="inlineStr">
+        <is>
+          <t>Help!</t>
+        </is>
+      </c>
+      <c r="C1395" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4i12c</t>
+        </is>
+      </c>
+    </row>
+    <row r="1396">
+      <c r="A1396" t="inlineStr">
+        <is>
+          <t>1i4hvqe</t>
+        </is>
+      </c>
+      <c r="B1396" t="inlineStr">
+        <is>
+          <t>Actually lokey obsessed with this crappy Amazon polish 💚</t>
+        </is>
+      </c>
+      <c r="C1396" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4hvqe</t>
+        </is>
+      </c>
+    </row>
+    <row r="1397">
+      <c r="A1397" t="inlineStr">
+        <is>
+          <t>1i4hswi</t>
+        </is>
+      </c>
+      <c r="B1397" t="inlineStr">
+        <is>
+          <t>🌌 Galaxy Sparkle 🎆</t>
+        </is>
+      </c>
+      <c r="C1397" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/qkxoorpvktde1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1398">
+      <c r="A1398" t="inlineStr">
+        <is>
+          <t>1i4hmcy</t>
+        </is>
+      </c>
+      <c r="B1398" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Painting my nails to match the incoming snowstorm tomorrow </t>
+        </is>
+      </c>
+      <c r="C1398" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4hmcy</t>
+        </is>
+      </c>
+    </row>
+    <row r="1399">
+      <c r="A1399" t="inlineStr">
+        <is>
+          <t>1i4hcce</t>
+        </is>
+      </c>
+      <c r="B1399" t="inlineStr">
+        <is>
+          <t>Cookie Monster!!</t>
+        </is>
+      </c>
+      <c r="C1399" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4hcce</t>
+        </is>
+      </c>
+    </row>
+    <row r="1400">
+      <c r="A1400" t="inlineStr">
+        <is>
+          <t>1i4h74a</t>
+        </is>
+      </c>
+      <c r="B1400" t="inlineStr">
+        <is>
+          <t>All at the same time - inspired by a mani I saw here</t>
+        </is>
+      </c>
+      <c r="C1400" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4h74a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1401">
+      <c r="A1401" t="inlineStr">
+        <is>
+          <t>1i4gxis</t>
+        </is>
+      </c>
+      <c r="B1401" t="inlineStr">
+        <is>
+          <t>Books &amp; matching manis</t>
+        </is>
+      </c>
+      <c r="C1401" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4gxis</t>
+        </is>
+      </c>
+    </row>
+    <row r="1402">
+      <c r="A1402" t="inlineStr">
+        <is>
+          <t>1i4gle3</t>
+        </is>
+      </c>
+      <c r="B1402" t="inlineStr">
+        <is>
+          <t>Yet another person influenced to buy "Choose Life" by Bee's Knees Lacquer 😅</t>
+        </is>
+      </c>
+      <c r="C1402" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/76kzv690btde1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1403">
+      <c r="A1403" t="inlineStr">
+        <is>
+          <t>1i4glhu</t>
+        </is>
+      </c>
+      <c r="B1403" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What are these little dark spots? </t>
+        </is>
+      </c>
+      <c r="C1403" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4glhu</t>
+        </is>
+      </c>
+    </row>
+    <row r="1404">
+      <c r="A1404" t="inlineStr">
+        <is>
+          <t>1i4g9i8</t>
+        </is>
+      </c>
+      <c r="B1404" t="inlineStr">
+        <is>
+          <t>Mani 3/52: Going Dark 🖤✨</t>
+        </is>
+      </c>
+      <c r="C1404" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4g9i8</t>
+        </is>
+      </c>
+    </row>
+    <row r="1405">
+      <c r="A1405" t="inlineStr">
+        <is>
+          <t>1i4g0s0</t>
+        </is>
+      </c>
+      <c r="B1405" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Mooncat House of Hades w/ Star Destroyer...gorgeous combo! </t>
+        </is>
+      </c>
+      <c r="C1405" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4g0s0</t>
+        </is>
+      </c>
+    </row>
+    <row r="1406">
+      <c r="A1406" t="inlineStr">
+        <is>
+          <t>1i4fdrw</t>
+        </is>
+      </c>
+      <c r="B1406" t="inlineStr">
+        <is>
+          <t>And She was a Ruby</t>
+        </is>
+      </c>
+      <c r="C1406" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/cpuwcslb1tde1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1407">
+      <c r="A1407" t="inlineStr">
+        <is>
+          <t>1i4ew2o</t>
+        </is>
+      </c>
+      <c r="B1407" t="inlineStr">
+        <is>
+          <t>🖤🌈Peekaboo🌈🖤</t>
+        </is>
+      </c>
+      <c r="C1407" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4ew2o</t>
+        </is>
+      </c>
+    </row>
+    <row r="1408">
+      <c r="A1408" t="inlineStr">
+        <is>
+          <t>1i4eg9q</t>
+        </is>
+      </c>
+      <c r="B1408" t="inlineStr">
+        <is>
+          <t>Best way to label swatch sticks?</t>
+        </is>
+      </c>
+      <c r="C1408" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/x78y1ogvtsde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1409">
+      <c r="A1409" t="inlineStr">
+        <is>
+          <t>1i4ecit</t>
+        </is>
+      </c>
+      <c r="B1409" t="inlineStr">
+        <is>
+          <t>Cereal dolphins</t>
+        </is>
+      </c>
+      <c r="C1409" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4ecit</t>
+        </is>
+      </c>
+    </row>
+    <row r="1410">
+      <c r="A1410" t="inlineStr">
+        <is>
+          <t>1i4dz7m</t>
+        </is>
+      </c>
+      <c r="B1410" t="inlineStr">
+        <is>
+          <t>Giving some love to my cremes by stamping</t>
+        </is>
+      </c>
+      <c r="C1410" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/tjpyh8w2qsde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1411">
+      <c r="A1411" t="inlineStr">
+        <is>
+          <t>1i4duyb</t>
+        </is>
+      </c>
+      <c r="B1411" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Tried My Own Art </t>
+        </is>
+      </c>
+      <c r="C1411" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8usnv8b5psde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1412">
+      <c r="A1412" t="inlineStr">
+        <is>
+          <t>1i4dlxa</t>
+        </is>
+      </c>
+      <c r="B1412" t="inlineStr">
+        <is>
+          <t>Dupe help - OPI Kennebunk-port</t>
+        </is>
+      </c>
+      <c r="C1412" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i4dlxa/dupe_help_opi_kennebunkport/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1413">
+      <c r="A1413" t="inlineStr">
+        <is>
+          <t>1i4dfxo</t>
+        </is>
+      </c>
+      <c r="B1413" t="inlineStr">
+        <is>
+          <t>I overlooked this shade for too long!</t>
+        </is>
+      </c>
+      <c r="C1413" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4dfxo</t>
+        </is>
+      </c>
+    </row>
+    <row r="1414">
+      <c r="A1414" t="inlineStr">
+        <is>
+          <t>1i4b6y4</t>
+        </is>
+      </c>
+      <c r="B1414" t="inlineStr">
+        <is>
+          <t>Storing nail polish</t>
+        </is>
+      </c>
+      <c r="C1414" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4b6y4</t>
+        </is>
+      </c>
+    </row>
+    <row r="1415">
+      <c r="A1415" t="inlineStr">
+        <is>
+          <t>1i4b52j</t>
+        </is>
+      </c>
+      <c r="B1415" t="inlineStr">
+        <is>
+          <t>The resemblance was uncanny!</t>
+        </is>
+      </c>
+      <c r="C1415" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/ixwga13p3sde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1416">
+      <c r="A1416" t="inlineStr">
+        <is>
+          <t>1i4ab7g</t>
+        </is>
+      </c>
+      <c r="B1416" t="inlineStr">
+        <is>
+          <t>Spent two weeks in India and this is how my manicure faired</t>
+        </is>
+      </c>
+      <c r="C1416" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4ab7g</t>
+        </is>
+      </c>
+    </row>
+    <row r="1417">
+      <c r="A1417" t="inlineStr">
+        <is>
+          <t>1i4a8da</t>
+        </is>
+      </c>
+      <c r="B1417" t="inlineStr">
+        <is>
+          <t>Winter Pastel 🩷</t>
+        </is>
+      </c>
+      <c r="C1417" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4a8da</t>
+        </is>
+      </c>
+    </row>
+    <row r="1418">
+      <c r="A1418" t="inlineStr">
+        <is>
+          <t>1i4a420</t>
+        </is>
+      </c>
+      <c r="B1418" t="inlineStr">
+        <is>
+          <t>Love lighting in the elevator</t>
+        </is>
+      </c>
+      <c r="C1418" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4a420</t>
+        </is>
+      </c>
+    </row>
+    <row r="1419">
+      <c r="A1419" t="inlineStr">
+        <is>
+          <t>1i49fwx</t>
+        </is>
+      </c>
+      <c r="B1419" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Pelvic Sorcery is breathtaking 😍 </t>
+        </is>
+      </c>
+      <c r="C1419" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i49fwx</t>
+        </is>
+      </c>
+    </row>
+    <row r="1420">
+      <c r="A1420" t="inlineStr">
+        <is>
+          <t>1i45kkj</t>
+        </is>
+      </c>
+      <c r="B1420" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Having a classic silver holo moment </t>
+        </is>
+      </c>
+      <c r="C1420" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i45kkj</t>
+        </is>
+      </c>
+    </row>
+    <row r="1421">
+      <c r="A1421" t="inlineStr">
+        <is>
+          <t>1i45532</t>
+        </is>
+      </c>
+      <c r="B1421" t="inlineStr">
+        <is>
+          <t>absolutely blinding in the sun ✨☀️</t>
+        </is>
+      </c>
+      <c r="C1421" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i45532</t>
+        </is>
+      </c>
+    </row>
+    <row r="1422">
+      <c r="A1422" t="inlineStr">
+        <is>
+          <t>1i454gf</t>
+        </is>
+      </c>
+      <c r="B1422" t="inlineStr">
+        <is>
+          <t>Struggling with impulse control</t>
+        </is>
+      </c>
+      <c r="C1422" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i454gf</t>
+        </is>
+      </c>
+    </row>
+    <row r="1423">
+      <c r="A1423" t="inlineStr">
+        <is>
+          <t>1i43xdq</t>
+        </is>
+      </c>
+      <c r="B1423" t="inlineStr">
+        <is>
+          <t>acrylate allergy - new to lacquer and need recommendations</t>
+        </is>
+      </c>
+      <c r="C1423" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/r/RedditLaqueristas/comments/1i43xdq/acrylate_allergy_new_to_lacquer_and_need/</t>
+        </is>
+      </c>
+    </row>
+    <row r="1424">
+      <c r="A1424" t="inlineStr">
+        <is>
+          <t>1i43gif</t>
+        </is>
+      </c>
+      <c r="B1424" t="inlineStr">
+        <is>
+          <t>When you chip before you take photos 🥴</t>
+        </is>
+      </c>
+      <c r="C1424" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/7alpfvqaupde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1425">
+      <c r="A1425" t="inlineStr">
+        <is>
+          <t>1i43fnz</t>
+        </is>
+      </c>
+      <c r="B1425" t="inlineStr">
+        <is>
+          <t>Love a juicy shimmer + glitter combo 🌟</t>
+        </is>
+      </c>
+      <c r="C1425" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i43fnz</t>
+        </is>
+      </c>
+    </row>
+    <row r="1426">
+      <c r="A1426" t="inlineStr">
+        <is>
+          <t>1i4397c</t>
+        </is>
+      </c>
+      <c r="B1426" t="inlineStr">
+        <is>
+          <t xml:space="preserve">First time doing velvet nails. I think it was a success! </t>
+        </is>
+      </c>
+      <c r="C1426" t="inlineStr">
+        <is>
+          <t>https://v.redd.it/s9ia2oijrpde1</t>
+        </is>
+      </c>
+    </row>
+    <row r="1427">
+      <c r="A1427" t="inlineStr">
+        <is>
+          <t>1i4o3yx</t>
+        </is>
+      </c>
+      <c r="B1427" t="inlineStr">
+        <is>
+          <t xml:space="preserve">thoughts? </t>
+        </is>
+      </c>
+      <c r="C1427" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/nepcjlsd4vde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1428">
+      <c r="A1428" t="inlineStr">
+        <is>
+          <t>1i4mt0a</t>
+        </is>
+      </c>
+      <c r="B1428" t="inlineStr">
+        <is>
+          <t xml:space="preserve">I just recently started learning how to paint characters </t>
+        </is>
+      </c>
+      <c r="C1428" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4mt0a</t>
+        </is>
+      </c>
+    </row>
+    <row r="1429">
+      <c r="A1429" t="inlineStr">
+        <is>
+          <t>1i4mnt6</t>
+        </is>
+      </c>
+      <c r="B1429" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Added better quality pics new nails what yall think </t>
+        </is>
+      </c>
+      <c r="C1429" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4mnt6</t>
+        </is>
+      </c>
+    </row>
+    <row r="1430">
+      <c r="A1430" t="inlineStr">
+        <is>
+          <t>1i4lers</t>
+        </is>
+      </c>
+      <c r="B1430" t="inlineStr">
+        <is>
+          <t>Look at this beauty! 💖</t>
+        </is>
+      </c>
+      <c r="C1430" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/57c5c4lkfude1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1431">
+      <c r="A1431" t="inlineStr">
+        <is>
+          <t>1i4jhxk</t>
+        </is>
+      </c>
+      <c r="B1431" t="inlineStr">
+        <is>
+          <t>Belle ✨📚🌹</t>
+        </is>
+      </c>
+      <c r="C1431" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/8znpjhjxytde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1432">
+      <c r="A1432" t="inlineStr">
+        <is>
+          <t>1i4hwnb</t>
+        </is>
+      </c>
+      <c r="B1432" t="inlineStr">
+        <is>
+          <t>regency romance for Feb 🫶🏻</t>
+        </is>
+      </c>
+      <c r="C1432" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4hwnb</t>
+        </is>
+      </c>
+    </row>
+    <row r="1433">
+      <c r="A1433" t="inlineStr">
+        <is>
+          <t>1i4gduh</t>
+        </is>
+      </c>
+      <c r="B1433" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Beautiful my new color and design </t>
+        </is>
+      </c>
+      <c r="C1433" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4gduh</t>
+        </is>
+      </c>
+    </row>
+    <row r="1434">
+      <c r="A1434" t="inlineStr">
+        <is>
+          <t>1i4fd9w</t>
+        </is>
+      </c>
+      <c r="B1434" t="inlineStr">
+        <is>
+          <t>First attempt at nails!</t>
+        </is>
+      </c>
+      <c r="C1434" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/wde5hzd81tde1.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="1435">
+      <c r="A1435" t="inlineStr">
+        <is>
+          <t>1i4e29w</t>
+        </is>
+      </c>
+      <c r="B1435" t="inlineStr">
+        <is>
+          <t>Square French</t>
+        </is>
+      </c>
+      <c r="C1435" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/mh42danrqsde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1436">
+      <c r="A1436" t="inlineStr">
+        <is>
+          <t>1i4czae</t>
+        </is>
+      </c>
+      <c r="B1436" t="inlineStr">
+        <is>
+          <t>Cute lil pink set</t>
+        </is>
+      </c>
+      <c r="C1436" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4czae</t>
+        </is>
+      </c>
+    </row>
+    <row r="1437">
+      <c r="A1437" t="inlineStr">
+        <is>
+          <t>1i4an3f</t>
+        </is>
+      </c>
+      <c r="B1437" t="inlineStr">
+        <is>
+          <t>Lunar New Year Nails 🧧</t>
+        </is>
+      </c>
+      <c r="C1437" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i4an3f</t>
+        </is>
+      </c>
+    </row>
+    <row r="1438">
+      <c r="A1438" t="inlineStr">
+        <is>
+          <t>1i4a7yh</t>
+        </is>
+      </c>
+      <c r="B1438" t="inlineStr">
+        <is>
+          <t>Winter Wonderland inspired - French tips are hard!</t>
+        </is>
+      </c>
+      <c r="C1438" t="inlineStr">
+        <is>
+          <t>https://i.redd.it/jh8u6or8wrde1.jpeg</t>
+        </is>
+      </c>
+    </row>
+    <row r="1439">
+      <c r="A1439" t="inlineStr">
+        <is>
+          <t>1i44p9h</t>
+        </is>
+      </c>
+      <c r="B1439" t="inlineStr">
+        <is>
+          <t>some press ons i made</t>
+        </is>
+      </c>
+      <c r="C1439" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i44p9h</t>
+        </is>
+      </c>
+    </row>
+    <row r="1440">
+      <c r="A1440" t="inlineStr">
+        <is>
+          <t>1i439pp</t>
+        </is>
+      </c>
+      <c r="B1440" t="inlineStr">
+        <is>
+          <t xml:space="preserve">What i asked for, what i got </t>
+        </is>
+      </c>
+      <c r="C1440" t="inlineStr">
+        <is>
+          <t>https://www.reddit.com/gallery/1i439pp</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>